<commit_message>
Updated documents and test cases for service
</commit_message>
<xml_diff>
--- a/Documents/ScreenLayouts/Dashboard-Customer.xlsx
+++ b/Documents/ScreenLayouts/Dashboard-Customer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev/booking/Documents/ScreenLayouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D0CCE0-CB80-7546-BBA6-1E198A55B08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD1DAF4-76AA-B844-93CF-41772951DA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="15800" xr2:uid="{90052BEC-FEBB-F247-ACB1-709744DE85BE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{90052BEC-FEBB-F247-ACB1-709744DE85BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="5" r:id="rId1"/>
@@ -96,9 +96,6 @@
     <t>SCR-DSH-04 : Request Panel</t>
   </si>
   <si>
-    <t>File Service Providers</t>
-  </si>
-  <si>
     <t>API: WS-SP-01:Search Service Provider For Post</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>Open Create post model in edit mode.</t>
+  </si>
+  <si>
+    <t>Filnd Service Providers</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -480,10 +480,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -492,29 +492,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -537,6 +516,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2657,211 +2658,214 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43867302-6022-BC45-9802-796B2A9AA285}">
   <dimension ref="A1:DD85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="BS56" sqref="BS55:BT56"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="CB33" sqref="CB33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2" defaultRowHeight="8" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="72" max="72" width="4.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="27" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
     </row>
     <row r="2" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="27"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
     </row>
     <row r="3" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="27"/>
-      <c r="V3" s="27"/>
-      <c r="W3" s="27"/>
-      <c r="X3" s="27"/>
-      <c r="Y3" s="27"/>
-      <c r="Z3" s="27"/>
-      <c r="AA3" s="27"/>
-      <c r="AB3" s="27"/>
-      <c r="AC3" s="27"/>
-      <c r="AD3" s="27"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="20"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20"/>
     </row>
     <row r="4" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="28" t="s">
-        <v>28</v>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="21" t="s">
+        <v>27</v>
       </c>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="28"/>
-      <c r="V4" s="28"/>
-      <c r="W4" s="28"/>
-      <c r="X4" s="28"/>
-      <c r="Y4" s="28"/>
-      <c r="Z4" s="28"/>
-      <c r="AA4" s="28"/>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="28"/>
-      <c r="AD4" s="28"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="21"/>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="21"/>
+      <c r="AC4" s="21"/>
+      <c r="AD4" s="21"/>
     </row>
     <row r="5" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="28"/>
-      <c r="V5" s="28"/>
-      <c r="W5" s="28"/>
-      <c r="X5" s="28"/>
-      <c r="Y5" s="28"/>
-      <c r="Z5" s="28"/>
-      <c r="AA5" s="28"/>
-      <c r="AB5" s="28"/>
-      <c r="AC5" s="28"/>
-      <c r="AD5" s="28"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="21"/>
+      <c r="AC5" s="21"/>
+      <c r="AD5" s="21"/>
     </row>
     <row r="6" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="28"/>
-      <c r="V6" s="28"/>
-      <c r="W6" s="28"/>
-      <c r="X6" s="28"/>
-      <c r="Y6" s="28"/>
-      <c r="Z6" s="28"/>
-      <c r="AA6" s="28"/>
-      <c r="AB6" s="28"/>
-      <c r="AC6" s="28"/>
-      <c r="AD6" s="28"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="21"/>
+      <c r="V6" s="21"/>
+      <c r="W6" s="21"/>
+      <c r="X6" s="21"/>
+      <c r="Y6" s="21"/>
+      <c r="Z6" s="21"/>
+      <c r="AA6" s="21"/>
+      <c r="AB6" s="21"/>
+      <c r="AC6" s="21"/>
+      <c r="AD6" s="21"/>
     </row>
     <row r="9" spans="1:108" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
@@ -5006,7 +5010,7 @@
       <c r="BQ29" s="5"/>
       <c r="BR29" s="5"/>
       <c r="BS29" s="5"/>
-      <c r="BT29" s="5"/>
+      <c r="BT29" s="32"/>
       <c r="BU29" s="5"/>
       <c r="BV29" s="5"/>
       <c r="BW29" s="5"/>
@@ -8634,222 +8638,222 @@
       <c r="CT67" s="11"/>
     </row>
     <row r="68" spans="3:98" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C68" s="31" t="s">
+      <c r="C68" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D68" s="29"/>
-      <c r="E68" s="29"/>
-      <c r="F68" s="29"/>
-      <c r="G68" s="29" t="s">
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="22"/>
+      <c r="G68" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H68" s="29"/>
-      <c r="I68" s="29"/>
-      <c r="J68" s="29"/>
-      <c r="K68" s="29"/>
-      <c r="L68" s="29"/>
-      <c r="M68" s="29"/>
-      <c r="N68" s="29"/>
-      <c r="O68" s="29"/>
-      <c r="P68" s="29"/>
-      <c r="Q68" s="29"/>
-      <c r="R68" s="29"/>
-      <c r="S68" s="29"/>
-      <c r="T68" s="29"/>
-      <c r="U68" s="29"/>
-      <c r="V68" s="29"/>
-      <c r="W68" s="29"/>
-      <c r="X68" s="29"/>
-      <c r="Y68" s="29" t="s">
+      <c r="H68" s="22"/>
+      <c r="I68" s="22"/>
+      <c r="J68" s="22"/>
+      <c r="K68" s="22"/>
+      <c r="L68" s="22"/>
+      <c r="M68" s="22"/>
+      <c r="N68" s="22"/>
+      <c r="O68" s="22"/>
+      <c r="P68" s="22"/>
+      <c r="Q68" s="22"/>
+      <c r="R68" s="22"/>
+      <c r="S68" s="22"/>
+      <c r="T68" s="22"/>
+      <c r="U68" s="22"/>
+      <c r="V68" s="22"/>
+      <c r="W68" s="22"/>
+      <c r="X68" s="22"/>
+      <c r="Y68" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="Z68" s="29"/>
-      <c r="AA68" s="29"/>
-      <c r="AB68" s="29"/>
-      <c r="AC68" s="29"/>
-      <c r="AD68" s="29"/>
-      <c r="AE68" s="29"/>
-      <c r="AF68" s="29"/>
-      <c r="AG68" s="29"/>
-      <c r="AH68" s="29"/>
-      <c r="AI68" s="29"/>
-      <c r="AJ68" s="29"/>
-      <c r="AK68" s="29"/>
-      <c r="AL68" s="29"/>
-      <c r="AM68" s="29"/>
-      <c r="AN68" s="29" t="s">
+      <c r="Z68" s="22"/>
+      <c r="AA68" s="22"/>
+      <c r="AB68" s="22"/>
+      <c r="AC68" s="22"/>
+      <c r="AD68" s="22"/>
+      <c r="AE68" s="22"/>
+      <c r="AF68" s="22"/>
+      <c r="AG68" s="22"/>
+      <c r="AH68" s="22"/>
+      <c r="AI68" s="22"/>
+      <c r="AJ68" s="22"/>
+      <c r="AK68" s="22"/>
+      <c r="AL68" s="22"/>
+      <c r="AM68" s="22"/>
+      <c r="AN68" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AO68" s="29"/>
-      <c r="AP68" s="29"/>
-      <c r="AQ68" s="29"/>
-      <c r="AR68" s="29"/>
-      <c r="AS68" s="29"/>
-      <c r="AT68" s="29"/>
-      <c r="AU68" s="29"/>
-      <c r="AV68" s="29"/>
-      <c r="AW68" s="29"/>
-      <c r="AX68" s="29"/>
-      <c r="AY68" s="29"/>
-      <c r="AZ68" s="29"/>
-      <c r="BA68" s="29"/>
-      <c r="BB68" s="29"/>
-      <c r="BC68" s="29"/>
-      <c r="BD68" s="29"/>
-      <c r="BE68" s="29"/>
-      <c r="BF68" s="29"/>
-      <c r="BG68" s="29"/>
-      <c r="BH68" s="29"/>
-      <c r="BI68" s="29"/>
-      <c r="BJ68" s="29" t="s">
+      <c r="AO68" s="22"/>
+      <c r="AP68" s="22"/>
+      <c r="AQ68" s="22"/>
+      <c r="AR68" s="22"/>
+      <c r="AS68" s="22"/>
+      <c r="AT68" s="22"/>
+      <c r="AU68" s="22"/>
+      <c r="AV68" s="22"/>
+      <c r="AW68" s="22"/>
+      <c r="AX68" s="22"/>
+      <c r="AY68" s="22"/>
+      <c r="AZ68" s="22"/>
+      <c r="BA68" s="22"/>
+      <c r="BB68" s="22"/>
+      <c r="BC68" s="22"/>
+      <c r="BD68" s="22"/>
+      <c r="BE68" s="22"/>
+      <c r="BF68" s="22"/>
+      <c r="BG68" s="22"/>
+      <c r="BH68" s="22"/>
+      <c r="BI68" s="22"/>
+      <c r="BJ68" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="BK68" s="29"/>
-      <c r="BL68" s="29"/>
-      <c r="BM68" s="29"/>
-      <c r="BN68" s="29"/>
-      <c r="BO68" s="29"/>
-      <c r="BP68" s="29"/>
-      <c r="BQ68" s="29"/>
-      <c r="BR68" s="29"/>
-      <c r="BS68" s="29"/>
-      <c r="BT68" s="29"/>
-      <c r="BU68" s="29"/>
-      <c r="BV68" s="29"/>
-      <c r="BW68" s="29"/>
-      <c r="BX68" s="29"/>
-      <c r="BY68" s="29"/>
-      <c r="BZ68" s="29" t="s">
+      <c r="BK68" s="22"/>
+      <c r="BL68" s="22"/>
+      <c r="BM68" s="22"/>
+      <c r="BN68" s="22"/>
+      <c r="BO68" s="22"/>
+      <c r="BP68" s="22"/>
+      <c r="BQ68" s="22"/>
+      <c r="BR68" s="22"/>
+      <c r="BS68" s="22"/>
+      <c r="BT68" s="22"/>
+      <c r="BU68" s="22"/>
+      <c r="BV68" s="22"/>
+      <c r="BW68" s="22"/>
+      <c r="BX68" s="22"/>
+      <c r="BY68" s="22"/>
+      <c r="BZ68" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="CA68" s="29"/>
-      <c r="CB68" s="29"/>
-      <c r="CC68" s="29"/>
-      <c r="CD68" s="29"/>
-      <c r="CE68" s="29"/>
-      <c r="CF68" s="29"/>
-      <c r="CG68" s="29"/>
-      <c r="CH68" s="29"/>
-      <c r="CI68" s="29"/>
-      <c r="CJ68" s="29"/>
-      <c r="CK68" s="29"/>
-      <c r="CL68" s="29"/>
-      <c r="CM68" s="29"/>
-      <c r="CN68" s="29"/>
-      <c r="CO68" s="29"/>
-      <c r="CP68" s="29"/>
-      <c r="CQ68" s="29"/>
-      <c r="CR68" s="29"/>
-      <c r="CS68" s="29"/>
-      <c r="CT68" s="30"/>
+      <c r="CA68" s="22"/>
+      <c r="CB68" s="22"/>
+      <c r="CC68" s="22"/>
+      <c r="CD68" s="22"/>
+      <c r="CE68" s="22"/>
+      <c r="CF68" s="22"/>
+      <c r="CG68" s="22"/>
+      <c r="CH68" s="22"/>
+      <c r="CI68" s="22"/>
+      <c r="CJ68" s="22"/>
+      <c r="CK68" s="22"/>
+      <c r="CL68" s="22"/>
+      <c r="CM68" s="22"/>
+      <c r="CN68" s="22"/>
+      <c r="CO68" s="22"/>
+      <c r="CP68" s="22"/>
+      <c r="CQ68" s="22"/>
+      <c r="CR68" s="22"/>
+      <c r="CS68" s="22"/>
+      <c r="CT68" s="23"/>
     </row>
     <row r="69" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C69" s="23">
+      <c r="C69" s="25">
         <v>1</v>
       </c>
-      <c r="D69" s="24"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
-      <c r="G69" s="21" t="s">
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H69" s="21"/>
-      <c r="I69" s="21"/>
-      <c r="J69" s="21"/>
-      <c r="K69" s="21"/>
-      <c r="L69" s="21"/>
-      <c r="M69" s="21"/>
-      <c r="N69" s="21"/>
-      <c r="O69" s="21"/>
-      <c r="P69" s="21"/>
-      <c r="Q69" s="21"/>
-      <c r="R69" s="21"/>
-      <c r="S69" s="21"/>
-      <c r="T69" s="21"/>
-      <c r="U69" s="21"/>
-      <c r="V69" s="21"/>
-      <c r="W69" s="21"/>
-      <c r="X69" s="21"/>
-      <c r="Y69" s="21" t="s">
+      <c r="H69" s="17"/>
+      <c r="I69" s="17"/>
+      <c r="J69" s="17"/>
+      <c r="K69" s="17"/>
+      <c r="L69" s="17"/>
+      <c r="M69" s="17"/>
+      <c r="N69" s="17"/>
+      <c r="O69" s="17"/>
+      <c r="P69" s="17"/>
+      <c r="Q69" s="17"/>
+      <c r="R69" s="17"/>
+      <c r="S69" s="17"/>
+      <c r="T69" s="17"/>
+      <c r="U69" s="17"/>
+      <c r="V69" s="17"/>
+      <c r="W69" s="17"/>
+      <c r="X69" s="17"/>
+      <c r="Y69" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="Z69" s="21"/>
-      <c r="AA69" s="21"/>
-      <c r="AB69" s="21"/>
-      <c r="AC69" s="21"/>
-      <c r="AD69" s="21"/>
-      <c r="AE69" s="21"/>
-      <c r="AF69" s="21"/>
-      <c r="AG69" s="21"/>
-      <c r="AH69" s="21"/>
-      <c r="AI69" s="21"/>
-      <c r="AJ69" s="21"/>
-      <c r="AK69" s="21"/>
-      <c r="AL69" s="21"/>
-      <c r="AM69" s="21"/>
-      <c r="AN69" s="24" t="s">
+      <c r="Z69" s="17"/>
+      <c r="AA69" s="17"/>
+      <c r="AB69" s="17"/>
+      <c r="AC69" s="17"/>
+      <c r="AD69" s="17"/>
+      <c r="AE69" s="17"/>
+      <c r="AF69" s="17"/>
+      <c r="AG69" s="17"/>
+      <c r="AH69" s="17"/>
+      <c r="AI69" s="17"/>
+      <c r="AJ69" s="17"/>
+      <c r="AK69" s="17"/>
+      <c r="AL69" s="17"/>
+      <c r="AM69" s="17"/>
+      <c r="AN69" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="AO69" s="24"/>
-      <c r="AP69" s="24"/>
-      <c r="AQ69" s="24"/>
-      <c r="AR69" s="24"/>
-      <c r="AS69" s="24"/>
-      <c r="AT69" s="24"/>
-      <c r="AU69" s="24"/>
-      <c r="AV69" s="24"/>
-      <c r="AW69" s="24"/>
-      <c r="AX69" s="24"/>
-      <c r="AY69" s="24"/>
-      <c r="AZ69" s="24"/>
-      <c r="BA69" s="24"/>
-      <c r="BB69" s="24"/>
-      <c r="BC69" s="24"/>
-      <c r="BD69" s="24"/>
-      <c r="BE69" s="24"/>
-      <c r="BF69" s="24"/>
-      <c r="BG69" s="24"/>
-      <c r="BH69" s="24"/>
-      <c r="BI69" s="24"/>
-      <c r="BJ69" s="21" t="s">
+      <c r="AO69" s="26"/>
+      <c r="AP69" s="26"/>
+      <c r="AQ69" s="26"/>
+      <c r="AR69" s="26"/>
+      <c r="AS69" s="26"/>
+      <c r="AT69" s="26"/>
+      <c r="AU69" s="26"/>
+      <c r="AV69" s="26"/>
+      <c r="AW69" s="26"/>
+      <c r="AX69" s="26"/>
+      <c r="AY69" s="26"/>
+      <c r="AZ69" s="26"/>
+      <c r="BA69" s="26"/>
+      <c r="BB69" s="26"/>
+      <c r="BC69" s="26"/>
+      <c r="BD69" s="26"/>
+      <c r="BE69" s="26"/>
+      <c r="BF69" s="26"/>
+      <c r="BG69" s="26"/>
+      <c r="BH69" s="26"/>
+      <c r="BI69" s="26"/>
+      <c r="BJ69" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="BK69" s="21"/>
-      <c r="BL69" s="21"/>
-      <c r="BM69" s="21"/>
-      <c r="BN69" s="21"/>
-      <c r="BO69" s="21"/>
-      <c r="BP69" s="21"/>
-      <c r="BQ69" s="21"/>
-      <c r="BR69" s="21"/>
-      <c r="BS69" s="21"/>
-      <c r="BT69" s="21"/>
-      <c r="BU69" s="21"/>
-      <c r="BV69" s="21"/>
-      <c r="BW69" s="21"/>
-      <c r="BX69" s="21"/>
-      <c r="BY69" s="21"/>
-      <c r="BZ69" s="21"/>
-      <c r="CA69" s="21"/>
-      <c r="CB69" s="21"/>
-      <c r="CC69" s="21"/>
-      <c r="CD69" s="21"/>
-      <c r="CE69" s="21"/>
-      <c r="CF69" s="21"/>
-      <c r="CG69" s="21"/>
-      <c r="CH69" s="21"/>
-      <c r="CI69" s="21"/>
-      <c r="CJ69" s="21"/>
-      <c r="CK69" s="21"/>
-      <c r="CL69" s="21"/>
-      <c r="CM69" s="21"/>
-      <c r="CN69" s="21"/>
-      <c r="CO69" s="21"/>
-      <c r="CP69" s="21"/>
-      <c r="CQ69" s="21"/>
-      <c r="CR69" s="21"/>
-      <c r="CS69" s="21"/>
-      <c r="CT69" s="25"/>
+      <c r="BK69" s="17"/>
+      <c r="BL69" s="17"/>
+      <c r="BM69" s="17"/>
+      <c r="BN69" s="17"/>
+      <c r="BO69" s="17"/>
+      <c r="BP69" s="17"/>
+      <c r="BQ69" s="17"/>
+      <c r="BR69" s="17"/>
+      <c r="BS69" s="17"/>
+      <c r="BT69" s="17"/>
+      <c r="BU69" s="17"/>
+      <c r="BV69" s="17"/>
+      <c r="BW69" s="17"/>
+      <c r="BX69" s="17"/>
+      <c r="BY69" s="17"/>
+      <c r="BZ69" s="17"/>
+      <c r="CA69" s="17"/>
+      <c r="CB69" s="17"/>
+      <c r="CC69" s="17"/>
+      <c r="CD69" s="17"/>
+      <c r="CE69" s="17"/>
+      <c r="CF69" s="17"/>
+      <c r="CG69" s="17"/>
+      <c r="CH69" s="17"/>
+      <c r="CI69" s="17"/>
+      <c r="CJ69" s="17"/>
+      <c r="CK69" s="17"/>
+      <c r="CL69" s="17"/>
+      <c r="CM69" s="17"/>
+      <c r="CN69" s="17"/>
+      <c r="CO69" s="17"/>
+      <c r="CP69" s="17"/>
+      <c r="CQ69" s="17"/>
+      <c r="CR69" s="17"/>
+      <c r="CS69" s="17"/>
+      <c r="CT69" s="18"/>
     </row>
     <row r="70" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C70" s="15">
@@ -8858,43 +8862,43 @@
       <c r="D70" s="16"/>
       <c r="E70" s="16"/>
       <c r="F70" s="16"/>
-      <c r="G70" s="22" t="s">
+      <c r="G70" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H70" s="17"/>
-      <c r="I70" s="17"/>
-      <c r="J70" s="17"/>
-      <c r="K70" s="17"/>
-      <c r="L70" s="17"/>
-      <c r="M70" s="17"/>
-      <c r="N70" s="17"/>
-      <c r="O70" s="17"/>
-      <c r="P70" s="17"/>
-      <c r="Q70" s="17"/>
-      <c r="R70" s="17"/>
-      <c r="S70" s="17"/>
-      <c r="T70" s="17"/>
-      <c r="U70" s="17"/>
-      <c r="V70" s="17"/>
-      <c r="W70" s="17"/>
-      <c r="X70" s="17"/>
-      <c r="Y70" s="17" t="s">
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="13"/>
+      <c r="L70" s="13"/>
+      <c r="M70" s="13"/>
+      <c r="N70" s="13"/>
+      <c r="O70" s="13"/>
+      <c r="P70" s="13"/>
+      <c r="Q70" s="13"/>
+      <c r="R70" s="13"/>
+      <c r="S70" s="13"/>
+      <c r="T70" s="13"/>
+      <c r="U70" s="13"/>
+      <c r="V70" s="13"/>
+      <c r="W70" s="13"/>
+      <c r="X70" s="13"/>
+      <c r="Y70" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="Z70" s="17"/>
-      <c r="AA70" s="17"/>
-      <c r="AB70" s="17"/>
-      <c r="AC70" s="17"/>
-      <c r="AD70" s="17"/>
-      <c r="AE70" s="17"/>
-      <c r="AF70" s="17"/>
-      <c r="AG70" s="17"/>
-      <c r="AH70" s="17"/>
-      <c r="AI70" s="17"/>
-      <c r="AJ70" s="17"/>
-      <c r="AK70" s="17"/>
-      <c r="AL70" s="17"/>
-      <c r="AM70" s="17"/>
+      <c r="Z70" s="13"/>
+      <c r="AA70" s="13"/>
+      <c r="AB70" s="13"/>
+      <c r="AC70" s="13"/>
+      <c r="AD70" s="13"/>
+      <c r="AE70" s="13"/>
+      <c r="AF70" s="13"/>
+      <c r="AG70" s="13"/>
+      <c r="AH70" s="13"/>
+      <c r="AI70" s="13"/>
+      <c r="AJ70" s="13"/>
+      <c r="AK70" s="13"/>
+      <c r="AL70" s="13"/>
+      <c r="AM70" s="13"/>
       <c r="AN70" s="16" t="s">
         <v>16</v>
       </c>
@@ -8919,45 +8923,45 @@
       <c r="BG70" s="16"/>
       <c r="BH70" s="16"/>
       <c r="BI70" s="16"/>
-      <c r="BJ70" s="17" t="s">
+      <c r="BJ70" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="BK70" s="17"/>
-      <c r="BL70" s="17"/>
-      <c r="BM70" s="17"/>
-      <c r="BN70" s="17"/>
-      <c r="BO70" s="17"/>
-      <c r="BP70" s="17"/>
-      <c r="BQ70" s="17"/>
-      <c r="BR70" s="17"/>
-      <c r="BS70" s="17"/>
-      <c r="BT70" s="17"/>
-      <c r="BU70" s="17"/>
-      <c r="BV70" s="17"/>
-      <c r="BW70" s="17"/>
-      <c r="BX70" s="17"/>
-      <c r="BY70" s="17"/>
-      <c r="BZ70" s="17"/>
-      <c r="CA70" s="17"/>
-      <c r="CB70" s="17"/>
-      <c r="CC70" s="17"/>
-      <c r="CD70" s="17"/>
-      <c r="CE70" s="17"/>
-      <c r="CF70" s="17"/>
-      <c r="CG70" s="17"/>
-      <c r="CH70" s="17"/>
-      <c r="CI70" s="17"/>
-      <c r="CJ70" s="17"/>
-      <c r="CK70" s="17"/>
-      <c r="CL70" s="17"/>
-      <c r="CM70" s="17"/>
-      <c r="CN70" s="17"/>
-      <c r="CO70" s="17"/>
-      <c r="CP70" s="17"/>
-      <c r="CQ70" s="17"/>
-      <c r="CR70" s="17"/>
-      <c r="CS70" s="17"/>
-      <c r="CT70" s="18"/>
+      <c r="BK70" s="13"/>
+      <c r="BL70" s="13"/>
+      <c r="BM70" s="13"/>
+      <c r="BN70" s="13"/>
+      <c r="BO70" s="13"/>
+      <c r="BP70" s="13"/>
+      <c r="BQ70" s="13"/>
+      <c r="BR70" s="13"/>
+      <c r="BS70" s="13"/>
+      <c r="BT70" s="13"/>
+      <c r="BU70" s="13"/>
+      <c r="BV70" s="13"/>
+      <c r="BW70" s="13"/>
+      <c r="BX70" s="13"/>
+      <c r="BY70" s="13"/>
+      <c r="BZ70" s="13"/>
+      <c r="CA70" s="13"/>
+      <c r="CB70" s="13"/>
+      <c r="CC70" s="13"/>
+      <c r="CD70" s="13"/>
+      <c r="CE70" s="13"/>
+      <c r="CF70" s="13"/>
+      <c r="CG70" s="13"/>
+      <c r="CH70" s="13"/>
+      <c r="CI70" s="13"/>
+      <c r="CJ70" s="13"/>
+      <c r="CK70" s="13"/>
+      <c r="CL70" s="13"/>
+      <c r="CM70" s="13"/>
+      <c r="CN70" s="13"/>
+      <c r="CO70" s="13"/>
+      <c r="CP70" s="13"/>
+      <c r="CQ70" s="13"/>
+      <c r="CR70" s="13"/>
+      <c r="CS70" s="13"/>
+      <c r="CT70" s="14"/>
     </row>
     <row r="71" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C71" s="15">
@@ -8966,43 +8970,43 @@
       <c r="D71" s="16"/>
       <c r="E71" s="16"/>
       <c r="F71" s="16"/>
-      <c r="G71" s="17" t="s">
-        <v>29</v>
+      <c r="G71" s="13" t="s">
+        <v>28</v>
       </c>
-      <c r="H71" s="17"/>
-      <c r="I71" s="17"/>
-      <c r="J71" s="17"/>
-      <c r="K71" s="17"/>
-      <c r="L71" s="17"/>
-      <c r="M71" s="17"/>
-      <c r="N71" s="17"/>
-      <c r="O71" s="17"/>
-      <c r="P71" s="17"/>
-      <c r="Q71" s="17"/>
-      <c r="R71" s="17"/>
-      <c r="S71" s="17"/>
-      <c r="T71" s="17"/>
-      <c r="U71" s="17"/>
-      <c r="V71" s="17"/>
-      <c r="W71" s="17"/>
-      <c r="X71" s="17"/>
-      <c r="Y71" s="17" t="s">
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
+      <c r="L71" s="13"/>
+      <c r="M71" s="13"/>
+      <c r="N71" s="13"/>
+      <c r="O71" s="13"/>
+      <c r="P71" s="13"/>
+      <c r="Q71" s="13"/>
+      <c r="R71" s="13"/>
+      <c r="S71" s="13"/>
+      <c r="T71" s="13"/>
+      <c r="U71" s="13"/>
+      <c r="V71" s="13"/>
+      <c r="W71" s="13"/>
+      <c r="X71" s="13"/>
+      <c r="Y71" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="Z71" s="17"/>
-      <c r="AA71" s="17"/>
-      <c r="AB71" s="17"/>
-      <c r="AC71" s="17"/>
-      <c r="AD71" s="17"/>
-      <c r="AE71" s="17"/>
-      <c r="AF71" s="17"/>
-      <c r="AG71" s="17"/>
-      <c r="AH71" s="17"/>
-      <c r="AI71" s="17"/>
-      <c r="AJ71" s="17"/>
-      <c r="AK71" s="17"/>
-      <c r="AL71" s="17"/>
-      <c r="AM71" s="17"/>
+      <c r="Z71" s="13"/>
+      <c r="AA71" s="13"/>
+      <c r="AB71" s="13"/>
+      <c r="AC71" s="13"/>
+      <c r="AD71" s="13"/>
+      <c r="AE71" s="13"/>
+      <c r="AF71" s="13"/>
+      <c r="AG71" s="13"/>
+      <c r="AH71" s="13"/>
+      <c r="AI71" s="13"/>
+      <c r="AJ71" s="13"/>
+      <c r="AK71" s="13"/>
+      <c r="AL71" s="13"/>
+      <c r="AM71" s="13"/>
       <c r="AN71" s="16" t="s">
         <v>16</v>
       </c>
@@ -9027,45 +9031,45 @@
       <c r="BG71" s="16"/>
       <c r="BH71" s="16"/>
       <c r="BI71" s="16"/>
-      <c r="BJ71" s="17" t="s">
-        <v>30</v>
+      <c r="BJ71" s="13" t="s">
+        <v>29</v>
       </c>
-      <c r="BK71" s="17"/>
-      <c r="BL71" s="17"/>
-      <c r="BM71" s="17"/>
-      <c r="BN71" s="17"/>
-      <c r="BO71" s="17"/>
-      <c r="BP71" s="17"/>
-      <c r="BQ71" s="17"/>
-      <c r="BR71" s="17"/>
-      <c r="BS71" s="17"/>
-      <c r="BT71" s="17"/>
-      <c r="BU71" s="17"/>
-      <c r="BV71" s="17"/>
-      <c r="BW71" s="17"/>
-      <c r="BX71" s="17"/>
-      <c r="BY71" s="17"/>
-      <c r="BZ71" s="17"/>
-      <c r="CA71" s="17"/>
-      <c r="CB71" s="17"/>
-      <c r="CC71" s="17"/>
-      <c r="CD71" s="17"/>
-      <c r="CE71" s="17"/>
-      <c r="CF71" s="17"/>
-      <c r="CG71" s="17"/>
-      <c r="CH71" s="17"/>
-      <c r="CI71" s="17"/>
-      <c r="CJ71" s="17"/>
-      <c r="CK71" s="17"/>
-      <c r="CL71" s="17"/>
-      <c r="CM71" s="17"/>
-      <c r="CN71" s="17"/>
-      <c r="CO71" s="17"/>
-      <c r="CP71" s="17"/>
-      <c r="CQ71" s="17"/>
-      <c r="CR71" s="17"/>
-      <c r="CS71" s="17"/>
-      <c r="CT71" s="18"/>
+      <c r="BK71" s="13"/>
+      <c r="BL71" s="13"/>
+      <c r="BM71" s="13"/>
+      <c r="BN71" s="13"/>
+      <c r="BO71" s="13"/>
+      <c r="BP71" s="13"/>
+      <c r="BQ71" s="13"/>
+      <c r="BR71" s="13"/>
+      <c r="BS71" s="13"/>
+      <c r="BT71" s="13"/>
+      <c r="BU71" s="13"/>
+      <c r="BV71" s="13"/>
+      <c r="BW71" s="13"/>
+      <c r="BX71" s="13"/>
+      <c r="BY71" s="13"/>
+      <c r="BZ71" s="13"/>
+      <c r="CA71" s="13"/>
+      <c r="CB71" s="13"/>
+      <c r="CC71" s="13"/>
+      <c r="CD71" s="13"/>
+      <c r="CE71" s="13"/>
+      <c r="CF71" s="13"/>
+      <c r="CG71" s="13"/>
+      <c r="CH71" s="13"/>
+      <c r="CI71" s="13"/>
+      <c r="CJ71" s="13"/>
+      <c r="CK71" s="13"/>
+      <c r="CL71" s="13"/>
+      <c r="CM71" s="13"/>
+      <c r="CN71" s="13"/>
+      <c r="CO71" s="13"/>
+      <c r="CP71" s="13"/>
+      <c r="CQ71" s="13"/>
+      <c r="CR71" s="13"/>
+      <c r="CS71" s="13"/>
+      <c r="CT71" s="14"/>
     </row>
     <row r="72" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C72" s="15">
@@ -9074,43 +9078,43 @@
       <c r="D72" s="16"/>
       <c r="E72" s="16"/>
       <c r="F72" s="16"/>
-      <c r="G72" s="17" t="s">
+      <c r="G72" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H72" s="17"/>
-      <c r="I72" s="17"/>
-      <c r="J72" s="17"/>
-      <c r="K72" s="17"/>
-      <c r="L72" s="17"/>
-      <c r="M72" s="17"/>
-      <c r="N72" s="17"/>
-      <c r="O72" s="17"/>
-      <c r="P72" s="17"/>
-      <c r="Q72" s="17"/>
-      <c r="R72" s="17"/>
-      <c r="S72" s="17"/>
-      <c r="T72" s="17"/>
-      <c r="U72" s="17"/>
-      <c r="V72" s="17"/>
-      <c r="W72" s="17"/>
-      <c r="X72" s="17"/>
-      <c r="Y72" s="17" t="s">
+      <c r="H72" s="13"/>
+      <c r="I72" s="13"/>
+      <c r="J72" s="13"/>
+      <c r="K72" s="13"/>
+      <c r="L72" s="13"/>
+      <c r="M72" s="13"/>
+      <c r="N72" s="13"/>
+      <c r="O72" s="13"/>
+      <c r="P72" s="13"/>
+      <c r="Q72" s="13"/>
+      <c r="R72" s="13"/>
+      <c r="S72" s="13"/>
+      <c r="T72" s="13"/>
+      <c r="U72" s="13"/>
+      <c r="V72" s="13"/>
+      <c r="W72" s="13"/>
+      <c r="X72" s="13"/>
+      <c r="Y72" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="Z72" s="17"/>
-      <c r="AA72" s="17"/>
-      <c r="AB72" s="17"/>
-      <c r="AC72" s="17"/>
-      <c r="AD72" s="17"/>
-      <c r="AE72" s="17"/>
-      <c r="AF72" s="17"/>
-      <c r="AG72" s="17"/>
-      <c r="AH72" s="17"/>
-      <c r="AI72" s="17"/>
-      <c r="AJ72" s="17"/>
-      <c r="AK72" s="17"/>
-      <c r="AL72" s="17"/>
-      <c r="AM72" s="17"/>
+      <c r="Z72" s="13"/>
+      <c r="AA72" s="13"/>
+      <c r="AB72" s="13"/>
+      <c r="AC72" s="13"/>
+      <c r="AD72" s="13"/>
+      <c r="AE72" s="13"/>
+      <c r="AF72" s="13"/>
+      <c r="AG72" s="13"/>
+      <c r="AH72" s="13"/>
+      <c r="AI72" s="13"/>
+      <c r="AJ72" s="13"/>
+      <c r="AK72" s="13"/>
+      <c r="AL72" s="13"/>
+      <c r="AM72" s="13"/>
       <c r="AN72" s="16" t="s">
         <v>19</v>
       </c>
@@ -9135,45 +9139,45 @@
       <c r="BG72" s="16"/>
       <c r="BH72" s="16"/>
       <c r="BI72" s="16"/>
-      <c r="BJ72" s="17" t="s">
+      <c r="BJ72" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="BK72" s="17"/>
-      <c r="BL72" s="17"/>
-      <c r="BM72" s="17"/>
-      <c r="BN72" s="17"/>
-      <c r="BO72" s="17"/>
-      <c r="BP72" s="17"/>
-      <c r="BQ72" s="17"/>
-      <c r="BR72" s="17"/>
-      <c r="BS72" s="17"/>
-      <c r="BT72" s="17"/>
-      <c r="BU72" s="17"/>
-      <c r="BV72" s="17"/>
-      <c r="BW72" s="17"/>
-      <c r="BX72" s="17"/>
-      <c r="BY72" s="17"/>
-      <c r="BZ72" s="17"/>
-      <c r="CA72" s="17"/>
-      <c r="CB72" s="17"/>
-      <c r="CC72" s="17"/>
-      <c r="CD72" s="17"/>
-      <c r="CE72" s="17"/>
-      <c r="CF72" s="17"/>
-      <c r="CG72" s="17"/>
-      <c r="CH72" s="17"/>
-      <c r="CI72" s="17"/>
-      <c r="CJ72" s="17"/>
-      <c r="CK72" s="17"/>
-      <c r="CL72" s="17"/>
-      <c r="CM72" s="17"/>
-      <c r="CN72" s="17"/>
-      <c r="CO72" s="17"/>
-      <c r="CP72" s="17"/>
-      <c r="CQ72" s="17"/>
-      <c r="CR72" s="17"/>
-      <c r="CS72" s="17"/>
-      <c r="CT72" s="18"/>
+      <c r="BK72" s="13"/>
+      <c r="BL72" s="13"/>
+      <c r="BM72" s="13"/>
+      <c r="BN72" s="13"/>
+      <c r="BO72" s="13"/>
+      <c r="BP72" s="13"/>
+      <c r="BQ72" s="13"/>
+      <c r="BR72" s="13"/>
+      <c r="BS72" s="13"/>
+      <c r="BT72" s="13"/>
+      <c r="BU72" s="13"/>
+      <c r="BV72" s="13"/>
+      <c r="BW72" s="13"/>
+      <c r="BX72" s="13"/>
+      <c r="BY72" s="13"/>
+      <c r="BZ72" s="13"/>
+      <c r="CA72" s="13"/>
+      <c r="CB72" s="13"/>
+      <c r="CC72" s="13"/>
+      <c r="CD72" s="13"/>
+      <c r="CE72" s="13"/>
+      <c r="CF72" s="13"/>
+      <c r="CG72" s="13"/>
+      <c r="CH72" s="13"/>
+      <c r="CI72" s="13"/>
+      <c r="CJ72" s="13"/>
+      <c r="CK72" s="13"/>
+      <c r="CL72" s="13"/>
+      <c r="CM72" s="13"/>
+      <c r="CN72" s="13"/>
+      <c r="CO72" s="13"/>
+      <c r="CP72" s="13"/>
+      <c r="CQ72" s="13"/>
+      <c r="CR72" s="13"/>
+      <c r="CS72" s="13"/>
+      <c r="CT72" s="14"/>
     </row>
     <row r="73" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C73" s="15">
@@ -9182,43 +9186,43 @@
       <c r="D73" s="16"/>
       <c r="E73" s="16"/>
       <c r="F73" s="16"/>
-      <c r="G73" s="17" t="s">
+      <c r="G73" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H73" s="17"/>
-      <c r="I73" s="17"/>
-      <c r="J73" s="17"/>
-      <c r="K73" s="17"/>
-      <c r="L73" s="17"/>
-      <c r="M73" s="17"/>
-      <c r="N73" s="17"/>
-      <c r="O73" s="17"/>
-      <c r="P73" s="17"/>
-      <c r="Q73" s="17"/>
-      <c r="R73" s="17"/>
-      <c r="S73" s="17"/>
-      <c r="T73" s="17"/>
-      <c r="U73" s="17"/>
-      <c r="V73" s="17"/>
-      <c r="W73" s="17"/>
-      <c r="X73" s="17"/>
-      <c r="Y73" s="17" t="s">
+      <c r="H73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="13"/>
+      <c r="L73" s="13"/>
+      <c r="M73" s="13"/>
+      <c r="N73" s="13"/>
+      <c r="O73" s="13"/>
+      <c r="P73" s="13"/>
+      <c r="Q73" s="13"/>
+      <c r="R73" s="13"/>
+      <c r="S73" s="13"/>
+      <c r="T73" s="13"/>
+      <c r="U73" s="13"/>
+      <c r="V73" s="13"/>
+      <c r="W73" s="13"/>
+      <c r="X73" s="13"/>
+      <c r="Y73" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="Z73" s="17"/>
-      <c r="AA73" s="17"/>
-      <c r="AB73" s="17"/>
-      <c r="AC73" s="17"/>
-      <c r="AD73" s="17"/>
-      <c r="AE73" s="17"/>
-      <c r="AF73" s="17"/>
-      <c r="AG73" s="17"/>
-      <c r="AH73" s="17"/>
-      <c r="AI73" s="17"/>
-      <c r="AJ73" s="17"/>
-      <c r="AK73" s="17"/>
-      <c r="AL73" s="17"/>
-      <c r="AM73" s="17"/>
+      <c r="Z73" s="13"/>
+      <c r="AA73" s="13"/>
+      <c r="AB73" s="13"/>
+      <c r="AC73" s="13"/>
+      <c r="AD73" s="13"/>
+      <c r="AE73" s="13"/>
+      <c r="AF73" s="13"/>
+      <c r="AG73" s="13"/>
+      <c r="AH73" s="13"/>
+      <c r="AI73" s="13"/>
+      <c r="AJ73" s="13"/>
+      <c r="AK73" s="13"/>
+      <c r="AL73" s="13"/>
+      <c r="AM73" s="13"/>
       <c r="AN73" s="16" t="s">
         <v>21</v>
       </c>
@@ -9243,45 +9247,45 @@
       <c r="BG73" s="16"/>
       <c r="BH73" s="16"/>
       <c r="BI73" s="16"/>
-      <c r="BJ73" s="17" t="s">
+      <c r="BJ73" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="BK73" s="17"/>
-      <c r="BL73" s="17"/>
-      <c r="BM73" s="17"/>
-      <c r="BN73" s="17"/>
-      <c r="BO73" s="17"/>
-      <c r="BP73" s="17"/>
-      <c r="BQ73" s="17"/>
-      <c r="BR73" s="17"/>
-      <c r="BS73" s="17"/>
-      <c r="BT73" s="17"/>
-      <c r="BU73" s="17"/>
-      <c r="BV73" s="17"/>
-      <c r="BW73" s="17"/>
-      <c r="BX73" s="17"/>
-      <c r="BY73" s="17"/>
-      <c r="BZ73" s="17"/>
-      <c r="CA73" s="17"/>
-      <c r="CB73" s="17"/>
-      <c r="CC73" s="17"/>
-      <c r="CD73" s="17"/>
-      <c r="CE73" s="17"/>
-      <c r="CF73" s="17"/>
-      <c r="CG73" s="17"/>
-      <c r="CH73" s="17"/>
-      <c r="CI73" s="17"/>
-      <c r="CJ73" s="17"/>
-      <c r="CK73" s="17"/>
-      <c r="CL73" s="17"/>
-      <c r="CM73" s="17"/>
-      <c r="CN73" s="17"/>
-      <c r="CO73" s="17"/>
-      <c r="CP73" s="17"/>
-      <c r="CQ73" s="17"/>
-      <c r="CR73" s="17"/>
-      <c r="CS73" s="17"/>
-      <c r="CT73" s="18"/>
+      <c r="BK73" s="13"/>
+      <c r="BL73" s="13"/>
+      <c r="BM73" s="13"/>
+      <c r="BN73" s="13"/>
+      <c r="BO73" s="13"/>
+      <c r="BP73" s="13"/>
+      <c r="BQ73" s="13"/>
+      <c r="BR73" s="13"/>
+      <c r="BS73" s="13"/>
+      <c r="BT73" s="13"/>
+      <c r="BU73" s="13"/>
+      <c r="BV73" s="13"/>
+      <c r="BW73" s="13"/>
+      <c r="BX73" s="13"/>
+      <c r="BY73" s="13"/>
+      <c r="BZ73" s="13"/>
+      <c r="CA73" s="13"/>
+      <c r="CB73" s="13"/>
+      <c r="CC73" s="13"/>
+      <c r="CD73" s="13"/>
+      <c r="CE73" s="13"/>
+      <c r="CF73" s="13"/>
+      <c r="CG73" s="13"/>
+      <c r="CH73" s="13"/>
+      <c r="CI73" s="13"/>
+      <c r="CJ73" s="13"/>
+      <c r="CK73" s="13"/>
+      <c r="CL73" s="13"/>
+      <c r="CM73" s="13"/>
+      <c r="CN73" s="13"/>
+      <c r="CO73" s="13"/>
+      <c r="CP73" s="13"/>
+      <c r="CQ73" s="13"/>
+      <c r="CR73" s="13"/>
+      <c r="CS73" s="13"/>
+      <c r="CT73" s="14"/>
     </row>
     <row r="74" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C74" s="15">
@@ -9290,45 +9294,45 @@
       <c r="D74" s="16"/>
       <c r="E74" s="16"/>
       <c r="F74" s="16"/>
-      <c r="G74" s="17" t="s">
-        <v>23</v>
+      <c r="G74" s="13" t="s">
+        <v>30</v>
       </c>
-      <c r="H74" s="17"/>
-      <c r="I74" s="17"/>
-      <c r="J74" s="17"/>
-      <c r="K74" s="17"/>
-      <c r="L74" s="17"/>
-      <c r="M74" s="17"/>
-      <c r="N74" s="17"/>
-      <c r="O74" s="17"/>
-      <c r="P74" s="17"/>
-      <c r="Q74" s="17"/>
-      <c r="R74" s="17"/>
-      <c r="S74" s="17"/>
-      <c r="T74" s="17"/>
-      <c r="U74" s="17"/>
-      <c r="V74" s="17"/>
-      <c r="W74" s="17"/>
-      <c r="X74" s="17"/>
-      <c r="Y74" s="17" t="s">
+      <c r="H74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="13"/>
+      <c r="L74" s="13"/>
+      <c r="M74" s="13"/>
+      <c r="N74" s="13"/>
+      <c r="O74" s="13"/>
+      <c r="P74" s="13"/>
+      <c r="Q74" s="13"/>
+      <c r="R74" s="13"/>
+      <c r="S74" s="13"/>
+      <c r="T74" s="13"/>
+      <c r="U74" s="13"/>
+      <c r="V74" s="13"/>
+      <c r="W74" s="13"/>
+      <c r="X74" s="13"/>
+      <c r="Y74" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="Z74" s="17"/>
-      <c r="AA74" s="17"/>
-      <c r="AB74" s="17"/>
-      <c r="AC74" s="17"/>
-      <c r="AD74" s="17"/>
-      <c r="AE74" s="17"/>
-      <c r="AF74" s="17"/>
-      <c r="AG74" s="17"/>
-      <c r="AH74" s="17"/>
-      <c r="AI74" s="17"/>
-      <c r="AJ74" s="17"/>
-      <c r="AK74" s="17"/>
-      <c r="AL74" s="17"/>
-      <c r="AM74" s="17"/>
+      <c r="Z74" s="13"/>
+      <c r="AA74" s="13"/>
+      <c r="AB74" s="13"/>
+      <c r="AC74" s="13"/>
+      <c r="AD74" s="13"/>
+      <c r="AE74" s="13"/>
+      <c r="AF74" s="13"/>
+      <c r="AG74" s="13"/>
+      <c r="AH74" s="13"/>
+      <c r="AI74" s="13"/>
+      <c r="AJ74" s="13"/>
+      <c r="AK74" s="13"/>
+      <c r="AL74" s="13"/>
+      <c r="AM74" s="13"/>
       <c r="AN74" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AO74" s="16"/>
       <c r="AP74" s="16"/>
@@ -9351,45 +9355,45 @@
       <c r="BG74" s="16"/>
       <c r="BH74" s="16"/>
       <c r="BI74" s="16"/>
-      <c r="BJ74" s="17" t="s">
-        <v>25</v>
+      <c r="BJ74" s="13" t="s">
+        <v>24</v>
       </c>
-      <c r="BK74" s="17"/>
-      <c r="BL74" s="17"/>
-      <c r="BM74" s="17"/>
-      <c r="BN74" s="17"/>
-      <c r="BO74" s="17"/>
-      <c r="BP74" s="17"/>
-      <c r="BQ74" s="17"/>
-      <c r="BR74" s="17"/>
-      <c r="BS74" s="17"/>
-      <c r="BT74" s="17"/>
-      <c r="BU74" s="17"/>
-      <c r="BV74" s="17"/>
-      <c r="BW74" s="17"/>
-      <c r="BX74" s="17"/>
-      <c r="BY74" s="17"/>
-      <c r="BZ74" s="17"/>
-      <c r="CA74" s="17"/>
-      <c r="CB74" s="17"/>
-      <c r="CC74" s="17"/>
-      <c r="CD74" s="17"/>
-      <c r="CE74" s="17"/>
-      <c r="CF74" s="17"/>
-      <c r="CG74" s="17"/>
-      <c r="CH74" s="17"/>
-      <c r="CI74" s="17"/>
-      <c r="CJ74" s="17"/>
-      <c r="CK74" s="17"/>
-      <c r="CL74" s="17"/>
-      <c r="CM74" s="17"/>
-      <c r="CN74" s="17"/>
-      <c r="CO74" s="17"/>
-      <c r="CP74" s="17"/>
-      <c r="CQ74" s="17"/>
-      <c r="CR74" s="17"/>
-      <c r="CS74" s="17"/>
-      <c r="CT74" s="18"/>
+      <c r="BK74" s="13"/>
+      <c r="BL74" s="13"/>
+      <c r="BM74" s="13"/>
+      <c r="BN74" s="13"/>
+      <c r="BO74" s="13"/>
+      <c r="BP74" s="13"/>
+      <c r="BQ74" s="13"/>
+      <c r="BR74" s="13"/>
+      <c r="BS74" s="13"/>
+      <c r="BT74" s="13"/>
+      <c r="BU74" s="13"/>
+      <c r="BV74" s="13"/>
+      <c r="BW74" s="13"/>
+      <c r="BX74" s="13"/>
+      <c r="BY74" s="13"/>
+      <c r="BZ74" s="13"/>
+      <c r="CA74" s="13"/>
+      <c r="CB74" s="13"/>
+      <c r="CC74" s="13"/>
+      <c r="CD74" s="13"/>
+      <c r="CE74" s="13"/>
+      <c r="CF74" s="13"/>
+      <c r="CG74" s="13"/>
+      <c r="CH74" s="13"/>
+      <c r="CI74" s="13"/>
+      <c r="CJ74" s="13"/>
+      <c r="CK74" s="13"/>
+      <c r="CL74" s="13"/>
+      <c r="CM74" s="13"/>
+      <c r="CN74" s="13"/>
+      <c r="CO74" s="13"/>
+      <c r="CP74" s="13"/>
+      <c r="CQ74" s="13"/>
+      <c r="CR74" s="13"/>
+      <c r="CS74" s="13"/>
+      <c r="CT74" s="14"/>
     </row>
     <row r="75" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C75" s="15">
@@ -9398,43 +9402,43 @@
       <c r="D75" s="16"/>
       <c r="E75" s="16"/>
       <c r="F75" s="16"/>
-      <c r="G75" s="17" t="s">
-        <v>26</v>
+      <c r="G75" s="13" t="s">
+        <v>25</v>
       </c>
-      <c r="H75" s="17"/>
-      <c r="I75" s="17"/>
-      <c r="J75" s="17"/>
-      <c r="K75" s="17"/>
-      <c r="L75" s="17"/>
-      <c r="M75" s="17"/>
-      <c r="N75" s="17"/>
-      <c r="O75" s="17"/>
-      <c r="P75" s="17"/>
-      <c r="Q75" s="17"/>
-      <c r="R75" s="17"/>
-      <c r="S75" s="17"/>
-      <c r="T75" s="17"/>
-      <c r="U75" s="17"/>
-      <c r="V75" s="17"/>
-      <c r="W75" s="17"/>
-      <c r="X75" s="17"/>
-      <c r="Y75" s="17" t="s">
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
+      <c r="M75" s="13"/>
+      <c r="N75" s="13"/>
+      <c r="O75" s="13"/>
+      <c r="P75" s="13"/>
+      <c r="Q75" s="13"/>
+      <c r="R75" s="13"/>
+      <c r="S75" s="13"/>
+      <c r="T75" s="13"/>
+      <c r="U75" s="13"/>
+      <c r="V75" s="13"/>
+      <c r="W75" s="13"/>
+      <c r="X75" s="13"/>
+      <c r="Y75" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="Z75" s="17"/>
-      <c r="AA75" s="17"/>
-      <c r="AB75" s="17"/>
-      <c r="AC75" s="17"/>
-      <c r="AD75" s="17"/>
-      <c r="AE75" s="17"/>
-      <c r="AF75" s="17"/>
-      <c r="AG75" s="17"/>
-      <c r="AH75" s="17"/>
-      <c r="AI75" s="17"/>
-      <c r="AJ75" s="17"/>
-      <c r="AK75" s="17"/>
-      <c r="AL75" s="17"/>
-      <c r="AM75" s="17"/>
+      <c r="Z75" s="13"/>
+      <c r="AA75" s="13"/>
+      <c r="AB75" s="13"/>
+      <c r="AC75" s="13"/>
+      <c r="AD75" s="13"/>
+      <c r="AE75" s="13"/>
+      <c r="AF75" s="13"/>
+      <c r="AG75" s="13"/>
+      <c r="AH75" s="13"/>
+      <c r="AI75" s="13"/>
+      <c r="AJ75" s="13"/>
+      <c r="AK75" s="13"/>
+      <c r="AL75" s="13"/>
+      <c r="AM75" s="13"/>
       <c r="AN75" s="16" t="s">
         <v>13</v>
       </c>
@@ -9459,43 +9463,43 @@
       <c r="BG75" s="16"/>
       <c r="BH75" s="16"/>
       <c r="BI75" s="16"/>
-      <c r="BJ75" s="17"/>
-      <c r="BK75" s="17"/>
-      <c r="BL75" s="17"/>
-      <c r="BM75" s="17"/>
-      <c r="BN75" s="17"/>
-      <c r="BO75" s="17"/>
-      <c r="BP75" s="17"/>
-      <c r="BQ75" s="17"/>
-      <c r="BR75" s="17"/>
-      <c r="BS75" s="17"/>
-      <c r="BT75" s="17"/>
-      <c r="BU75" s="17"/>
-      <c r="BV75" s="17"/>
-      <c r="BW75" s="17"/>
-      <c r="BX75" s="17"/>
-      <c r="BY75" s="17"/>
-      <c r="BZ75" s="17"/>
-      <c r="CA75" s="17"/>
-      <c r="CB75" s="17"/>
-      <c r="CC75" s="17"/>
-      <c r="CD75" s="17"/>
-      <c r="CE75" s="17"/>
-      <c r="CF75" s="17"/>
-      <c r="CG75" s="17"/>
-      <c r="CH75" s="17"/>
-      <c r="CI75" s="17"/>
-      <c r="CJ75" s="17"/>
-      <c r="CK75" s="17"/>
-      <c r="CL75" s="17"/>
-      <c r="CM75" s="17"/>
-      <c r="CN75" s="17"/>
-      <c r="CO75" s="17"/>
-      <c r="CP75" s="17"/>
-      <c r="CQ75" s="17"/>
-      <c r="CR75" s="17"/>
-      <c r="CS75" s="17"/>
-      <c r="CT75" s="18"/>
+      <c r="BJ75" s="13"/>
+      <c r="BK75" s="13"/>
+      <c r="BL75" s="13"/>
+      <c r="BM75" s="13"/>
+      <c r="BN75" s="13"/>
+      <c r="BO75" s="13"/>
+      <c r="BP75" s="13"/>
+      <c r="BQ75" s="13"/>
+      <c r="BR75" s="13"/>
+      <c r="BS75" s="13"/>
+      <c r="BT75" s="13"/>
+      <c r="BU75" s="13"/>
+      <c r="BV75" s="13"/>
+      <c r="BW75" s="13"/>
+      <c r="BX75" s="13"/>
+      <c r="BY75" s="13"/>
+      <c r="BZ75" s="13"/>
+      <c r="CA75" s="13"/>
+      <c r="CB75" s="13"/>
+      <c r="CC75" s="13"/>
+      <c r="CD75" s="13"/>
+      <c r="CE75" s="13"/>
+      <c r="CF75" s="13"/>
+      <c r="CG75" s="13"/>
+      <c r="CH75" s="13"/>
+      <c r="CI75" s="13"/>
+      <c r="CJ75" s="13"/>
+      <c r="CK75" s="13"/>
+      <c r="CL75" s="13"/>
+      <c r="CM75" s="13"/>
+      <c r="CN75" s="13"/>
+      <c r="CO75" s="13"/>
+      <c r="CP75" s="13"/>
+      <c r="CQ75" s="13"/>
+      <c r="CR75" s="13"/>
+      <c r="CS75" s="13"/>
+      <c r="CT75" s="14"/>
     </row>
     <row r="76" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C76" s="15">
@@ -9504,43 +9508,43 @@
       <c r="D76" s="16"/>
       <c r="E76" s="16"/>
       <c r="F76" s="16"/>
-      <c r="G76" s="17" t="s">
-        <v>27</v>
+      <c r="G76" s="13" t="s">
+        <v>26</v>
       </c>
-      <c r="H76" s="17"/>
-      <c r="I76" s="17"/>
-      <c r="J76" s="17"/>
-      <c r="K76" s="17"/>
-      <c r="L76" s="17"/>
-      <c r="M76" s="17"/>
-      <c r="N76" s="17"/>
-      <c r="O76" s="17"/>
-      <c r="P76" s="17"/>
-      <c r="Q76" s="17"/>
-      <c r="R76" s="17"/>
-      <c r="S76" s="17"/>
-      <c r="T76" s="17"/>
-      <c r="U76" s="17"/>
-      <c r="V76" s="17"/>
-      <c r="W76" s="17"/>
-      <c r="X76" s="17"/>
-      <c r="Y76" s="17" t="s">
+      <c r="H76" s="13"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="13"/>
+      <c r="L76" s="13"/>
+      <c r="M76" s="13"/>
+      <c r="N76" s="13"/>
+      <c r="O76" s="13"/>
+      <c r="P76" s="13"/>
+      <c r="Q76" s="13"/>
+      <c r="R76" s="13"/>
+      <c r="S76" s="13"/>
+      <c r="T76" s="13"/>
+      <c r="U76" s="13"/>
+      <c r="V76" s="13"/>
+      <c r="W76" s="13"/>
+      <c r="X76" s="13"/>
+      <c r="Y76" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="Z76" s="17"/>
-      <c r="AA76" s="17"/>
-      <c r="AB76" s="17"/>
-      <c r="AC76" s="17"/>
-      <c r="AD76" s="17"/>
-      <c r="AE76" s="17"/>
-      <c r="AF76" s="17"/>
-      <c r="AG76" s="17"/>
-      <c r="AH76" s="17"/>
-      <c r="AI76" s="17"/>
-      <c r="AJ76" s="17"/>
-      <c r="AK76" s="17"/>
-      <c r="AL76" s="17"/>
-      <c r="AM76" s="17"/>
+      <c r="Z76" s="13"/>
+      <c r="AA76" s="13"/>
+      <c r="AB76" s="13"/>
+      <c r="AC76" s="13"/>
+      <c r="AD76" s="13"/>
+      <c r="AE76" s="13"/>
+      <c r="AF76" s="13"/>
+      <c r="AG76" s="13"/>
+      <c r="AH76" s="13"/>
+      <c r="AI76" s="13"/>
+      <c r="AJ76" s="13"/>
+      <c r="AK76" s="13"/>
+      <c r="AL76" s="13"/>
+      <c r="AM76" s="13"/>
       <c r="AN76" s="16" t="s">
         <v>13</v>
       </c>
@@ -9565,43 +9569,43 @@
       <c r="BG76" s="16"/>
       <c r="BH76" s="16"/>
       <c r="BI76" s="16"/>
-      <c r="BJ76" s="17"/>
-      <c r="BK76" s="17"/>
-      <c r="BL76" s="17"/>
-      <c r="BM76" s="17"/>
-      <c r="BN76" s="17"/>
-      <c r="BO76" s="17"/>
-      <c r="BP76" s="17"/>
-      <c r="BQ76" s="17"/>
-      <c r="BR76" s="17"/>
-      <c r="BS76" s="17"/>
-      <c r="BT76" s="17"/>
-      <c r="BU76" s="17"/>
-      <c r="BV76" s="17"/>
-      <c r="BW76" s="17"/>
-      <c r="BX76" s="17"/>
-      <c r="BY76" s="17"/>
-      <c r="BZ76" s="17"/>
-      <c r="CA76" s="17"/>
-      <c r="CB76" s="17"/>
-      <c r="CC76" s="17"/>
-      <c r="CD76" s="17"/>
-      <c r="CE76" s="17"/>
-      <c r="CF76" s="17"/>
-      <c r="CG76" s="17"/>
-      <c r="CH76" s="17"/>
-      <c r="CI76" s="17"/>
-      <c r="CJ76" s="17"/>
-      <c r="CK76" s="17"/>
-      <c r="CL76" s="17"/>
-      <c r="CM76" s="17"/>
-      <c r="CN76" s="17"/>
-      <c r="CO76" s="17"/>
-      <c r="CP76" s="17"/>
-      <c r="CQ76" s="17"/>
-      <c r="CR76" s="17"/>
-      <c r="CS76" s="17"/>
-      <c r="CT76" s="18"/>
+      <c r="BJ76" s="13"/>
+      <c r="BK76" s="13"/>
+      <c r="BL76" s="13"/>
+      <c r="BM76" s="13"/>
+      <c r="BN76" s="13"/>
+      <c r="BO76" s="13"/>
+      <c r="BP76" s="13"/>
+      <c r="BQ76" s="13"/>
+      <c r="BR76" s="13"/>
+      <c r="BS76" s="13"/>
+      <c r="BT76" s="13"/>
+      <c r="BU76" s="13"/>
+      <c r="BV76" s="13"/>
+      <c r="BW76" s="13"/>
+      <c r="BX76" s="13"/>
+      <c r="BY76" s="13"/>
+      <c r="BZ76" s="13"/>
+      <c r="CA76" s="13"/>
+      <c r="CB76" s="13"/>
+      <c r="CC76" s="13"/>
+      <c r="CD76" s="13"/>
+      <c r="CE76" s="13"/>
+      <c r="CF76" s="13"/>
+      <c r="CG76" s="13"/>
+      <c r="CH76" s="13"/>
+      <c r="CI76" s="13"/>
+      <c r="CJ76" s="13"/>
+      <c r="CK76" s="13"/>
+      <c r="CL76" s="13"/>
+      <c r="CM76" s="13"/>
+      <c r="CN76" s="13"/>
+      <c r="CO76" s="13"/>
+      <c r="CP76" s="13"/>
+      <c r="CQ76" s="13"/>
+      <c r="CR76" s="13"/>
+      <c r="CS76" s="13"/>
+      <c r="CT76" s="14"/>
     </row>
     <row r="77" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C77" s="15">
@@ -9610,39 +9614,39 @@
       <c r="D77" s="16"/>
       <c r="E77" s="16"/>
       <c r="F77" s="16"/>
-      <c r="G77" s="22"/>
-      <c r="H77" s="17"/>
-      <c r="I77" s="17"/>
-      <c r="J77" s="17"/>
-      <c r="K77" s="17"/>
-      <c r="L77" s="17"/>
-      <c r="M77" s="17"/>
-      <c r="N77" s="17"/>
-      <c r="O77" s="17"/>
-      <c r="P77" s="17"/>
-      <c r="Q77" s="17"/>
-      <c r="R77" s="17"/>
-      <c r="S77" s="17"/>
-      <c r="T77" s="17"/>
-      <c r="U77" s="17"/>
-      <c r="V77" s="17"/>
-      <c r="W77" s="17"/>
-      <c r="X77" s="17"/>
-      <c r="Y77" s="17"/>
-      <c r="Z77" s="17"/>
-      <c r="AA77" s="17"/>
-      <c r="AB77" s="17"/>
-      <c r="AC77" s="17"/>
-      <c r="AD77" s="17"/>
-      <c r="AE77" s="17"/>
-      <c r="AF77" s="17"/>
-      <c r="AG77" s="17"/>
-      <c r="AH77" s="17"/>
-      <c r="AI77" s="17"/>
-      <c r="AJ77" s="17"/>
-      <c r="AK77" s="17"/>
-      <c r="AL77" s="17"/>
-      <c r="AM77" s="17"/>
+      <c r="G77" s="27"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="13"/>
+      <c r="K77" s="13"/>
+      <c r="L77" s="13"/>
+      <c r="M77" s="13"/>
+      <c r="N77" s="13"/>
+      <c r="O77" s="13"/>
+      <c r="P77" s="13"/>
+      <c r="Q77" s="13"/>
+      <c r="R77" s="13"/>
+      <c r="S77" s="13"/>
+      <c r="T77" s="13"/>
+      <c r="U77" s="13"/>
+      <c r="V77" s="13"/>
+      <c r="W77" s="13"/>
+      <c r="X77" s="13"/>
+      <c r="Y77" s="13"/>
+      <c r="Z77" s="13"/>
+      <c r="AA77" s="13"/>
+      <c r="AB77" s="13"/>
+      <c r="AC77" s="13"/>
+      <c r="AD77" s="13"/>
+      <c r="AE77" s="13"/>
+      <c r="AF77" s="13"/>
+      <c r="AG77" s="13"/>
+      <c r="AH77" s="13"/>
+      <c r="AI77" s="13"/>
+      <c r="AJ77" s="13"/>
+      <c r="AK77" s="13"/>
+      <c r="AL77" s="13"/>
+      <c r="AM77" s="13"/>
       <c r="AN77" s="16"/>
       <c r="AO77" s="16"/>
       <c r="AP77" s="16"/>
@@ -9665,82 +9669,82 @@
       <c r="BG77" s="16"/>
       <c r="BH77" s="16"/>
       <c r="BI77" s="16"/>
-      <c r="BJ77" s="17"/>
-      <c r="BK77" s="17"/>
-      <c r="BL77" s="17"/>
-      <c r="BM77" s="17"/>
-      <c r="BN77" s="17"/>
-      <c r="BO77" s="17"/>
-      <c r="BP77" s="17"/>
-      <c r="BQ77" s="17"/>
-      <c r="BR77" s="17"/>
-      <c r="BS77" s="17"/>
-      <c r="BT77" s="17"/>
-      <c r="BU77" s="17"/>
-      <c r="BV77" s="17"/>
-      <c r="BW77" s="17"/>
-      <c r="BX77" s="17"/>
-      <c r="BY77" s="17"/>
-      <c r="BZ77" s="17"/>
-      <c r="CA77" s="17"/>
-      <c r="CB77" s="17"/>
-      <c r="CC77" s="17"/>
-      <c r="CD77" s="17"/>
-      <c r="CE77" s="17"/>
-      <c r="CF77" s="17"/>
-      <c r="CG77" s="17"/>
-      <c r="CH77" s="17"/>
-      <c r="CI77" s="17"/>
-      <c r="CJ77" s="17"/>
-      <c r="CK77" s="17"/>
-      <c r="CL77" s="17"/>
-      <c r="CM77" s="17"/>
-      <c r="CN77" s="17"/>
-      <c r="CO77" s="17"/>
-      <c r="CP77" s="17"/>
-      <c r="CQ77" s="17"/>
-      <c r="CR77" s="17"/>
-      <c r="CS77" s="17"/>
-      <c r="CT77" s="18"/>
+      <c r="BJ77" s="13"/>
+      <c r="BK77" s="13"/>
+      <c r="BL77" s="13"/>
+      <c r="BM77" s="13"/>
+      <c r="BN77" s="13"/>
+      <c r="BO77" s="13"/>
+      <c r="BP77" s="13"/>
+      <c r="BQ77" s="13"/>
+      <c r="BR77" s="13"/>
+      <c r="BS77" s="13"/>
+      <c r="BT77" s="13"/>
+      <c r="BU77" s="13"/>
+      <c r="BV77" s="13"/>
+      <c r="BW77" s="13"/>
+      <c r="BX77" s="13"/>
+      <c r="BY77" s="13"/>
+      <c r="BZ77" s="13"/>
+      <c r="CA77" s="13"/>
+      <c r="CB77" s="13"/>
+      <c r="CC77" s="13"/>
+      <c r="CD77" s="13"/>
+      <c r="CE77" s="13"/>
+      <c r="CF77" s="13"/>
+      <c r="CG77" s="13"/>
+      <c r="CH77" s="13"/>
+      <c r="CI77" s="13"/>
+      <c r="CJ77" s="13"/>
+      <c r="CK77" s="13"/>
+      <c r="CL77" s="13"/>
+      <c r="CM77" s="13"/>
+      <c r="CN77" s="13"/>
+      <c r="CO77" s="13"/>
+      <c r="CP77" s="13"/>
+      <c r="CQ77" s="13"/>
+      <c r="CR77" s="13"/>
+      <c r="CS77" s="13"/>
+      <c r="CT77" s="14"/>
     </row>
     <row r="78" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C78" s="15"/>
       <c r="D78" s="16"/>
       <c r="E78" s="16"/>
       <c r="F78" s="16"/>
-      <c r="G78" s="17"/>
-      <c r="H78" s="17"/>
-      <c r="I78" s="17"/>
-      <c r="J78" s="17"/>
-      <c r="K78" s="17"/>
-      <c r="L78" s="17"/>
-      <c r="M78" s="17"/>
-      <c r="N78" s="17"/>
-      <c r="O78" s="17"/>
-      <c r="P78" s="17"/>
-      <c r="Q78" s="17"/>
-      <c r="R78" s="17"/>
-      <c r="S78" s="17"/>
-      <c r="T78" s="17"/>
-      <c r="U78" s="17"/>
-      <c r="V78" s="17"/>
-      <c r="W78" s="17"/>
-      <c r="X78" s="17"/>
-      <c r="Y78" s="17"/>
-      <c r="Z78" s="17"/>
-      <c r="AA78" s="17"/>
-      <c r="AB78" s="17"/>
-      <c r="AC78" s="17"/>
-      <c r="AD78" s="17"/>
-      <c r="AE78" s="17"/>
-      <c r="AF78" s="17"/>
-      <c r="AG78" s="17"/>
-      <c r="AH78" s="17"/>
-      <c r="AI78" s="17"/>
-      <c r="AJ78" s="17"/>
-      <c r="AK78" s="17"/>
-      <c r="AL78" s="17"/>
-      <c r="AM78" s="17"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="13"/>
+      <c r="J78" s="13"/>
+      <c r="K78" s="13"/>
+      <c r="L78" s="13"/>
+      <c r="M78" s="13"/>
+      <c r="N78" s="13"/>
+      <c r="O78" s="13"/>
+      <c r="P78" s="13"/>
+      <c r="Q78" s="13"/>
+      <c r="R78" s="13"/>
+      <c r="S78" s="13"/>
+      <c r="T78" s="13"/>
+      <c r="U78" s="13"/>
+      <c r="V78" s="13"/>
+      <c r="W78" s="13"/>
+      <c r="X78" s="13"/>
+      <c r="Y78" s="13"/>
+      <c r="Z78" s="13"/>
+      <c r="AA78" s="13"/>
+      <c r="AB78" s="13"/>
+      <c r="AC78" s="13"/>
+      <c r="AD78" s="13"/>
+      <c r="AE78" s="13"/>
+      <c r="AF78" s="13"/>
+      <c r="AG78" s="13"/>
+      <c r="AH78" s="13"/>
+      <c r="AI78" s="13"/>
+      <c r="AJ78" s="13"/>
+      <c r="AK78" s="13"/>
+      <c r="AL78" s="13"/>
+      <c r="AM78" s="13"/>
       <c r="AN78" s="16"/>
       <c r="AO78" s="16"/>
       <c r="AP78" s="16"/>
@@ -9763,141 +9767,141 @@
       <c r="BG78" s="16"/>
       <c r="BH78" s="16"/>
       <c r="BI78" s="16"/>
-      <c r="BJ78" s="17"/>
-      <c r="BK78" s="17"/>
-      <c r="BL78" s="17"/>
-      <c r="BM78" s="17"/>
-      <c r="BN78" s="17"/>
-      <c r="BO78" s="17"/>
-      <c r="BP78" s="17"/>
-      <c r="BQ78" s="17"/>
-      <c r="BR78" s="17"/>
-      <c r="BS78" s="17"/>
-      <c r="BT78" s="17"/>
-      <c r="BU78" s="17"/>
-      <c r="BV78" s="17"/>
-      <c r="BW78" s="17"/>
-      <c r="BX78" s="17"/>
-      <c r="BY78" s="17"/>
-      <c r="BZ78" s="17"/>
-      <c r="CA78" s="17"/>
-      <c r="CB78" s="17"/>
-      <c r="CC78" s="17"/>
-      <c r="CD78" s="17"/>
-      <c r="CE78" s="17"/>
-      <c r="CF78" s="17"/>
-      <c r="CG78" s="17"/>
-      <c r="CH78" s="17"/>
-      <c r="CI78" s="17"/>
-      <c r="CJ78" s="17"/>
-      <c r="CK78" s="17"/>
-      <c r="CL78" s="17"/>
-      <c r="CM78" s="17"/>
-      <c r="CN78" s="17"/>
-      <c r="CO78" s="17"/>
-      <c r="CP78" s="17"/>
-      <c r="CQ78" s="17"/>
-      <c r="CR78" s="17"/>
-      <c r="CS78" s="17"/>
-      <c r="CT78" s="18"/>
+      <c r="BJ78" s="13"/>
+      <c r="BK78" s="13"/>
+      <c r="BL78" s="13"/>
+      <c r="BM78" s="13"/>
+      <c r="BN78" s="13"/>
+      <c r="BO78" s="13"/>
+      <c r="BP78" s="13"/>
+      <c r="BQ78" s="13"/>
+      <c r="BR78" s="13"/>
+      <c r="BS78" s="13"/>
+      <c r="BT78" s="13"/>
+      <c r="BU78" s="13"/>
+      <c r="BV78" s="13"/>
+      <c r="BW78" s="13"/>
+      <c r="BX78" s="13"/>
+      <c r="BY78" s="13"/>
+      <c r="BZ78" s="13"/>
+      <c r="CA78" s="13"/>
+      <c r="CB78" s="13"/>
+      <c r="CC78" s="13"/>
+      <c r="CD78" s="13"/>
+      <c r="CE78" s="13"/>
+      <c r="CF78" s="13"/>
+      <c r="CG78" s="13"/>
+      <c r="CH78" s="13"/>
+      <c r="CI78" s="13"/>
+      <c r="CJ78" s="13"/>
+      <c r="CK78" s="13"/>
+      <c r="CL78" s="13"/>
+      <c r="CM78" s="13"/>
+      <c r="CN78" s="13"/>
+      <c r="CO78" s="13"/>
+      <c r="CP78" s="13"/>
+      <c r="CQ78" s="13"/>
+      <c r="CR78" s="13"/>
+      <c r="CS78" s="13"/>
+      <c r="CT78" s="14"/>
     </row>
     <row r="79" spans="3:98" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C79" s="19"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="20"/>
-      <c r="G79" s="13"/>
-      <c r="H79" s="13"/>
-      <c r="I79" s="13"/>
-      <c r="J79" s="13"/>
-      <c r="K79" s="13"/>
-      <c r="L79" s="13"/>
-      <c r="M79" s="13"/>
-      <c r="N79" s="13"/>
-      <c r="O79" s="13"/>
-      <c r="P79" s="13"/>
-      <c r="Q79" s="13"/>
-      <c r="R79" s="13"/>
-      <c r="S79" s="13"/>
-      <c r="T79" s="13"/>
-      <c r="U79" s="13"/>
-      <c r="V79" s="13"/>
-      <c r="W79" s="13"/>
-      <c r="X79" s="13"/>
-      <c r="Y79" s="13"/>
-      <c r="Z79" s="13"/>
-      <c r="AA79" s="13"/>
-      <c r="AB79" s="13"/>
-      <c r="AC79" s="13"/>
-      <c r="AD79" s="13"/>
-      <c r="AE79" s="13"/>
-      <c r="AF79" s="13"/>
-      <c r="AG79" s="13"/>
-      <c r="AH79" s="13"/>
-      <c r="AI79" s="13"/>
-      <c r="AJ79" s="13"/>
-      <c r="AK79" s="13"/>
-      <c r="AL79" s="13"/>
-      <c r="AM79" s="13"/>
-      <c r="AN79" s="20"/>
-      <c r="AO79" s="20"/>
-      <c r="AP79" s="20"/>
-      <c r="AQ79" s="20"/>
-      <c r="AR79" s="20"/>
-      <c r="AS79" s="20"/>
-      <c r="AT79" s="20"/>
-      <c r="AU79" s="20"/>
-      <c r="AV79" s="20"/>
-      <c r="AW79" s="20"/>
-      <c r="AX79" s="20"/>
-      <c r="AY79" s="20"/>
-      <c r="AZ79" s="20"/>
-      <c r="BA79" s="20"/>
-      <c r="BB79" s="20"/>
-      <c r="BC79" s="20"/>
-      <c r="BD79" s="20"/>
-      <c r="BE79" s="20"/>
-      <c r="BF79" s="20"/>
-      <c r="BG79" s="20"/>
-      <c r="BH79" s="20"/>
-      <c r="BI79" s="20"/>
-      <c r="BJ79" s="13"/>
-      <c r="BK79" s="13"/>
-      <c r="BL79" s="13"/>
-      <c r="BM79" s="13"/>
-      <c r="BN79" s="13"/>
-      <c r="BO79" s="13"/>
-      <c r="BP79" s="13"/>
-      <c r="BQ79" s="13"/>
-      <c r="BR79" s="13"/>
-      <c r="BS79" s="13"/>
-      <c r="BT79" s="13"/>
-      <c r="BU79" s="13"/>
-      <c r="BV79" s="13"/>
-      <c r="BW79" s="13"/>
-      <c r="BX79" s="13"/>
-      <c r="BY79" s="13"/>
-      <c r="BZ79" s="13"/>
-      <c r="CA79" s="13"/>
-      <c r="CB79" s="13"/>
-      <c r="CC79" s="13"/>
-      <c r="CD79" s="13"/>
-      <c r="CE79" s="13"/>
-      <c r="CF79" s="13"/>
-      <c r="CG79" s="13"/>
-      <c r="CH79" s="13"/>
-      <c r="CI79" s="13"/>
-      <c r="CJ79" s="13"/>
-      <c r="CK79" s="13"/>
-      <c r="CL79" s="13"/>
-      <c r="CM79" s="13"/>
-      <c r="CN79" s="13"/>
-      <c r="CO79" s="13"/>
-      <c r="CP79" s="13"/>
-      <c r="CQ79" s="13"/>
-      <c r="CR79" s="13"/>
-      <c r="CS79" s="13"/>
-      <c r="CT79" s="14"/>
+      <c r="C79" s="30"/>
+      <c r="D79" s="31"/>
+      <c r="E79" s="31"/>
+      <c r="F79" s="31"/>
+      <c r="G79" s="28"/>
+      <c r="H79" s="28"/>
+      <c r="I79" s="28"/>
+      <c r="J79" s="28"/>
+      <c r="K79" s="28"/>
+      <c r="L79" s="28"/>
+      <c r="M79" s="28"/>
+      <c r="N79" s="28"/>
+      <c r="O79" s="28"/>
+      <c r="P79" s="28"/>
+      <c r="Q79" s="28"/>
+      <c r="R79" s="28"/>
+      <c r="S79" s="28"/>
+      <c r="T79" s="28"/>
+      <c r="U79" s="28"/>
+      <c r="V79" s="28"/>
+      <c r="W79" s="28"/>
+      <c r="X79" s="28"/>
+      <c r="Y79" s="28"/>
+      <c r="Z79" s="28"/>
+      <c r="AA79" s="28"/>
+      <c r="AB79" s="28"/>
+      <c r="AC79" s="28"/>
+      <c r="AD79" s="28"/>
+      <c r="AE79" s="28"/>
+      <c r="AF79" s="28"/>
+      <c r="AG79" s="28"/>
+      <c r="AH79" s="28"/>
+      <c r="AI79" s="28"/>
+      <c r="AJ79" s="28"/>
+      <c r="AK79" s="28"/>
+      <c r="AL79" s="28"/>
+      <c r="AM79" s="28"/>
+      <c r="AN79" s="31"/>
+      <c r="AO79" s="31"/>
+      <c r="AP79" s="31"/>
+      <c r="AQ79" s="31"/>
+      <c r="AR79" s="31"/>
+      <c r="AS79" s="31"/>
+      <c r="AT79" s="31"/>
+      <c r="AU79" s="31"/>
+      <c r="AV79" s="31"/>
+      <c r="AW79" s="31"/>
+      <c r="AX79" s="31"/>
+      <c r="AY79" s="31"/>
+      <c r="AZ79" s="31"/>
+      <c r="BA79" s="31"/>
+      <c r="BB79" s="31"/>
+      <c r="BC79" s="31"/>
+      <c r="BD79" s="31"/>
+      <c r="BE79" s="31"/>
+      <c r="BF79" s="31"/>
+      <c r="BG79" s="31"/>
+      <c r="BH79" s="31"/>
+      <c r="BI79" s="31"/>
+      <c r="BJ79" s="28"/>
+      <c r="BK79" s="28"/>
+      <c r="BL79" s="28"/>
+      <c r="BM79" s="28"/>
+      <c r="BN79" s="28"/>
+      <c r="BO79" s="28"/>
+      <c r="BP79" s="28"/>
+      <c r="BQ79" s="28"/>
+      <c r="BR79" s="28"/>
+      <c r="BS79" s="28"/>
+      <c r="BT79" s="28"/>
+      <c r="BU79" s="28"/>
+      <c r="BV79" s="28"/>
+      <c r="BW79" s="28"/>
+      <c r="BX79" s="28"/>
+      <c r="BY79" s="28"/>
+      <c r="BZ79" s="28"/>
+      <c r="CA79" s="28"/>
+      <c r="CB79" s="28"/>
+      <c r="CC79" s="28"/>
+      <c r="CD79" s="28"/>
+      <c r="CE79" s="28"/>
+      <c r="CF79" s="28"/>
+      <c r="CG79" s="28"/>
+      <c r="CH79" s="28"/>
+      <c r="CI79" s="28"/>
+      <c r="CJ79" s="28"/>
+      <c r="CK79" s="28"/>
+      <c r="CL79" s="28"/>
+      <c r="CM79" s="28"/>
+      <c r="CN79" s="28"/>
+      <c r="CO79" s="28"/>
+      <c r="CP79" s="28"/>
+      <c r="CQ79" s="28"/>
+      <c r="CR79" s="28"/>
+      <c r="CS79" s="28"/>
+      <c r="CT79" s="29"/>
     </row>
     <row r="80" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9907,30 +9911,42 @@
     <row r="85" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="BZ71:CT71"/>
-    <mergeCell ref="C71:F71"/>
-    <mergeCell ref="G71:X71"/>
-    <mergeCell ref="Y71:AM71"/>
-    <mergeCell ref="AN71:BI71"/>
-    <mergeCell ref="BJ71:BY71"/>
-    <mergeCell ref="BZ69:CT69"/>
-    <mergeCell ref="A1:F3"/>
-    <mergeCell ref="A4:F6"/>
-    <mergeCell ref="G1:AD3"/>
-    <mergeCell ref="G4:AD6"/>
-    <mergeCell ref="BZ68:CT68"/>
-    <mergeCell ref="BJ68:BY68"/>
-    <mergeCell ref="AN68:BI68"/>
-    <mergeCell ref="Y68:AM68"/>
-    <mergeCell ref="G68:X68"/>
-    <mergeCell ref="C68:F68"/>
-    <mergeCell ref="Y70:AM70"/>
-    <mergeCell ref="AN70:BI70"/>
-    <mergeCell ref="BJ70:BY70"/>
-    <mergeCell ref="C69:F69"/>
-    <mergeCell ref="G69:X69"/>
-    <mergeCell ref="Y69:AM69"/>
-    <mergeCell ref="AN69:BI69"/>
+    <mergeCell ref="BZ79:CT79"/>
+    <mergeCell ref="C78:F78"/>
+    <mergeCell ref="G78:X78"/>
+    <mergeCell ref="Y78:AM78"/>
+    <mergeCell ref="AN78:BI78"/>
+    <mergeCell ref="BJ78:BY78"/>
+    <mergeCell ref="BZ78:CT78"/>
+    <mergeCell ref="C79:F79"/>
+    <mergeCell ref="G79:X79"/>
+    <mergeCell ref="Y79:AM79"/>
+    <mergeCell ref="AN79:BI79"/>
+    <mergeCell ref="BJ79:BY79"/>
+    <mergeCell ref="BZ77:CT77"/>
+    <mergeCell ref="C76:F76"/>
+    <mergeCell ref="G76:X76"/>
+    <mergeCell ref="Y76:AM76"/>
+    <mergeCell ref="AN76:BI76"/>
+    <mergeCell ref="BJ76:BY76"/>
+    <mergeCell ref="BZ76:CT76"/>
+    <mergeCell ref="C77:F77"/>
+    <mergeCell ref="G77:X77"/>
+    <mergeCell ref="Y77:AM77"/>
+    <mergeCell ref="AN77:BI77"/>
+    <mergeCell ref="BJ77:BY77"/>
+    <mergeCell ref="BZ75:CT75"/>
+    <mergeCell ref="C74:F74"/>
+    <mergeCell ref="G74:X74"/>
+    <mergeCell ref="Y74:AM74"/>
+    <mergeCell ref="AN74:BI74"/>
+    <mergeCell ref="BJ74:BY74"/>
+    <mergeCell ref="BZ74:CT74"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="G75:X75"/>
+    <mergeCell ref="Y75:AM75"/>
+    <mergeCell ref="AN75:BI75"/>
+    <mergeCell ref="BJ75:BY75"/>
     <mergeCell ref="BZ70:CT70"/>
     <mergeCell ref="BJ69:BY69"/>
     <mergeCell ref="BZ73:CT73"/>
@@ -9947,42 +9963,30 @@
     <mergeCell ref="BJ73:BY73"/>
     <mergeCell ref="C70:F70"/>
     <mergeCell ref="G70:X70"/>
-    <mergeCell ref="BZ75:CT75"/>
-    <mergeCell ref="C74:F74"/>
-    <mergeCell ref="G74:X74"/>
-    <mergeCell ref="Y74:AM74"/>
-    <mergeCell ref="AN74:BI74"/>
-    <mergeCell ref="BJ74:BY74"/>
-    <mergeCell ref="BZ74:CT74"/>
-    <mergeCell ref="C75:F75"/>
-    <mergeCell ref="G75:X75"/>
-    <mergeCell ref="Y75:AM75"/>
-    <mergeCell ref="AN75:BI75"/>
-    <mergeCell ref="BJ75:BY75"/>
-    <mergeCell ref="BZ77:CT77"/>
-    <mergeCell ref="C76:F76"/>
-    <mergeCell ref="G76:X76"/>
-    <mergeCell ref="Y76:AM76"/>
-    <mergeCell ref="AN76:BI76"/>
-    <mergeCell ref="BJ76:BY76"/>
-    <mergeCell ref="BZ76:CT76"/>
-    <mergeCell ref="C77:F77"/>
-    <mergeCell ref="G77:X77"/>
-    <mergeCell ref="Y77:AM77"/>
-    <mergeCell ref="AN77:BI77"/>
-    <mergeCell ref="BJ77:BY77"/>
-    <mergeCell ref="BZ79:CT79"/>
-    <mergeCell ref="C78:F78"/>
-    <mergeCell ref="G78:X78"/>
-    <mergeCell ref="Y78:AM78"/>
-    <mergeCell ref="AN78:BI78"/>
-    <mergeCell ref="BJ78:BY78"/>
-    <mergeCell ref="BZ78:CT78"/>
-    <mergeCell ref="C79:F79"/>
-    <mergeCell ref="G79:X79"/>
-    <mergeCell ref="Y79:AM79"/>
-    <mergeCell ref="AN79:BI79"/>
-    <mergeCell ref="BJ79:BY79"/>
+    <mergeCell ref="Y70:AM70"/>
+    <mergeCell ref="AN70:BI70"/>
+    <mergeCell ref="BJ70:BY70"/>
+    <mergeCell ref="C69:F69"/>
+    <mergeCell ref="G69:X69"/>
+    <mergeCell ref="Y69:AM69"/>
+    <mergeCell ref="AN69:BI69"/>
+    <mergeCell ref="BZ69:CT69"/>
+    <mergeCell ref="A1:F3"/>
+    <mergeCell ref="A4:F6"/>
+    <mergeCell ref="G1:AD3"/>
+    <mergeCell ref="G4:AD6"/>
+    <mergeCell ref="BZ68:CT68"/>
+    <mergeCell ref="BJ68:BY68"/>
+    <mergeCell ref="AN68:BI68"/>
+    <mergeCell ref="Y68:AM68"/>
+    <mergeCell ref="G68:X68"/>
+    <mergeCell ref="C68:F68"/>
+    <mergeCell ref="BZ71:CT71"/>
+    <mergeCell ref="C71:F71"/>
+    <mergeCell ref="G71:X71"/>
+    <mergeCell ref="Y71:AM71"/>
+    <mergeCell ref="AN71:BI71"/>
+    <mergeCell ref="BJ71:BY71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Mobile transport service basic
</commit_message>
<xml_diff>
--- a/Documents/ScreenLayouts/Dashboard-Customer.xlsx
+++ b/Documents/ScreenLayouts/Dashboard-Customer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev/booking/Documents/ScreenLayouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD1DAF4-76AA-B844-93CF-41772951DA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8FDC28-2978-1744-9D64-7FEB516D959E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{90052BEC-FEBB-F247-ACB1-709744DE85BE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{90052BEC-FEBB-F247-ACB1-709744DE85BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="5" r:id="rId1"/>
@@ -480,10 +480,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -492,8 +493,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -516,28 +538,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2658,8 +2658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43867302-6022-BC45-9802-796B2A9AA285}">
   <dimension ref="A1:DD85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="CB33" sqref="CB33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="BJ73" sqref="BJ73:BY73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2" defaultRowHeight="8" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2668,204 +2668,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="20" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
     </row>
     <row r="2" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="28"/>
     </row>
     <row r="3" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="20"/>
-      <c r="W3" s="20"/>
-      <c r="X3" s="20"/>
-      <c r="Y3" s="20"/>
-      <c r="Z3" s="20"/>
-      <c r="AA3" s="20"/>
-      <c r="AB3" s="20"/>
-      <c r="AC3" s="20"/>
-      <c r="AD3" s="20"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="28"/>
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
+      <c r="X3" s="28"/>
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="28"/>
+      <c r="AD3" s="28"/>
     </row>
     <row r="4" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="21" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="21"/>
-      <c r="X4" s="21"/>
-      <c r="Y4" s="21"/>
-      <c r="Z4" s="21"/>
-      <c r="AA4" s="21"/>
-      <c r="AB4" s="21"/>
-      <c r="AC4" s="21"/>
-      <c r="AD4" s="21"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="29"/>
+      <c r="W4" s="29"/>
+      <c r="X4" s="29"/>
+      <c r="Y4" s="29"/>
+      <c r="Z4" s="29"/>
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="29"/>
+      <c r="AC4" s="29"/>
+      <c r="AD4" s="29"/>
     </row>
     <row r="5" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21"/>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="21"/>
-      <c r="AC5" s="21"/>
-      <c r="AD5" s="21"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="29"/>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="29"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="29"/>
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="29"/>
+      <c r="AD5" s="29"/>
     </row>
     <row r="6" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
-      <c r="W6" s="21"/>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="21"/>
-      <c r="AA6" s="21"/>
-      <c r="AB6" s="21"/>
-      <c r="AC6" s="21"/>
-      <c r="AD6" s="21"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="29"/>
+      <c r="X6" s="29"/>
+      <c r="Y6" s="29"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="29"/>
+      <c r="AB6" s="29"/>
+      <c r="AC6" s="29"/>
+      <c r="AD6" s="29"/>
     </row>
     <row r="9" spans="1:108" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
@@ -5010,7 +5010,7 @@
       <c r="BQ29" s="5"/>
       <c r="BR29" s="5"/>
       <c r="BS29" s="5"/>
-      <c r="BT29" s="32"/>
+      <c r="BT29" s="13"/>
       <c r="BU29" s="5"/>
       <c r="BV29" s="5"/>
       <c r="BW29" s="5"/>
@@ -8638,1270 +8638,1270 @@
       <c r="CT67" s="11"/>
     </row>
     <row r="68" spans="3:98" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C68" s="24" t="s">
+      <c r="C68" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D68" s="22"/>
-      <c r="E68" s="22"/>
-      <c r="F68" s="22"/>
-      <c r="G68" s="22" t="s">
+      <c r="D68" s="30"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="30"/>
+      <c r="G68" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="H68" s="22"/>
-      <c r="I68" s="22"/>
-      <c r="J68" s="22"/>
-      <c r="K68" s="22"/>
-      <c r="L68" s="22"/>
-      <c r="M68" s="22"/>
-      <c r="N68" s="22"/>
-      <c r="O68" s="22"/>
-      <c r="P68" s="22"/>
-      <c r="Q68" s="22"/>
-      <c r="R68" s="22"/>
-      <c r="S68" s="22"/>
-      <c r="T68" s="22"/>
-      <c r="U68" s="22"/>
-      <c r="V68" s="22"/>
-      <c r="W68" s="22"/>
-      <c r="X68" s="22"/>
-      <c r="Y68" s="22" t="s">
+      <c r="H68" s="30"/>
+      <c r="I68" s="30"/>
+      <c r="J68" s="30"/>
+      <c r="K68" s="30"/>
+      <c r="L68" s="30"/>
+      <c r="M68" s="30"/>
+      <c r="N68" s="30"/>
+      <c r="O68" s="30"/>
+      <c r="P68" s="30"/>
+      <c r="Q68" s="30"/>
+      <c r="R68" s="30"/>
+      <c r="S68" s="30"/>
+      <c r="T68" s="30"/>
+      <c r="U68" s="30"/>
+      <c r="V68" s="30"/>
+      <c r="W68" s="30"/>
+      <c r="X68" s="30"/>
+      <c r="Y68" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="Z68" s="22"/>
-      <c r="AA68" s="22"/>
-      <c r="AB68" s="22"/>
-      <c r="AC68" s="22"/>
-      <c r="AD68" s="22"/>
-      <c r="AE68" s="22"/>
-      <c r="AF68" s="22"/>
-      <c r="AG68" s="22"/>
-      <c r="AH68" s="22"/>
-      <c r="AI68" s="22"/>
-      <c r="AJ68" s="22"/>
-      <c r="AK68" s="22"/>
-      <c r="AL68" s="22"/>
-      <c r="AM68" s="22"/>
-      <c r="AN68" s="22" t="s">
+      <c r="Z68" s="30"/>
+      <c r="AA68" s="30"/>
+      <c r="AB68" s="30"/>
+      <c r="AC68" s="30"/>
+      <c r="AD68" s="30"/>
+      <c r="AE68" s="30"/>
+      <c r="AF68" s="30"/>
+      <c r="AG68" s="30"/>
+      <c r="AH68" s="30"/>
+      <c r="AI68" s="30"/>
+      <c r="AJ68" s="30"/>
+      <c r="AK68" s="30"/>
+      <c r="AL68" s="30"/>
+      <c r="AM68" s="30"/>
+      <c r="AN68" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="AO68" s="22"/>
-      <c r="AP68" s="22"/>
-      <c r="AQ68" s="22"/>
-      <c r="AR68" s="22"/>
-      <c r="AS68" s="22"/>
-      <c r="AT68" s="22"/>
-      <c r="AU68" s="22"/>
-      <c r="AV68" s="22"/>
-      <c r="AW68" s="22"/>
-      <c r="AX68" s="22"/>
-      <c r="AY68" s="22"/>
-      <c r="AZ68" s="22"/>
-      <c r="BA68" s="22"/>
-      <c r="BB68" s="22"/>
-      <c r="BC68" s="22"/>
-      <c r="BD68" s="22"/>
-      <c r="BE68" s="22"/>
-      <c r="BF68" s="22"/>
-      <c r="BG68" s="22"/>
-      <c r="BH68" s="22"/>
-      <c r="BI68" s="22"/>
-      <c r="BJ68" s="22" t="s">
+      <c r="AO68" s="30"/>
+      <c r="AP68" s="30"/>
+      <c r="AQ68" s="30"/>
+      <c r="AR68" s="30"/>
+      <c r="AS68" s="30"/>
+      <c r="AT68" s="30"/>
+      <c r="AU68" s="30"/>
+      <c r="AV68" s="30"/>
+      <c r="AW68" s="30"/>
+      <c r="AX68" s="30"/>
+      <c r="AY68" s="30"/>
+      <c r="AZ68" s="30"/>
+      <c r="BA68" s="30"/>
+      <c r="BB68" s="30"/>
+      <c r="BC68" s="30"/>
+      <c r="BD68" s="30"/>
+      <c r="BE68" s="30"/>
+      <c r="BF68" s="30"/>
+      <c r="BG68" s="30"/>
+      <c r="BH68" s="30"/>
+      <c r="BI68" s="30"/>
+      <c r="BJ68" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="BK68" s="22"/>
-      <c r="BL68" s="22"/>
-      <c r="BM68" s="22"/>
-      <c r="BN68" s="22"/>
-      <c r="BO68" s="22"/>
-      <c r="BP68" s="22"/>
-      <c r="BQ68" s="22"/>
-      <c r="BR68" s="22"/>
-      <c r="BS68" s="22"/>
-      <c r="BT68" s="22"/>
-      <c r="BU68" s="22"/>
-      <c r="BV68" s="22"/>
-      <c r="BW68" s="22"/>
-      <c r="BX68" s="22"/>
-      <c r="BY68" s="22"/>
-      <c r="BZ68" s="22" t="s">
+      <c r="BK68" s="30"/>
+      <c r="BL68" s="30"/>
+      <c r="BM68" s="30"/>
+      <c r="BN68" s="30"/>
+      <c r="BO68" s="30"/>
+      <c r="BP68" s="30"/>
+      <c r="BQ68" s="30"/>
+      <c r="BR68" s="30"/>
+      <c r="BS68" s="30"/>
+      <c r="BT68" s="30"/>
+      <c r="BU68" s="30"/>
+      <c r="BV68" s="30"/>
+      <c r="BW68" s="30"/>
+      <c r="BX68" s="30"/>
+      <c r="BY68" s="30"/>
+      <c r="BZ68" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="CA68" s="22"/>
-      <c r="CB68" s="22"/>
-      <c r="CC68" s="22"/>
-      <c r="CD68" s="22"/>
-      <c r="CE68" s="22"/>
-      <c r="CF68" s="22"/>
-      <c r="CG68" s="22"/>
-      <c r="CH68" s="22"/>
-      <c r="CI68" s="22"/>
-      <c r="CJ68" s="22"/>
-      <c r="CK68" s="22"/>
-      <c r="CL68" s="22"/>
-      <c r="CM68" s="22"/>
-      <c r="CN68" s="22"/>
-      <c r="CO68" s="22"/>
-      <c r="CP68" s="22"/>
-      <c r="CQ68" s="22"/>
-      <c r="CR68" s="22"/>
-      <c r="CS68" s="22"/>
-      <c r="CT68" s="23"/>
+      <c r="CA68" s="30"/>
+      <c r="CB68" s="30"/>
+      <c r="CC68" s="30"/>
+      <c r="CD68" s="30"/>
+      <c r="CE68" s="30"/>
+      <c r="CF68" s="30"/>
+      <c r="CG68" s="30"/>
+      <c r="CH68" s="30"/>
+      <c r="CI68" s="30"/>
+      <c r="CJ68" s="30"/>
+      <c r="CK68" s="30"/>
+      <c r="CL68" s="30"/>
+      <c r="CM68" s="30"/>
+      <c r="CN68" s="30"/>
+      <c r="CO68" s="30"/>
+      <c r="CP68" s="30"/>
+      <c r="CQ68" s="30"/>
+      <c r="CR68" s="30"/>
+      <c r="CS68" s="30"/>
+      <c r="CT68" s="31"/>
     </row>
     <row r="69" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C69" s="25">
+      <c r="C69" s="24">
         <v>1</v>
       </c>
-      <c r="D69" s="26"/>
-      <c r="E69" s="26"/>
-      <c r="F69" s="26"/>
-      <c r="G69" s="17" t="s">
+      <c r="D69" s="25"/>
+      <c r="E69" s="25"/>
+      <c r="F69" s="25"/>
+      <c r="G69" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H69" s="17"/>
-      <c r="I69" s="17"/>
-      <c r="J69" s="17"/>
-      <c r="K69" s="17"/>
-      <c r="L69" s="17"/>
-      <c r="M69" s="17"/>
-      <c r="N69" s="17"/>
-      <c r="O69" s="17"/>
-      <c r="P69" s="17"/>
-      <c r="Q69" s="17"/>
-      <c r="R69" s="17"/>
-      <c r="S69" s="17"/>
-      <c r="T69" s="17"/>
-      <c r="U69" s="17"/>
-      <c r="V69" s="17"/>
-      <c r="W69" s="17"/>
-      <c r="X69" s="17"/>
-      <c r="Y69" s="17" t="s">
+      <c r="H69" s="23"/>
+      <c r="I69" s="23"/>
+      <c r="J69" s="23"/>
+      <c r="K69" s="23"/>
+      <c r="L69" s="23"/>
+      <c r="M69" s="23"/>
+      <c r="N69" s="23"/>
+      <c r="O69" s="23"/>
+      <c r="P69" s="23"/>
+      <c r="Q69" s="23"/>
+      <c r="R69" s="23"/>
+      <c r="S69" s="23"/>
+      <c r="T69" s="23"/>
+      <c r="U69" s="23"/>
+      <c r="V69" s="23"/>
+      <c r="W69" s="23"/>
+      <c r="X69" s="23"/>
+      <c r="Y69" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="Z69" s="17"/>
-      <c r="AA69" s="17"/>
-      <c r="AB69" s="17"/>
-      <c r="AC69" s="17"/>
-      <c r="AD69" s="17"/>
-      <c r="AE69" s="17"/>
-      <c r="AF69" s="17"/>
-      <c r="AG69" s="17"/>
-      <c r="AH69" s="17"/>
-      <c r="AI69" s="17"/>
-      <c r="AJ69" s="17"/>
-      <c r="AK69" s="17"/>
-      <c r="AL69" s="17"/>
-      <c r="AM69" s="17"/>
-      <c r="AN69" s="26" t="s">
+      <c r="Z69" s="23"/>
+      <c r="AA69" s="23"/>
+      <c r="AB69" s="23"/>
+      <c r="AC69" s="23"/>
+      <c r="AD69" s="23"/>
+      <c r="AE69" s="23"/>
+      <c r="AF69" s="23"/>
+      <c r="AG69" s="23"/>
+      <c r="AH69" s="23"/>
+      <c r="AI69" s="23"/>
+      <c r="AJ69" s="23"/>
+      <c r="AK69" s="23"/>
+      <c r="AL69" s="23"/>
+      <c r="AM69" s="23"/>
+      <c r="AN69" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="AO69" s="26"/>
-      <c r="AP69" s="26"/>
-      <c r="AQ69" s="26"/>
-      <c r="AR69" s="26"/>
-      <c r="AS69" s="26"/>
-      <c r="AT69" s="26"/>
-      <c r="AU69" s="26"/>
-      <c r="AV69" s="26"/>
-      <c r="AW69" s="26"/>
-      <c r="AX69" s="26"/>
-      <c r="AY69" s="26"/>
-      <c r="AZ69" s="26"/>
-      <c r="BA69" s="26"/>
-      <c r="BB69" s="26"/>
-      <c r="BC69" s="26"/>
-      <c r="BD69" s="26"/>
-      <c r="BE69" s="26"/>
-      <c r="BF69" s="26"/>
-      <c r="BG69" s="26"/>
-      <c r="BH69" s="26"/>
-      <c r="BI69" s="26"/>
-      <c r="BJ69" s="17" t="s">
+      <c r="AO69" s="25"/>
+      <c r="AP69" s="25"/>
+      <c r="AQ69" s="25"/>
+      <c r="AR69" s="25"/>
+      <c r="AS69" s="25"/>
+      <c r="AT69" s="25"/>
+      <c r="AU69" s="25"/>
+      <c r="AV69" s="25"/>
+      <c r="AW69" s="25"/>
+      <c r="AX69" s="25"/>
+      <c r="AY69" s="25"/>
+      <c r="AZ69" s="25"/>
+      <c r="BA69" s="25"/>
+      <c r="BB69" s="25"/>
+      <c r="BC69" s="25"/>
+      <c r="BD69" s="25"/>
+      <c r="BE69" s="25"/>
+      <c r="BF69" s="25"/>
+      <c r="BG69" s="25"/>
+      <c r="BH69" s="25"/>
+      <c r="BI69" s="25"/>
+      <c r="BJ69" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="BK69" s="17"/>
-      <c r="BL69" s="17"/>
-      <c r="BM69" s="17"/>
-      <c r="BN69" s="17"/>
-      <c r="BO69" s="17"/>
-      <c r="BP69" s="17"/>
-      <c r="BQ69" s="17"/>
-      <c r="BR69" s="17"/>
-      <c r="BS69" s="17"/>
-      <c r="BT69" s="17"/>
-      <c r="BU69" s="17"/>
-      <c r="BV69" s="17"/>
-      <c r="BW69" s="17"/>
-      <c r="BX69" s="17"/>
-      <c r="BY69" s="17"/>
-      <c r="BZ69" s="17"/>
-      <c r="CA69" s="17"/>
-      <c r="CB69" s="17"/>
-      <c r="CC69" s="17"/>
-      <c r="CD69" s="17"/>
-      <c r="CE69" s="17"/>
-      <c r="CF69" s="17"/>
-      <c r="CG69" s="17"/>
-      <c r="CH69" s="17"/>
-      <c r="CI69" s="17"/>
-      <c r="CJ69" s="17"/>
-      <c r="CK69" s="17"/>
-      <c r="CL69" s="17"/>
-      <c r="CM69" s="17"/>
-      <c r="CN69" s="17"/>
-      <c r="CO69" s="17"/>
-      <c r="CP69" s="17"/>
-      <c r="CQ69" s="17"/>
-      <c r="CR69" s="17"/>
-      <c r="CS69" s="17"/>
-      <c r="CT69" s="18"/>
+      <c r="BK69" s="23"/>
+      <c r="BL69" s="23"/>
+      <c r="BM69" s="23"/>
+      <c r="BN69" s="23"/>
+      <c r="BO69" s="23"/>
+      <c r="BP69" s="23"/>
+      <c r="BQ69" s="23"/>
+      <c r="BR69" s="23"/>
+      <c r="BS69" s="23"/>
+      <c r="BT69" s="23"/>
+      <c r="BU69" s="23"/>
+      <c r="BV69" s="23"/>
+      <c r="BW69" s="23"/>
+      <c r="BX69" s="23"/>
+      <c r="BY69" s="23"/>
+      <c r="BZ69" s="23"/>
+      <c r="CA69" s="23"/>
+      <c r="CB69" s="23"/>
+      <c r="CC69" s="23"/>
+      <c r="CD69" s="23"/>
+      <c r="CE69" s="23"/>
+      <c r="CF69" s="23"/>
+      <c r="CG69" s="23"/>
+      <c r="CH69" s="23"/>
+      <c r="CI69" s="23"/>
+      <c r="CJ69" s="23"/>
+      <c r="CK69" s="23"/>
+      <c r="CL69" s="23"/>
+      <c r="CM69" s="23"/>
+      <c r="CN69" s="23"/>
+      <c r="CO69" s="23"/>
+      <c r="CP69" s="23"/>
+      <c r="CQ69" s="23"/>
+      <c r="CR69" s="23"/>
+      <c r="CS69" s="23"/>
+      <c r="CT69" s="26"/>
     </row>
     <row r="70" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C70" s="15">
+      <c r="C70" s="16">
         <v>2</v>
       </c>
-      <c r="D70" s="16"/>
-      <c r="E70" s="16"/>
-      <c r="F70" s="16"/>
-      <c r="G70" s="27" t="s">
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H70" s="13"/>
-      <c r="I70" s="13"/>
-      <c r="J70" s="13"/>
-      <c r="K70" s="13"/>
-      <c r="L70" s="13"/>
-      <c r="M70" s="13"/>
-      <c r="N70" s="13"/>
-      <c r="O70" s="13"/>
-      <c r="P70" s="13"/>
-      <c r="Q70" s="13"/>
-      <c r="R70" s="13"/>
-      <c r="S70" s="13"/>
-      <c r="T70" s="13"/>
-      <c r="U70" s="13"/>
-      <c r="V70" s="13"/>
-      <c r="W70" s="13"/>
-      <c r="X70" s="13"/>
-      <c r="Y70" s="13" t="s">
+      <c r="H70" s="18"/>
+      <c r="I70" s="18"/>
+      <c r="J70" s="18"/>
+      <c r="K70" s="18"/>
+      <c r="L70" s="18"/>
+      <c r="M70" s="18"/>
+      <c r="N70" s="18"/>
+      <c r="O70" s="18"/>
+      <c r="P70" s="18"/>
+      <c r="Q70" s="18"/>
+      <c r="R70" s="18"/>
+      <c r="S70" s="18"/>
+      <c r="T70" s="18"/>
+      <c r="U70" s="18"/>
+      <c r="V70" s="18"/>
+      <c r="W70" s="18"/>
+      <c r="X70" s="18"/>
+      <c r="Y70" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="Z70" s="13"/>
-      <c r="AA70" s="13"/>
-      <c r="AB70" s="13"/>
-      <c r="AC70" s="13"/>
-      <c r="AD70" s="13"/>
-      <c r="AE70" s="13"/>
-      <c r="AF70" s="13"/>
-      <c r="AG70" s="13"/>
-      <c r="AH70" s="13"/>
-      <c r="AI70" s="13"/>
-      <c r="AJ70" s="13"/>
-      <c r="AK70" s="13"/>
-      <c r="AL70" s="13"/>
-      <c r="AM70" s="13"/>
-      <c r="AN70" s="16" t="s">
+      <c r="Z70" s="18"/>
+      <c r="AA70" s="18"/>
+      <c r="AB70" s="18"/>
+      <c r="AC70" s="18"/>
+      <c r="AD70" s="18"/>
+      <c r="AE70" s="18"/>
+      <c r="AF70" s="18"/>
+      <c r="AG70" s="18"/>
+      <c r="AH70" s="18"/>
+      <c r="AI70" s="18"/>
+      <c r="AJ70" s="18"/>
+      <c r="AK70" s="18"/>
+      <c r="AL70" s="18"/>
+      <c r="AM70" s="18"/>
+      <c r="AN70" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="AO70" s="16"/>
-      <c r="AP70" s="16"/>
-      <c r="AQ70" s="16"/>
-      <c r="AR70" s="16"/>
-      <c r="AS70" s="16"/>
-      <c r="AT70" s="16"/>
-      <c r="AU70" s="16"/>
-      <c r="AV70" s="16"/>
-      <c r="AW70" s="16"/>
-      <c r="AX70" s="16"/>
-      <c r="AY70" s="16"/>
-      <c r="AZ70" s="16"/>
-      <c r="BA70" s="16"/>
-      <c r="BB70" s="16"/>
-      <c r="BC70" s="16"/>
-      <c r="BD70" s="16"/>
-      <c r="BE70" s="16"/>
-      <c r="BF70" s="16"/>
-      <c r="BG70" s="16"/>
-      <c r="BH70" s="16"/>
-      <c r="BI70" s="16"/>
-      <c r="BJ70" s="13" t="s">
+      <c r="AO70" s="17"/>
+      <c r="AP70" s="17"/>
+      <c r="AQ70" s="17"/>
+      <c r="AR70" s="17"/>
+      <c r="AS70" s="17"/>
+      <c r="AT70" s="17"/>
+      <c r="AU70" s="17"/>
+      <c r="AV70" s="17"/>
+      <c r="AW70" s="17"/>
+      <c r="AX70" s="17"/>
+      <c r="AY70" s="17"/>
+      <c r="AZ70" s="17"/>
+      <c r="BA70" s="17"/>
+      <c r="BB70" s="17"/>
+      <c r="BC70" s="17"/>
+      <c r="BD70" s="17"/>
+      <c r="BE70" s="17"/>
+      <c r="BF70" s="17"/>
+      <c r="BG70" s="17"/>
+      <c r="BH70" s="17"/>
+      <c r="BI70" s="17"/>
+      <c r="BJ70" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="BK70" s="13"/>
-      <c r="BL70" s="13"/>
-      <c r="BM70" s="13"/>
-      <c r="BN70" s="13"/>
-      <c r="BO70" s="13"/>
-      <c r="BP70" s="13"/>
-      <c r="BQ70" s="13"/>
-      <c r="BR70" s="13"/>
-      <c r="BS70" s="13"/>
-      <c r="BT70" s="13"/>
-      <c r="BU70" s="13"/>
-      <c r="BV70" s="13"/>
-      <c r="BW70" s="13"/>
-      <c r="BX70" s="13"/>
-      <c r="BY70" s="13"/>
-      <c r="BZ70" s="13"/>
-      <c r="CA70" s="13"/>
-      <c r="CB70" s="13"/>
-      <c r="CC70" s="13"/>
-      <c r="CD70" s="13"/>
-      <c r="CE70" s="13"/>
-      <c r="CF70" s="13"/>
-      <c r="CG70" s="13"/>
-      <c r="CH70" s="13"/>
-      <c r="CI70" s="13"/>
-      <c r="CJ70" s="13"/>
-      <c r="CK70" s="13"/>
-      <c r="CL70" s="13"/>
-      <c r="CM70" s="13"/>
-      <c r="CN70" s="13"/>
-      <c r="CO70" s="13"/>
-      <c r="CP70" s="13"/>
-      <c r="CQ70" s="13"/>
-      <c r="CR70" s="13"/>
-      <c r="CS70" s="13"/>
-      <c r="CT70" s="14"/>
+      <c r="BK70" s="18"/>
+      <c r="BL70" s="18"/>
+      <c r="BM70" s="18"/>
+      <c r="BN70" s="18"/>
+      <c r="BO70" s="18"/>
+      <c r="BP70" s="18"/>
+      <c r="BQ70" s="18"/>
+      <c r="BR70" s="18"/>
+      <c r="BS70" s="18"/>
+      <c r="BT70" s="18"/>
+      <c r="BU70" s="18"/>
+      <c r="BV70" s="18"/>
+      <c r="BW70" s="18"/>
+      <c r="BX70" s="18"/>
+      <c r="BY70" s="18"/>
+      <c r="BZ70" s="18"/>
+      <c r="CA70" s="18"/>
+      <c r="CB70" s="18"/>
+      <c r="CC70" s="18"/>
+      <c r="CD70" s="18"/>
+      <c r="CE70" s="18"/>
+      <c r="CF70" s="18"/>
+      <c r="CG70" s="18"/>
+      <c r="CH70" s="18"/>
+      <c r="CI70" s="18"/>
+      <c r="CJ70" s="18"/>
+      <c r="CK70" s="18"/>
+      <c r="CL70" s="18"/>
+      <c r="CM70" s="18"/>
+      <c r="CN70" s="18"/>
+      <c r="CO70" s="18"/>
+      <c r="CP70" s="18"/>
+      <c r="CQ70" s="18"/>
+      <c r="CR70" s="18"/>
+      <c r="CS70" s="18"/>
+      <c r="CT70" s="19"/>
     </row>
     <row r="71" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C71" s="15">
+      <c r="C71" s="16">
         <v>3</v>
       </c>
-      <c r="D71" s="16"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="16"/>
-      <c r="G71" s="13" t="s">
+      <c r="D71" s="17"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H71" s="13"/>
-      <c r="I71" s="13"/>
-      <c r="J71" s="13"/>
-      <c r="K71" s="13"/>
-      <c r="L71" s="13"/>
-      <c r="M71" s="13"/>
-      <c r="N71" s="13"/>
-      <c r="O71" s="13"/>
-      <c r="P71" s="13"/>
-      <c r="Q71" s="13"/>
-      <c r="R71" s="13"/>
-      <c r="S71" s="13"/>
-      <c r="T71" s="13"/>
-      <c r="U71" s="13"/>
-      <c r="V71" s="13"/>
-      <c r="W71" s="13"/>
-      <c r="X71" s="13"/>
-      <c r="Y71" s="13" t="s">
+      <c r="H71" s="18"/>
+      <c r="I71" s="18"/>
+      <c r="J71" s="18"/>
+      <c r="K71" s="18"/>
+      <c r="L71" s="18"/>
+      <c r="M71" s="18"/>
+      <c r="N71" s="18"/>
+      <c r="O71" s="18"/>
+      <c r="P71" s="18"/>
+      <c r="Q71" s="18"/>
+      <c r="R71" s="18"/>
+      <c r="S71" s="18"/>
+      <c r="T71" s="18"/>
+      <c r="U71" s="18"/>
+      <c r="V71" s="18"/>
+      <c r="W71" s="18"/>
+      <c r="X71" s="18"/>
+      <c r="Y71" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="Z71" s="13"/>
-      <c r="AA71" s="13"/>
-      <c r="AB71" s="13"/>
-      <c r="AC71" s="13"/>
-      <c r="AD71" s="13"/>
-      <c r="AE71" s="13"/>
-      <c r="AF71" s="13"/>
-      <c r="AG71" s="13"/>
-      <c r="AH71" s="13"/>
-      <c r="AI71" s="13"/>
-      <c r="AJ71" s="13"/>
-      <c r="AK71" s="13"/>
-      <c r="AL71" s="13"/>
-      <c r="AM71" s="13"/>
-      <c r="AN71" s="16" t="s">
+      <c r="Z71" s="18"/>
+      <c r="AA71" s="18"/>
+      <c r="AB71" s="18"/>
+      <c r="AC71" s="18"/>
+      <c r="AD71" s="18"/>
+      <c r="AE71" s="18"/>
+      <c r="AF71" s="18"/>
+      <c r="AG71" s="18"/>
+      <c r="AH71" s="18"/>
+      <c r="AI71" s="18"/>
+      <c r="AJ71" s="18"/>
+      <c r="AK71" s="18"/>
+      <c r="AL71" s="18"/>
+      <c r="AM71" s="18"/>
+      <c r="AN71" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="AO71" s="16"/>
-      <c r="AP71" s="16"/>
-      <c r="AQ71" s="16"/>
-      <c r="AR71" s="16"/>
-      <c r="AS71" s="16"/>
-      <c r="AT71" s="16"/>
-      <c r="AU71" s="16"/>
-      <c r="AV71" s="16"/>
-      <c r="AW71" s="16"/>
-      <c r="AX71" s="16"/>
-      <c r="AY71" s="16"/>
-      <c r="AZ71" s="16"/>
-      <c r="BA71" s="16"/>
-      <c r="BB71" s="16"/>
-      <c r="BC71" s="16"/>
-      <c r="BD71" s="16"/>
-      <c r="BE71" s="16"/>
-      <c r="BF71" s="16"/>
-      <c r="BG71" s="16"/>
-      <c r="BH71" s="16"/>
-      <c r="BI71" s="16"/>
-      <c r="BJ71" s="13" t="s">
+      <c r="AO71" s="17"/>
+      <c r="AP71" s="17"/>
+      <c r="AQ71" s="17"/>
+      <c r="AR71" s="17"/>
+      <c r="AS71" s="17"/>
+      <c r="AT71" s="17"/>
+      <c r="AU71" s="17"/>
+      <c r="AV71" s="17"/>
+      <c r="AW71" s="17"/>
+      <c r="AX71" s="17"/>
+      <c r="AY71" s="17"/>
+      <c r="AZ71" s="17"/>
+      <c r="BA71" s="17"/>
+      <c r="BB71" s="17"/>
+      <c r="BC71" s="17"/>
+      <c r="BD71" s="17"/>
+      <c r="BE71" s="17"/>
+      <c r="BF71" s="17"/>
+      <c r="BG71" s="17"/>
+      <c r="BH71" s="17"/>
+      <c r="BI71" s="17"/>
+      <c r="BJ71" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="BK71" s="13"/>
-      <c r="BL71" s="13"/>
-      <c r="BM71" s="13"/>
-      <c r="BN71" s="13"/>
-      <c r="BO71" s="13"/>
-      <c r="BP71" s="13"/>
-      <c r="BQ71" s="13"/>
-      <c r="BR71" s="13"/>
-      <c r="BS71" s="13"/>
-      <c r="BT71" s="13"/>
-      <c r="BU71" s="13"/>
-      <c r="BV71" s="13"/>
-      <c r="BW71" s="13"/>
-      <c r="BX71" s="13"/>
-      <c r="BY71" s="13"/>
-      <c r="BZ71" s="13"/>
-      <c r="CA71" s="13"/>
-      <c r="CB71" s="13"/>
-      <c r="CC71" s="13"/>
-      <c r="CD71" s="13"/>
-      <c r="CE71" s="13"/>
-      <c r="CF71" s="13"/>
-      <c r="CG71" s="13"/>
-      <c r="CH71" s="13"/>
-      <c r="CI71" s="13"/>
-      <c r="CJ71" s="13"/>
-      <c r="CK71" s="13"/>
-      <c r="CL71" s="13"/>
-      <c r="CM71" s="13"/>
-      <c r="CN71" s="13"/>
-      <c r="CO71" s="13"/>
-      <c r="CP71" s="13"/>
-      <c r="CQ71" s="13"/>
-      <c r="CR71" s="13"/>
-      <c r="CS71" s="13"/>
-      <c r="CT71" s="14"/>
+      <c r="BK71" s="18"/>
+      <c r="BL71" s="18"/>
+      <c r="BM71" s="18"/>
+      <c r="BN71" s="18"/>
+      <c r="BO71" s="18"/>
+      <c r="BP71" s="18"/>
+      <c r="BQ71" s="18"/>
+      <c r="BR71" s="18"/>
+      <c r="BS71" s="18"/>
+      <c r="BT71" s="18"/>
+      <c r="BU71" s="18"/>
+      <c r="BV71" s="18"/>
+      <c r="BW71" s="18"/>
+      <c r="BX71" s="18"/>
+      <c r="BY71" s="18"/>
+      <c r="BZ71" s="18"/>
+      <c r="CA71" s="18"/>
+      <c r="CB71" s="18"/>
+      <c r="CC71" s="18"/>
+      <c r="CD71" s="18"/>
+      <c r="CE71" s="18"/>
+      <c r="CF71" s="18"/>
+      <c r="CG71" s="18"/>
+      <c r="CH71" s="18"/>
+      <c r="CI71" s="18"/>
+      <c r="CJ71" s="18"/>
+      <c r="CK71" s="18"/>
+      <c r="CL71" s="18"/>
+      <c r="CM71" s="18"/>
+      <c r="CN71" s="18"/>
+      <c r="CO71" s="18"/>
+      <c r="CP71" s="18"/>
+      <c r="CQ71" s="18"/>
+      <c r="CR71" s="18"/>
+      <c r="CS71" s="18"/>
+      <c r="CT71" s="19"/>
     </row>
     <row r="72" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C72" s="15">
+      <c r="C72" s="16">
         <v>4</v>
       </c>
-      <c r="D72" s="16"/>
-      <c r="E72" s="16"/>
-      <c r="F72" s="16"/>
-      <c r="G72" s="13" t="s">
+      <c r="D72" s="17"/>
+      <c r="E72" s="17"/>
+      <c r="F72" s="17"/>
+      <c r="G72" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H72" s="13"/>
-      <c r="I72" s="13"/>
-      <c r="J72" s="13"/>
-      <c r="K72" s="13"/>
-      <c r="L72" s="13"/>
-      <c r="M72" s="13"/>
-      <c r="N72" s="13"/>
-      <c r="O72" s="13"/>
-      <c r="P72" s="13"/>
-      <c r="Q72" s="13"/>
-      <c r="R72" s="13"/>
-      <c r="S72" s="13"/>
-      <c r="T72" s="13"/>
-      <c r="U72" s="13"/>
-      <c r="V72" s="13"/>
-      <c r="W72" s="13"/>
-      <c r="X72" s="13"/>
-      <c r="Y72" s="13" t="s">
+      <c r="H72" s="18"/>
+      <c r="I72" s="18"/>
+      <c r="J72" s="18"/>
+      <c r="K72" s="18"/>
+      <c r="L72" s="18"/>
+      <c r="M72" s="18"/>
+      <c r="N72" s="18"/>
+      <c r="O72" s="18"/>
+      <c r="P72" s="18"/>
+      <c r="Q72" s="18"/>
+      <c r="R72" s="18"/>
+      <c r="S72" s="18"/>
+      <c r="T72" s="18"/>
+      <c r="U72" s="18"/>
+      <c r="V72" s="18"/>
+      <c r="W72" s="18"/>
+      <c r="X72" s="18"/>
+      <c r="Y72" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="Z72" s="13"/>
-      <c r="AA72" s="13"/>
-      <c r="AB72" s="13"/>
-      <c r="AC72" s="13"/>
-      <c r="AD72" s="13"/>
-      <c r="AE72" s="13"/>
-      <c r="AF72" s="13"/>
-      <c r="AG72" s="13"/>
-      <c r="AH72" s="13"/>
-      <c r="AI72" s="13"/>
-      <c r="AJ72" s="13"/>
-      <c r="AK72" s="13"/>
-      <c r="AL72" s="13"/>
-      <c r="AM72" s="13"/>
-      <c r="AN72" s="16" t="s">
+      <c r="Z72" s="18"/>
+      <c r="AA72" s="18"/>
+      <c r="AB72" s="18"/>
+      <c r="AC72" s="18"/>
+      <c r="AD72" s="18"/>
+      <c r="AE72" s="18"/>
+      <c r="AF72" s="18"/>
+      <c r="AG72" s="18"/>
+      <c r="AH72" s="18"/>
+      <c r="AI72" s="18"/>
+      <c r="AJ72" s="18"/>
+      <c r="AK72" s="18"/>
+      <c r="AL72" s="18"/>
+      <c r="AM72" s="18"/>
+      <c r="AN72" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="AO72" s="16"/>
-      <c r="AP72" s="16"/>
-      <c r="AQ72" s="16"/>
-      <c r="AR72" s="16"/>
-      <c r="AS72" s="16"/>
-      <c r="AT72" s="16"/>
-      <c r="AU72" s="16"/>
-      <c r="AV72" s="16"/>
-      <c r="AW72" s="16"/>
-      <c r="AX72" s="16"/>
-      <c r="AY72" s="16"/>
-      <c r="AZ72" s="16"/>
-      <c r="BA72" s="16"/>
-      <c r="BB72" s="16"/>
-      <c r="BC72" s="16"/>
-      <c r="BD72" s="16"/>
-      <c r="BE72" s="16"/>
-      <c r="BF72" s="16"/>
-      <c r="BG72" s="16"/>
-      <c r="BH72" s="16"/>
-      <c r="BI72" s="16"/>
-      <c r="BJ72" s="13" t="s">
+      <c r="AO72" s="17"/>
+      <c r="AP72" s="17"/>
+      <c r="AQ72" s="17"/>
+      <c r="AR72" s="17"/>
+      <c r="AS72" s="17"/>
+      <c r="AT72" s="17"/>
+      <c r="AU72" s="17"/>
+      <c r="AV72" s="17"/>
+      <c r="AW72" s="17"/>
+      <c r="AX72" s="17"/>
+      <c r="AY72" s="17"/>
+      <c r="AZ72" s="17"/>
+      <c r="BA72" s="17"/>
+      <c r="BB72" s="17"/>
+      <c r="BC72" s="17"/>
+      <c r="BD72" s="17"/>
+      <c r="BE72" s="17"/>
+      <c r="BF72" s="17"/>
+      <c r="BG72" s="17"/>
+      <c r="BH72" s="17"/>
+      <c r="BI72" s="17"/>
+      <c r="BJ72" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="BK72" s="13"/>
-      <c r="BL72" s="13"/>
-      <c r="BM72" s="13"/>
-      <c r="BN72" s="13"/>
-      <c r="BO72" s="13"/>
-      <c r="BP72" s="13"/>
-      <c r="BQ72" s="13"/>
-      <c r="BR72" s="13"/>
-      <c r="BS72" s="13"/>
-      <c r="BT72" s="13"/>
-      <c r="BU72" s="13"/>
-      <c r="BV72" s="13"/>
-      <c r="BW72" s="13"/>
-      <c r="BX72" s="13"/>
-      <c r="BY72" s="13"/>
-      <c r="BZ72" s="13"/>
-      <c r="CA72" s="13"/>
-      <c r="CB72" s="13"/>
-      <c r="CC72" s="13"/>
-      <c r="CD72" s="13"/>
-      <c r="CE72" s="13"/>
-      <c r="CF72" s="13"/>
-      <c r="CG72" s="13"/>
-      <c r="CH72" s="13"/>
-      <c r="CI72" s="13"/>
-      <c r="CJ72" s="13"/>
-      <c r="CK72" s="13"/>
-      <c r="CL72" s="13"/>
-      <c r="CM72" s="13"/>
-      <c r="CN72" s="13"/>
-      <c r="CO72" s="13"/>
-      <c r="CP72" s="13"/>
-      <c r="CQ72" s="13"/>
-      <c r="CR72" s="13"/>
-      <c r="CS72" s="13"/>
-      <c r="CT72" s="14"/>
+      <c r="BK72" s="18"/>
+      <c r="BL72" s="18"/>
+      <c r="BM72" s="18"/>
+      <c r="BN72" s="18"/>
+      <c r="BO72" s="18"/>
+      <c r="BP72" s="18"/>
+      <c r="BQ72" s="18"/>
+      <c r="BR72" s="18"/>
+      <c r="BS72" s="18"/>
+      <c r="BT72" s="18"/>
+      <c r="BU72" s="18"/>
+      <c r="BV72" s="18"/>
+      <c r="BW72" s="18"/>
+      <c r="BX72" s="18"/>
+      <c r="BY72" s="18"/>
+      <c r="BZ72" s="18"/>
+      <c r="CA72" s="18"/>
+      <c r="CB72" s="18"/>
+      <c r="CC72" s="18"/>
+      <c r="CD72" s="18"/>
+      <c r="CE72" s="18"/>
+      <c r="CF72" s="18"/>
+      <c r="CG72" s="18"/>
+      <c r="CH72" s="18"/>
+      <c r="CI72" s="18"/>
+      <c r="CJ72" s="18"/>
+      <c r="CK72" s="18"/>
+      <c r="CL72" s="18"/>
+      <c r="CM72" s="18"/>
+      <c r="CN72" s="18"/>
+      <c r="CO72" s="18"/>
+      <c r="CP72" s="18"/>
+      <c r="CQ72" s="18"/>
+      <c r="CR72" s="18"/>
+      <c r="CS72" s="18"/>
+      <c r="CT72" s="19"/>
     </row>
     <row r="73" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C73" s="15">
+      <c r="C73" s="16">
         <v>5</v>
       </c>
-      <c r="D73" s="16"/>
-      <c r="E73" s="16"/>
-      <c r="F73" s="16"/>
-      <c r="G73" s="13" t="s">
+      <c r="D73" s="17"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H73" s="13"/>
-      <c r="I73" s="13"/>
-      <c r="J73" s="13"/>
-      <c r="K73" s="13"/>
-      <c r="L73" s="13"/>
-      <c r="M73" s="13"/>
-      <c r="N73" s="13"/>
-      <c r="O73" s="13"/>
-      <c r="P73" s="13"/>
-      <c r="Q73" s="13"/>
-      <c r="R73" s="13"/>
-      <c r="S73" s="13"/>
-      <c r="T73" s="13"/>
-      <c r="U73" s="13"/>
-      <c r="V73" s="13"/>
-      <c r="W73" s="13"/>
-      <c r="X73" s="13"/>
-      <c r="Y73" s="13" t="s">
+      <c r="H73" s="18"/>
+      <c r="I73" s="18"/>
+      <c r="J73" s="18"/>
+      <c r="K73" s="18"/>
+      <c r="L73" s="18"/>
+      <c r="M73" s="18"/>
+      <c r="N73" s="18"/>
+      <c r="O73" s="18"/>
+      <c r="P73" s="18"/>
+      <c r="Q73" s="18"/>
+      <c r="R73" s="18"/>
+      <c r="S73" s="18"/>
+      <c r="T73" s="18"/>
+      <c r="U73" s="18"/>
+      <c r="V73" s="18"/>
+      <c r="W73" s="18"/>
+      <c r="X73" s="18"/>
+      <c r="Y73" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="Z73" s="13"/>
-      <c r="AA73" s="13"/>
-      <c r="AB73" s="13"/>
-      <c r="AC73" s="13"/>
-      <c r="AD73" s="13"/>
-      <c r="AE73" s="13"/>
-      <c r="AF73" s="13"/>
-      <c r="AG73" s="13"/>
-      <c r="AH73" s="13"/>
-      <c r="AI73" s="13"/>
-      <c r="AJ73" s="13"/>
-      <c r="AK73" s="13"/>
-      <c r="AL73" s="13"/>
-      <c r="AM73" s="13"/>
-      <c r="AN73" s="16" t="s">
+      <c r="Z73" s="18"/>
+      <c r="AA73" s="18"/>
+      <c r="AB73" s="18"/>
+      <c r="AC73" s="18"/>
+      <c r="AD73" s="18"/>
+      <c r="AE73" s="18"/>
+      <c r="AF73" s="18"/>
+      <c r="AG73" s="18"/>
+      <c r="AH73" s="18"/>
+      <c r="AI73" s="18"/>
+      <c r="AJ73" s="18"/>
+      <c r="AK73" s="18"/>
+      <c r="AL73" s="18"/>
+      <c r="AM73" s="18"/>
+      <c r="AN73" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="AO73" s="16"/>
-      <c r="AP73" s="16"/>
-      <c r="AQ73" s="16"/>
-      <c r="AR73" s="16"/>
-      <c r="AS73" s="16"/>
-      <c r="AT73" s="16"/>
-      <c r="AU73" s="16"/>
-      <c r="AV73" s="16"/>
-      <c r="AW73" s="16"/>
-      <c r="AX73" s="16"/>
-      <c r="AY73" s="16"/>
-      <c r="AZ73" s="16"/>
-      <c r="BA73" s="16"/>
-      <c r="BB73" s="16"/>
-      <c r="BC73" s="16"/>
-      <c r="BD73" s="16"/>
-      <c r="BE73" s="16"/>
-      <c r="BF73" s="16"/>
-      <c r="BG73" s="16"/>
-      <c r="BH73" s="16"/>
-      <c r="BI73" s="16"/>
-      <c r="BJ73" s="13" t="s">
+      <c r="AO73" s="17"/>
+      <c r="AP73" s="17"/>
+      <c r="AQ73" s="17"/>
+      <c r="AR73" s="17"/>
+      <c r="AS73" s="17"/>
+      <c r="AT73" s="17"/>
+      <c r="AU73" s="17"/>
+      <c r="AV73" s="17"/>
+      <c r="AW73" s="17"/>
+      <c r="AX73" s="17"/>
+      <c r="AY73" s="17"/>
+      <c r="AZ73" s="17"/>
+      <c r="BA73" s="17"/>
+      <c r="BB73" s="17"/>
+      <c r="BC73" s="17"/>
+      <c r="BD73" s="17"/>
+      <c r="BE73" s="17"/>
+      <c r="BF73" s="17"/>
+      <c r="BG73" s="17"/>
+      <c r="BH73" s="17"/>
+      <c r="BI73" s="17"/>
+      <c r="BJ73" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="BK73" s="13"/>
-      <c r="BL73" s="13"/>
-      <c r="BM73" s="13"/>
-      <c r="BN73" s="13"/>
-      <c r="BO73" s="13"/>
-      <c r="BP73" s="13"/>
-      <c r="BQ73" s="13"/>
-      <c r="BR73" s="13"/>
-      <c r="BS73" s="13"/>
-      <c r="BT73" s="13"/>
-      <c r="BU73" s="13"/>
-      <c r="BV73" s="13"/>
-      <c r="BW73" s="13"/>
-      <c r="BX73" s="13"/>
-      <c r="BY73" s="13"/>
-      <c r="BZ73" s="13"/>
-      <c r="CA73" s="13"/>
-      <c r="CB73" s="13"/>
-      <c r="CC73" s="13"/>
-      <c r="CD73" s="13"/>
-      <c r="CE73" s="13"/>
-      <c r="CF73" s="13"/>
-      <c r="CG73" s="13"/>
-      <c r="CH73" s="13"/>
-      <c r="CI73" s="13"/>
-      <c r="CJ73" s="13"/>
-      <c r="CK73" s="13"/>
-      <c r="CL73" s="13"/>
-      <c r="CM73" s="13"/>
-      <c r="CN73" s="13"/>
-      <c r="CO73" s="13"/>
-      <c r="CP73" s="13"/>
-      <c r="CQ73" s="13"/>
-      <c r="CR73" s="13"/>
-      <c r="CS73" s="13"/>
-      <c r="CT73" s="14"/>
+      <c r="BK73" s="18"/>
+      <c r="BL73" s="18"/>
+      <c r="BM73" s="18"/>
+      <c r="BN73" s="18"/>
+      <c r="BO73" s="18"/>
+      <c r="BP73" s="18"/>
+      <c r="BQ73" s="18"/>
+      <c r="BR73" s="18"/>
+      <c r="BS73" s="18"/>
+      <c r="BT73" s="18"/>
+      <c r="BU73" s="18"/>
+      <c r="BV73" s="18"/>
+      <c r="BW73" s="18"/>
+      <c r="BX73" s="18"/>
+      <c r="BY73" s="18"/>
+      <c r="BZ73" s="18"/>
+      <c r="CA73" s="18"/>
+      <c r="CB73" s="18"/>
+      <c r="CC73" s="18"/>
+      <c r="CD73" s="18"/>
+      <c r="CE73" s="18"/>
+      <c r="CF73" s="18"/>
+      <c r="CG73" s="18"/>
+      <c r="CH73" s="18"/>
+      <c r="CI73" s="18"/>
+      <c r="CJ73" s="18"/>
+      <c r="CK73" s="18"/>
+      <c r="CL73" s="18"/>
+      <c r="CM73" s="18"/>
+      <c r="CN73" s="18"/>
+      <c r="CO73" s="18"/>
+      <c r="CP73" s="18"/>
+      <c r="CQ73" s="18"/>
+      <c r="CR73" s="18"/>
+      <c r="CS73" s="18"/>
+      <c r="CT73" s="19"/>
     </row>
     <row r="74" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C74" s="15">
+      <c r="C74" s="16">
         <v>6</v>
       </c>
-      <c r="D74" s="16"/>
-      <c r="E74" s="16"/>
-      <c r="F74" s="16"/>
-      <c r="G74" s="13" t="s">
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="13"/>
-      <c r="K74" s="13"/>
-      <c r="L74" s="13"/>
-      <c r="M74" s="13"/>
-      <c r="N74" s="13"/>
-      <c r="O74" s="13"/>
-      <c r="P74" s="13"/>
-      <c r="Q74" s="13"/>
-      <c r="R74" s="13"/>
-      <c r="S74" s="13"/>
-      <c r="T74" s="13"/>
-      <c r="U74" s="13"/>
-      <c r="V74" s="13"/>
-      <c r="W74" s="13"/>
-      <c r="X74" s="13"/>
-      <c r="Y74" s="13" t="s">
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
+      <c r="J74" s="18"/>
+      <c r="K74" s="18"/>
+      <c r="L74" s="18"/>
+      <c r="M74" s="18"/>
+      <c r="N74" s="18"/>
+      <c r="O74" s="18"/>
+      <c r="P74" s="18"/>
+      <c r="Q74" s="18"/>
+      <c r="R74" s="18"/>
+      <c r="S74" s="18"/>
+      <c r="T74" s="18"/>
+      <c r="U74" s="18"/>
+      <c r="V74" s="18"/>
+      <c r="W74" s="18"/>
+      <c r="X74" s="18"/>
+      <c r="Y74" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="Z74" s="13"/>
-      <c r="AA74" s="13"/>
-      <c r="AB74" s="13"/>
-      <c r="AC74" s="13"/>
-      <c r="AD74" s="13"/>
-      <c r="AE74" s="13"/>
-      <c r="AF74" s="13"/>
-      <c r="AG74" s="13"/>
-      <c r="AH74" s="13"/>
-      <c r="AI74" s="13"/>
-      <c r="AJ74" s="13"/>
-      <c r="AK74" s="13"/>
-      <c r="AL74" s="13"/>
-      <c r="AM74" s="13"/>
-      <c r="AN74" s="16" t="s">
+      <c r="Z74" s="18"/>
+      <c r="AA74" s="18"/>
+      <c r="AB74" s="18"/>
+      <c r="AC74" s="18"/>
+      <c r="AD74" s="18"/>
+      <c r="AE74" s="18"/>
+      <c r="AF74" s="18"/>
+      <c r="AG74" s="18"/>
+      <c r="AH74" s="18"/>
+      <c r="AI74" s="18"/>
+      <c r="AJ74" s="18"/>
+      <c r="AK74" s="18"/>
+      <c r="AL74" s="18"/>
+      <c r="AM74" s="18"/>
+      <c r="AN74" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="AO74" s="16"/>
-      <c r="AP74" s="16"/>
-      <c r="AQ74" s="16"/>
-      <c r="AR74" s="16"/>
-      <c r="AS74" s="16"/>
-      <c r="AT74" s="16"/>
-      <c r="AU74" s="16"/>
-      <c r="AV74" s="16"/>
-      <c r="AW74" s="16"/>
-      <c r="AX74" s="16"/>
-      <c r="AY74" s="16"/>
-      <c r="AZ74" s="16"/>
-      <c r="BA74" s="16"/>
-      <c r="BB74" s="16"/>
-      <c r="BC74" s="16"/>
-      <c r="BD74" s="16"/>
-      <c r="BE74" s="16"/>
-      <c r="BF74" s="16"/>
-      <c r="BG74" s="16"/>
-      <c r="BH74" s="16"/>
-      <c r="BI74" s="16"/>
-      <c r="BJ74" s="13" t="s">
+      <c r="AO74" s="17"/>
+      <c r="AP74" s="17"/>
+      <c r="AQ74" s="17"/>
+      <c r="AR74" s="17"/>
+      <c r="AS74" s="17"/>
+      <c r="AT74" s="17"/>
+      <c r="AU74" s="17"/>
+      <c r="AV74" s="17"/>
+      <c r="AW74" s="17"/>
+      <c r="AX74" s="17"/>
+      <c r="AY74" s="17"/>
+      <c r="AZ74" s="17"/>
+      <c r="BA74" s="17"/>
+      <c r="BB74" s="17"/>
+      <c r="BC74" s="17"/>
+      <c r="BD74" s="17"/>
+      <c r="BE74" s="17"/>
+      <c r="BF74" s="17"/>
+      <c r="BG74" s="17"/>
+      <c r="BH74" s="17"/>
+      <c r="BI74" s="17"/>
+      <c r="BJ74" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="BK74" s="13"/>
-      <c r="BL74" s="13"/>
-      <c r="BM74" s="13"/>
-      <c r="BN74" s="13"/>
-      <c r="BO74" s="13"/>
-      <c r="BP74" s="13"/>
-      <c r="BQ74" s="13"/>
-      <c r="BR74" s="13"/>
-      <c r="BS74" s="13"/>
-      <c r="BT74" s="13"/>
-      <c r="BU74" s="13"/>
-      <c r="BV74" s="13"/>
-      <c r="BW74" s="13"/>
-      <c r="BX74" s="13"/>
-      <c r="BY74" s="13"/>
-      <c r="BZ74" s="13"/>
-      <c r="CA74" s="13"/>
-      <c r="CB74" s="13"/>
-      <c r="CC74" s="13"/>
-      <c r="CD74" s="13"/>
-      <c r="CE74" s="13"/>
-      <c r="CF74" s="13"/>
-      <c r="CG74" s="13"/>
-      <c r="CH74" s="13"/>
-      <c r="CI74" s="13"/>
-      <c r="CJ74" s="13"/>
-      <c r="CK74" s="13"/>
-      <c r="CL74" s="13"/>
-      <c r="CM74" s="13"/>
-      <c r="CN74" s="13"/>
-      <c r="CO74" s="13"/>
-      <c r="CP74" s="13"/>
-      <c r="CQ74" s="13"/>
-      <c r="CR74" s="13"/>
-      <c r="CS74" s="13"/>
-      <c r="CT74" s="14"/>
+      <c r="BK74" s="18"/>
+      <c r="BL74" s="18"/>
+      <c r="BM74" s="18"/>
+      <c r="BN74" s="18"/>
+      <c r="BO74" s="18"/>
+      <c r="BP74" s="18"/>
+      <c r="BQ74" s="18"/>
+      <c r="BR74" s="18"/>
+      <c r="BS74" s="18"/>
+      <c r="BT74" s="18"/>
+      <c r="BU74" s="18"/>
+      <c r="BV74" s="18"/>
+      <c r="BW74" s="18"/>
+      <c r="BX74" s="18"/>
+      <c r="BY74" s="18"/>
+      <c r="BZ74" s="18"/>
+      <c r="CA74" s="18"/>
+      <c r="CB74" s="18"/>
+      <c r="CC74" s="18"/>
+      <c r="CD74" s="18"/>
+      <c r="CE74" s="18"/>
+      <c r="CF74" s="18"/>
+      <c r="CG74" s="18"/>
+      <c r="CH74" s="18"/>
+      <c r="CI74" s="18"/>
+      <c r="CJ74" s="18"/>
+      <c r="CK74" s="18"/>
+      <c r="CL74" s="18"/>
+      <c r="CM74" s="18"/>
+      <c r="CN74" s="18"/>
+      <c r="CO74" s="18"/>
+      <c r="CP74" s="18"/>
+      <c r="CQ74" s="18"/>
+      <c r="CR74" s="18"/>
+      <c r="CS74" s="18"/>
+      <c r="CT74" s="19"/>
     </row>
     <row r="75" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C75" s="15">
+      <c r="C75" s="16">
         <v>7</v>
       </c>
-      <c r="D75" s="16"/>
-      <c r="E75" s="16"/>
-      <c r="F75" s="16"/>
-      <c r="G75" s="13" t="s">
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="13"/>
-      <c r="K75" s="13"/>
-      <c r="L75" s="13"/>
-      <c r="M75" s="13"/>
-      <c r="N75" s="13"/>
-      <c r="O75" s="13"/>
-      <c r="P75" s="13"/>
-      <c r="Q75" s="13"/>
-      <c r="R75" s="13"/>
-      <c r="S75" s="13"/>
-      <c r="T75" s="13"/>
-      <c r="U75" s="13"/>
-      <c r="V75" s="13"/>
-      <c r="W75" s="13"/>
-      <c r="X75" s="13"/>
-      <c r="Y75" s="13" t="s">
+      <c r="H75" s="18"/>
+      <c r="I75" s="18"/>
+      <c r="J75" s="18"/>
+      <c r="K75" s="18"/>
+      <c r="L75" s="18"/>
+      <c r="M75" s="18"/>
+      <c r="N75" s="18"/>
+      <c r="O75" s="18"/>
+      <c r="P75" s="18"/>
+      <c r="Q75" s="18"/>
+      <c r="R75" s="18"/>
+      <c r="S75" s="18"/>
+      <c r="T75" s="18"/>
+      <c r="U75" s="18"/>
+      <c r="V75" s="18"/>
+      <c r="W75" s="18"/>
+      <c r="X75" s="18"/>
+      <c r="Y75" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="Z75" s="13"/>
-      <c r="AA75" s="13"/>
-      <c r="AB75" s="13"/>
-      <c r="AC75" s="13"/>
-      <c r="AD75" s="13"/>
-      <c r="AE75" s="13"/>
-      <c r="AF75" s="13"/>
-      <c r="AG75" s="13"/>
-      <c r="AH75" s="13"/>
-      <c r="AI75" s="13"/>
-      <c r="AJ75" s="13"/>
-      <c r="AK75" s="13"/>
-      <c r="AL75" s="13"/>
-      <c r="AM75" s="13"/>
-      <c r="AN75" s="16" t="s">
+      <c r="Z75" s="18"/>
+      <c r="AA75" s="18"/>
+      <c r="AB75" s="18"/>
+      <c r="AC75" s="18"/>
+      <c r="AD75" s="18"/>
+      <c r="AE75" s="18"/>
+      <c r="AF75" s="18"/>
+      <c r="AG75" s="18"/>
+      <c r="AH75" s="18"/>
+      <c r="AI75" s="18"/>
+      <c r="AJ75" s="18"/>
+      <c r="AK75" s="18"/>
+      <c r="AL75" s="18"/>
+      <c r="AM75" s="18"/>
+      <c r="AN75" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="AO75" s="16"/>
-      <c r="AP75" s="16"/>
-      <c r="AQ75" s="16"/>
-      <c r="AR75" s="16"/>
-      <c r="AS75" s="16"/>
-      <c r="AT75" s="16"/>
-      <c r="AU75" s="16"/>
-      <c r="AV75" s="16"/>
-      <c r="AW75" s="16"/>
-      <c r="AX75" s="16"/>
-      <c r="AY75" s="16"/>
-      <c r="AZ75" s="16"/>
-      <c r="BA75" s="16"/>
-      <c r="BB75" s="16"/>
-      <c r="BC75" s="16"/>
-      <c r="BD75" s="16"/>
-      <c r="BE75" s="16"/>
-      <c r="BF75" s="16"/>
-      <c r="BG75" s="16"/>
-      <c r="BH75" s="16"/>
-      <c r="BI75" s="16"/>
-      <c r="BJ75" s="13"/>
-      <c r="BK75" s="13"/>
-      <c r="BL75" s="13"/>
-      <c r="BM75" s="13"/>
-      <c r="BN75" s="13"/>
-      <c r="BO75" s="13"/>
-      <c r="BP75" s="13"/>
-      <c r="BQ75" s="13"/>
-      <c r="BR75" s="13"/>
-      <c r="BS75" s="13"/>
-      <c r="BT75" s="13"/>
-      <c r="BU75" s="13"/>
-      <c r="BV75" s="13"/>
-      <c r="BW75" s="13"/>
-      <c r="BX75" s="13"/>
-      <c r="BY75" s="13"/>
-      <c r="BZ75" s="13"/>
-      <c r="CA75" s="13"/>
-      <c r="CB75" s="13"/>
-      <c r="CC75" s="13"/>
-      <c r="CD75" s="13"/>
-      <c r="CE75" s="13"/>
-      <c r="CF75" s="13"/>
-      <c r="CG75" s="13"/>
-      <c r="CH75" s="13"/>
-      <c r="CI75" s="13"/>
-      <c r="CJ75" s="13"/>
-      <c r="CK75" s="13"/>
-      <c r="CL75" s="13"/>
-      <c r="CM75" s="13"/>
-      <c r="CN75" s="13"/>
-      <c r="CO75" s="13"/>
-      <c r="CP75" s="13"/>
-      <c r="CQ75" s="13"/>
-      <c r="CR75" s="13"/>
-      <c r="CS75" s="13"/>
-      <c r="CT75" s="14"/>
+      <c r="AO75" s="17"/>
+      <c r="AP75" s="17"/>
+      <c r="AQ75" s="17"/>
+      <c r="AR75" s="17"/>
+      <c r="AS75" s="17"/>
+      <c r="AT75" s="17"/>
+      <c r="AU75" s="17"/>
+      <c r="AV75" s="17"/>
+      <c r="AW75" s="17"/>
+      <c r="AX75" s="17"/>
+      <c r="AY75" s="17"/>
+      <c r="AZ75" s="17"/>
+      <c r="BA75" s="17"/>
+      <c r="BB75" s="17"/>
+      <c r="BC75" s="17"/>
+      <c r="BD75" s="17"/>
+      <c r="BE75" s="17"/>
+      <c r="BF75" s="17"/>
+      <c r="BG75" s="17"/>
+      <c r="BH75" s="17"/>
+      <c r="BI75" s="17"/>
+      <c r="BJ75" s="18"/>
+      <c r="BK75" s="18"/>
+      <c r="BL75" s="18"/>
+      <c r="BM75" s="18"/>
+      <c r="BN75" s="18"/>
+      <c r="BO75" s="18"/>
+      <c r="BP75" s="18"/>
+      <c r="BQ75" s="18"/>
+      <c r="BR75" s="18"/>
+      <c r="BS75" s="18"/>
+      <c r="BT75" s="18"/>
+      <c r="BU75" s="18"/>
+      <c r="BV75" s="18"/>
+      <c r="BW75" s="18"/>
+      <c r="BX75" s="18"/>
+      <c r="BY75" s="18"/>
+      <c r="BZ75" s="18"/>
+      <c r="CA75" s="18"/>
+      <c r="CB75" s="18"/>
+      <c r="CC75" s="18"/>
+      <c r="CD75" s="18"/>
+      <c r="CE75" s="18"/>
+      <c r="CF75" s="18"/>
+      <c r="CG75" s="18"/>
+      <c r="CH75" s="18"/>
+      <c r="CI75" s="18"/>
+      <c r="CJ75" s="18"/>
+      <c r="CK75" s="18"/>
+      <c r="CL75" s="18"/>
+      <c r="CM75" s="18"/>
+      <c r="CN75" s="18"/>
+      <c r="CO75" s="18"/>
+      <c r="CP75" s="18"/>
+      <c r="CQ75" s="18"/>
+      <c r="CR75" s="18"/>
+      <c r="CS75" s="18"/>
+      <c r="CT75" s="19"/>
     </row>
     <row r="76" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C76" s="15">
+      <c r="C76" s="16">
         <v>8</v>
       </c>
-      <c r="D76" s="16"/>
-      <c r="E76" s="16"/>
-      <c r="F76" s="16"/>
-      <c r="G76" s="13" t="s">
+      <c r="D76" s="17"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H76" s="13"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="13"/>
-      <c r="K76" s="13"/>
-      <c r="L76" s="13"/>
-      <c r="M76" s="13"/>
-      <c r="N76" s="13"/>
-      <c r="O76" s="13"/>
-      <c r="P76" s="13"/>
-      <c r="Q76" s="13"/>
-      <c r="R76" s="13"/>
-      <c r="S76" s="13"/>
-      <c r="T76" s="13"/>
-      <c r="U76" s="13"/>
-      <c r="V76" s="13"/>
-      <c r="W76" s="13"/>
-      <c r="X76" s="13"/>
-      <c r="Y76" s="13" t="s">
+      <c r="H76" s="18"/>
+      <c r="I76" s="18"/>
+      <c r="J76" s="18"/>
+      <c r="K76" s="18"/>
+      <c r="L76" s="18"/>
+      <c r="M76" s="18"/>
+      <c r="N76" s="18"/>
+      <c r="O76" s="18"/>
+      <c r="P76" s="18"/>
+      <c r="Q76" s="18"/>
+      <c r="R76" s="18"/>
+      <c r="S76" s="18"/>
+      <c r="T76" s="18"/>
+      <c r="U76" s="18"/>
+      <c r="V76" s="18"/>
+      <c r="W76" s="18"/>
+      <c r="X76" s="18"/>
+      <c r="Y76" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="Z76" s="13"/>
-      <c r="AA76" s="13"/>
-      <c r="AB76" s="13"/>
-      <c r="AC76" s="13"/>
-      <c r="AD76" s="13"/>
-      <c r="AE76" s="13"/>
-      <c r="AF76" s="13"/>
-      <c r="AG76" s="13"/>
-      <c r="AH76" s="13"/>
-      <c r="AI76" s="13"/>
-      <c r="AJ76" s="13"/>
-      <c r="AK76" s="13"/>
-      <c r="AL76" s="13"/>
-      <c r="AM76" s="13"/>
-      <c r="AN76" s="16" t="s">
+      <c r="Z76" s="18"/>
+      <c r="AA76" s="18"/>
+      <c r="AB76" s="18"/>
+      <c r="AC76" s="18"/>
+      <c r="AD76" s="18"/>
+      <c r="AE76" s="18"/>
+      <c r="AF76" s="18"/>
+      <c r="AG76" s="18"/>
+      <c r="AH76" s="18"/>
+      <c r="AI76" s="18"/>
+      <c r="AJ76" s="18"/>
+      <c r="AK76" s="18"/>
+      <c r="AL76" s="18"/>
+      <c r="AM76" s="18"/>
+      <c r="AN76" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="AO76" s="16"/>
-      <c r="AP76" s="16"/>
-      <c r="AQ76" s="16"/>
-      <c r="AR76" s="16"/>
-      <c r="AS76" s="16"/>
-      <c r="AT76" s="16"/>
-      <c r="AU76" s="16"/>
-      <c r="AV76" s="16"/>
-      <c r="AW76" s="16"/>
-      <c r="AX76" s="16"/>
-      <c r="AY76" s="16"/>
-      <c r="AZ76" s="16"/>
-      <c r="BA76" s="16"/>
-      <c r="BB76" s="16"/>
-      <c r="BC76" s="16"/>
-      <c r="BD76" s="16"/>
-      <c r="BE76" s="16"/>
-      <c r="BF76" s="16"/>
-      <c r="BG76" s="16"/>
-      <c r="BH76" s="16"/>
-      <c r="BI76" s="16"/>
-      <c r="BJ76" s="13"/>
-      <c r="BK76" s="13"/>
-      <c r="BL76" s="13"/>
-      <c r="BM76" s="13"/>
-      <c r="BN76" s="13"/>
-      <c r="BO76" s="13"/>
-      <c r="BP76" s="13"/>
-      <c r="BQ76" s="13"/>
-      <c r="BR76" s="13"/>
-      <c r="BS76" s="13"/>
-      <c r="BT76" s="13"/>
-      <c r="BU76" s="13"/>
-      <c r="BV76" s="13"/>
-      <c r="BW76" s="13"/>
-      <c r="BX76" s="13"/>
-      <c r="BY76" s="13"/>
-      <c r="BZ76" s="13"/>
-      <c r="CA76" s="13"/>
-      <c r="CB76" s="13"/>
-      <c r="CC76" s="13"/>
-      <c r="CD76" s="13"/>
-      <c r="CE76" s="13"/>
-      <c r="CF76" s="13"/>
-      <c r="CG76" s="13"/>
-      <c r="CH76" s="13"/>
-      <c r="CI76" s="13"/>
-      <c r="CJ76" s="13"/>
-      <c r="CK76" s="13"/>
-      <c r="CL76" s="13"/>
-      <c r="CM76" s="13"/>
-      <c r="CN76" s="13"/>
-      <c r="CO76" s="13"/>
-      <c r="CP76" s="13"/>
-      <c r="CQ76" s="13"/>
-      <c r="CR76" s="13"/>
-      <c r="CS76" s="13"/>
-      <c r="CT76" s="14"/>
+      <c r="AO76" s="17"/>
+      <c r="AP76" s="17"/>
+      <c r="AQ76" s="17"/>
+      <c r="AR76" s="17"/>
+      <c r="AS76" s="17"/>
+      <c r="AT76" s="17"/>
+      <c r="AU76" s="17"/>
+      <c r="AV76" s="17"/>
+      <c r="AW76" s="17"/>
+      <c r="AX76" s="17"/>
+      <c r="AY76" s="17"/>
+      <c r="AZ76" s="17"/>
+      <c r="BA76" s="17"/>
+      <c r="BB76" s="17"/>
+      <c r="BC76" s="17"/>
+      <c r="BD76" s="17"/>
+      <c r="BE76" s="17"/>
+      <c r="BF76" s="17"/>
+      <c r="BG76" s="17"/>
+      <c r="BH76" s="17"/>
+      <c r="BI76" s="17"/>
+      <c r="BJ76" s="18"/>
+      <c r="BK76" s="18"/>
+      <c r="BL76" s="18"/>
+      <c r="BM76" s="18"/>
+      <c r="BN76" s="18"/>
+      <c r="BO76" s="18"/>
+      <c r="BP76" s="18"/>
+      <c r="BQ76" s="18"/>
+      <c r="BR76" s="18"/>
+      <c r="BS76" s="18"/>
+      <c r="BT76" s="18"/>
+      <c r="BU76" s="18"/>
+      <c r="BV76" s="18"/>
+      <c r="BW76" s="18"/>
+      <c r="BX76" s="18"/>
+      <c r="BY76" s="18"/>
+      <c r="BZ76" s="18"/>
+      <c r="CA76" s="18"/>
+      <c r="CB76" s="18"/>
+      <c r="CC76" s="18"/>
+      <c r="CD76" s="18"/>
+      <c r="CE76" s="18"/>
+      <c r="CF76" s="18"/>
+      <c r="CG76" s="18"/>
+      <c r="CH76" s="18"/>
+      <c r="CI76" s="18"/>
+      <c r="CJ76" s="18"/>
+      <c r="CK76" s="18"/>
+      <c r="CL76" s="18"/>
+      <c r="CM76" s="18"/>
+      <c r="CN76" s="18"/>
+      <c r="CO76" s="18"/>
+      <c r="CP76" s="18"/>
+      <c r="CQ76" s="18"/>
+      <c r="CR76" s="18"/>
+      <c r="CS76" s="18"/>
+      <c r="CT76" s="19"/>
     </row>
     <row r="77" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C77" s="15">
+      <c r="C77" s="16">
         <v>9</v>
       </c>
-      <c r="D77" s="16"/>
-      <c r="E77" s="16"/>
-      <c r="F77" s="16"/>
-      <c r="G77" s="27"/>
-      <c r="H77" s="13"/>
-      <c r="I77" s="13"/>
-      <c r="J77" s="13"/>
-      <c r="K77" s="13"/>
-      <c r="L77" s="13"/>
-      <c r="M77" s="13"/>
-      <c r="N77" s="13"/>
-      <c r="O77" s="13"/>
-      <c r="P77" s="13"/>
-      <c r="Q77" s="13"/>
-      <c r="R77" s="13"/>
-      <c r="S77" s="13"/>
-      <c r="T77" s="13"/>
-      <c r="U77" s="13"/>
-      <c r="V77" s="13"/>
-      <c r="W77" s="13"/>
-      <c r="X77" s="13"/>
-      <c r="Y77" s="13"/>
-      <c r="Z77" s="13"/>
-      <c r="AA77" s="13"/>
-      <c r="AB77" s="13"/>
-      <c r="AC77" s="13"/>
-      <c r="AD77" s="13"/>
-      <c r="AE77" s="13"/>
-      <c r="AF77" s="13"/>
-      <c r="AG77" s="13"/>
-      <c r="AH77" s="13"/>
-      <c r="AI77" s="13"/>
-      <c r="AJ77" s="13"/>
-      <c r="AK77" s="13"/>
-      <c r="AL77" s="13"/>
-      <c r="AM77" s="13"/>
-      <c r="AN77" s="16"/>
-      <c r="AO77" s="16"/>
-      <c r="AP77" s="16"/>
-      <c r="AQ77" s="16"/>
-      <c r="AR77" s="16"/>
-      <c r="AS77" s="16"/>
-      <c r="AT77" s="16"/>
-      <c r="AU77" s="16"/>
-      <c r="AV77" s="16"/>
-      <c r="AW77" s="16"/>
-      <c r="AX77" s="16"/>
-      <c r="AY77" s="16"/>
-      <c r="AZ77" s="16"/>
-      <c r="BA77" s="16"/>
-      <c r="BB77" s="16"/>
-      <c r="BC77" s="16"/>
-      <c r="BD77" s="16"/>
-      <c r="BE77" s="16"/>
-      <c r="BF77" s="16"/>
-      <c r="BG77" s="16"/>
-      <c r="BH77" s="16"/>
-      <c r="BI77" s="16"/>
-      <c r="BJ77" s="13"/>
-      <c r="BK77" s="13"/>
-      <c r="BL77" s="13"/>
-      <c r="BM77" s="13"/>
-      <c r="BN77" s="13"/>
-      <c r="BO77" s="13"/>
-      <c r="BP77" s="13"/>
-      <c r="BQ77" s="13"/>
-      <c r="BR77" s="13"/>
-      <c r="BS77" s="13"/>
-      <c r="BT77" s="13"/>
-      <c r="BU77" s="13"/>
-      <c r="BV77" s="13"/>
-      <c r="BW77" s="13"/>
-      <c r="BX77" s="13"/>
-      <c r="BY77" s="13"/>
-      <c r="BZ77" s="13"/>
-      <c r="CA77" s="13"/>
-      <c r="CB77" s="13"/>
-      <c r="CC77" s="13"/>
-      <c r="CD77" s="13"/>
-      <c r="CE77" s="13"/>
-      <c r="CF77" s="13"/>
-      <c r="CG77" s="13"/>
-      <c r="CH77" s="13"/>
-      <c r="CI77" s="13"/>
-      <c r="CJ77" s="13"/>
-      <c r="CK77" s="13"/>
-      <c r="CL77" s="13"/>
-      <c r="CM77" s="13"/>
-      <c r="CN77" s="13"/>
-      <c r="CO77" s="13"/>
-      <c r="CP77" s="13"/>
-      <c r="CQ77" s="13"/>
-      <c r="CR77" s="13"/>
-      <c r="CS77" s="13"/>
-      <c r="CT77" s="14"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="22"/>
+      <c r="H77" s="18"/>
+      <c r="I77" s="18"/>
+      <c r="J77" s="18"/>
+      <c r="K77" s="18"/>
+      <c r="L77" s="18"/>
+      <c r="M77" s="18"/>
+      <c r="N77" s="18"/>
+      <c r="O77" s="18"/>
+      <c r="P77" s="18"/>
+      <c r="Q77" s="18"/>
+      <c r="R77" s="18"/>
+      <c r="S77" s="18"/>
+      <c r="T77" s="18"/>
+      <c r="U77" s="18"/>
+      <c r="V77" s="18"/>
+      <c r="W77" s="18"/>
+      <c r="X77" s="18"/>
+      <c r="Y77" s="18"/>
+      <c r="Z77" s="18"/>
+      <c r="AA77" s="18"/>
+      <c r="AB77" s="18"/>
+      <c r="AC77" s="18"/>
+      <c r="AD77" s="18"/>
+      <c r="AE77" s="18"/>
+      <c r="AF77" s="18"/>
+      <c r="AG77" s="18"/>
+      <c r="AH77" s="18"/>
+      <c r="AI77" s="18"/>
+      <c r="AJ77" s="18"/>
+      <c r="AK77" s="18"/>
+      <c r="AL77" s="18"/>
+      <c r="AM77" s="18"/>
+      <c r="AN77" s="17"/>
+      <c r="AO77" s="17"/>
+      <c r="AP77" s="17"/>
+      <c r="AQ77" s="17"/>
+      <c r="AR77" s="17"/>
+      <c r="AS77" s="17"/>
+      <c r="AT77" s="17"/>
+      <c r="AU77" s="17"/>
+      <c r="AV77" s="17"/>
+      <c r="AW77" s="17"/>
+      <c r="AX77" s="17"/>
+      <c r="AY77" s="17"/>
+      <c r="AZ77" s="17"/>
+      <c r="BA77" s="17"/>
+      <c r="BB77" s="17"/>
+      <c r="BC77" s="17"/>
+      <c r="BD77" s="17"/>
+      <c r="BE77" s="17"/>
+      <c r="BF77" s="17"/>
+      <c r="BG77" s="17"/>
+      <c r="BH77" s="17"/>
+      <c r="BI77" s="17"/>
+      <c r="BJ77" s="18"/>
+      <c r="BK77" s="18"/>
+      <c r="BL77" s="18"/>
+      <c r="BM77" s="18"/>
+      <c r="BN77" s="18"/>
+      <c r="BO77" s="18"/>
+      <c r="BP77" s="18"/>
+      <c r="BQ77" s="18"/>
+      <c r="BR77" s="18"/>
+      <c r="BS77" s="18"/>
+      <c r="BT77" s="18"/>
+      <c r="BU77" s="18"/>
+      <c r="BV77" s="18"/>
+      <c r="BW77" s="18"/>
+      <c r="BX77" s="18"/>
+      <c r="BY77" s="18"/>
+      <c r="BZ77" s="18"/>
+      <c r="CA77" s="18"/>
+      <c r="CB77" s="18"/>
+      <c r="CC77" s="18"/>
+      <c r="CD77" s="18"/>
+      <c r="CE77" s="18"/>
+      <c r="CF77" s="18"/>
+      <c r="CG77" s="18"/>
+      <c r="CH77" s="18"/>
+      <c r="CI77" s="18"/>
+      <c r="CJ77" s="18"/>
+      <c r="CK77" s="18"/>
+      <c r="CL77" s="18"/>
+      <c r="CM77" s="18"/>
+      <c r="CN77" s="18"/>
+      <c r="CO77" s="18"/>
+      <c r="CP77" s="18"/>
+      <c r="CQ77" s="18"/>
+      <c r="CR77" s="18"/>
+      <c r="CS77" s="18"/>
+      <c r="CT77" s="19"/>
     </row>
     <row r="78" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C78" s="15"/>
-      <c r="D78" s="16"/>
-      <c r="E78" s="16"/>
-      <c r="F78" s="16"/>
-      <c r="G78" s="13"/>
-      <c r="H78" s="13"/>
-      <c r="I78" s="13"/>
-      <c r="J78" s="13"/>
-      <c r="K78" s="13"/>
-      <c r="L78" s="13"/>
-      <c r="M78" s="13"/>
-      <c r="N78" s="13"/>
-      <c r="O78" s="13"/>
-      <c r="P78" s="13"/>
-      <c r="Q78" s="13"/>
-      <c r="R78" s="13"/>
-      <c r="S78" s="13"/>
-      <c r="T78" s="13"/>
-      <c r="U78" s="13"/>
-      <c r="V78" s="13"/>
-      <c r="W78" s="13"/>
-      <c r="X78" s="13"/>
-      <c r="Y78" s="13"/>
-      <c r="Z78" s="13"/>
-      <c r="AA78" s="13"/>
-      <c r="AB78" s="13"/>
-      <c r="AC78" s="13"/>
-      <c r="AD78" s="13"/>
-      <c r="AE78" s="13"/>
-      <c r="AF78" s="13"/>
-      <c r="AG78" s="13"/>
-      <c r="AH78" s="13"/>
-      <c r="AI78" s="13"/>
-      <c r="AJ78" s="13"/>
-      <c r="AK78" s="13"/>
-      <c r="AL78" s="13"/>
-      <c r="AM78" s="13"/>
-      <c r="AN78" s="16"/>
-      <c r="AO78" s="16"/>
-      <c r="AP78" s="16"/>
-      <c r="AQ78" s="16"/>
-      <c r="AR78" s="16"/>
-      <c r="AS78" s="16"/>
-      <c r="AT78" s="16"/>
-      <c r="AU78" s="16"/>
-      <c r="AV78" s="16"/>
-      <c r="AW78" s="16"/>
-      <c r="AX78" s="16"/>
-      <c r="AY78" s="16"/>
-      <c r="AZ78" s="16"/>
-      <c r="BA78" s="16"/>
-      <c r="BB78" s="16"/>
-      <c r="BC78" s="16"/>
-      <c r="BD78" s="16"/>
-      <c r="BE78" s="16"/>
-      <c r="BF78" s="16"/>
-      <c r="BG78" s="16"/>
-      <c r="BH78" s="16"/>
-      <c r="BI78" s="16"/>
-      <c r="BJ78" s="13"/>
-      <c r="BK78" s="13"/>
-      <c r="BL78" s="13"/>
-      <c r="BM78" s="13"/>
-      <c r="BN78" s="13"/>
-      <c r="BO78" s="13"/>
-      <c r="BP78" s="13"/>
-      <c r="BQ78" s="13"/>
-      <c r="BR78" s="13"/>
-      <c r="BS78" s="13"/>
-      <c r="BT78" s="13"/>
-      <c r="BU78" s="13"/>
-      <c r="BV78" s="13"/>
-      <c r="BW78" s="13"/>
-      <c r="BX78" s="13"/>
-      <c r="BY78" s="13"/>
-      <c r="BZ78" s="13"/>
-      <c r="CA78" s="13"/>
-      <c r="CB78" s="13"/>
-      <c r="CC78" s="13"/>
-      <c r="CD78" s="13"/>
-      <c r="CE78" s="13"/>
-      <c r="CF78" s="13"/>
-      <c r="CG78" s="13"/>
-      <c r="CH78" s="13"/>
-      <c r="CI78" s="13"/>
-      <c r="CJ78" s="13"/>
-      <c r="CK78" s="13"/>
-      <c r="CL78" s="13"/>
-      <c r="CM78" s="13"/>
-      <c r="CN78" s="13"/>
-      <c r="CO78" s="13"/>
-      <c r="CP78" s="13"/>
-      <c r="CQ78" s="13"/>
-      <c r="CR78" s="13"/>
-      <c r="CS78" s="13"/>
-      <c r="CT78" s="14"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="18"/>
+      <c r="I78" s="18"/>
+      <c r="J78" s="18"/>
+      <c r="K78" s="18"/>
+      <c r="L78" s="18"/>
+      <c r="M78" s="18"/>
+      <c r="N78" s="18"/>
+      <c r="O78" s="18"/>
+      <c r="P78" s="18"/>
+      <c r="Q78" s="18"/>
+      <c r="R78" s="18"/>
+      <c r="S78" s="18"/>
+      <c r="T78" s="18"/>
+      <c r="U78" s="18"/>
+      <c r="V78" s="18"/>
+      <c r="W78" s="18"/>
+      <c r="X78" s="18"/>
+      <c r="Y78" s="18"/>
+      <c r="Z78" s="18"/>
+      <c r="AA78" s="18"/>
+      <c r="AB78" s="18"/>
+      <c r="AC78" s="18"/>
+      <c r="AD78" s="18"/>
+      <c r="AE78" s="18"/>
+      <c r="AF78" s="18"/>
+      <c r="AG78" s="18"/>
+      <c r="AH78" s="18"/>
+      <c r="AI78" s="18"/>
+      <c r="AJ78" s="18"/>
+      <c r="AK78" s="18"/>
+      <c r="AL78" s="18"/>
+      <c r="AM78" s="18"/>
+      <c r="AN78" s="17"/>
+      <c r="AO78" s="17"/>
+      <c r="AP78" s="17"/>
+      <c r="AQ78" s="17"/>
+      <c r="AR78" s="17"/>
+      <c r="AS78" s="17"/>
+      <c r="AT78" s="17"/>
+      <c r="AU78" s="17"/>
+      <c r="AV78" s="17"/>
+      <c r="AW78" s="17"/>
+      <c r="AX78" s="17"/>
+      <c r="AY78" s="17"/>
+      <c r="AZ78" s="17"/>
+      <c r="BA78" s="17"/>
+      <c r="BB78" s="17"/>
+      <c r="BC78" s="17"/>
+      <c r="BD78" s="17"/>
+      <c r="BE78" s="17"/>
+      <c r="BF78" s="17"/>
+      <c r="BG78" s="17"/>
+      <c r="BH78" s="17"/>
+      <c r="BI78" s="17"/>
+      <c r="BJ78" s="18"/>
+      <c r="BK78" s="18"/>
+      <c r="BL78" s="18"/>
+      <c r="BM78" s="18"/>
+      <c r="BN78" s="18"/>
+      <c r="BO78" s="18"/>
+      <c r="BP78" s="18"/>
+      <c r="BQ78" s="18"/>
+      <c r="BR78" s="18"/>
+      <c r="BS78" s="18"/>
+      <c r="BT78" s="18"/>
+      <c r="BU78" s="18"/>
+      <c r="BV78" s="18"/>
+      <c r="BW78" s="18"/>
+      <c r="BX78" s="18"/>
+      <c r="BY78" s="18"/>
+      <c r="BZ78" s="18"/>
+      <c r="CA78" s="18"/>
+      <c r="CB78" s="18"/>
+      <c r="CC78" s="18"/>
+      <c r="CD78" s="18"/>
+      <c r="CE78" s="18"/>
+      <c r="CF78" s="18"/>
+      <c r="CG78" s="18"/>
+      <c r="CH78" s="18"/>
+      <c r="CI78" s="18"/>
+      <c r="CJ78" s="18"/>
+      <c r="CK78" s="18"/>
+      <c r="CL78" s="18"/>
+      <c r="CM78" s="18"/>
+      <c r="CN78" s="18"/>
+      <c r="CO78" s="18"/>
+      <c r="CP78" s="18"/>
+      <c r="CQ78" s="18"/>
+      <c r="CR78" s="18"/>
+      <c r="CS78" s="18"/>
+      <c r="CT78" s="19"/>
     </row>
     <row r="79" spans="3:98" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C79" s="30"/>
-      <c r="D79" s="31"/>
-      <c r="E79" s="31"/>
-      <c r="F79" s="31"/>
-      <c r="G79" s="28"/>
-      <c r="H79" s="28"/>
-      <c r="I79" s="28"/>
-      <c r="J79" s="28"/>
-      <c r="K79" s="28"/>
-      <c r="L79" s="28"/>
-      <c r="M79" s="28"/>
-      <c r="N79" s="28"/>
-      <c r="O79" s="28"/>
-      <c r="P79" s="28"/>
-      <c r="Q79" s="28"/>
-      <c r="R79" s="28"/>
-      <c r="S79" s="28"/>
-      <c r="T79" s="28"/>
-      <c r="U79" s="28"/>
-      <c r="V79" s="28"/>
-      <c r="W79" s="28"/>
-      <c r="X79" s="28"/>
-      <c r="Y79" s="28"/>
-      <c r="Z79" s="28"/>
-      <c r="AA79" s="28"/>
-      <c r="AB79" s="28"/>
-      <c r="AC79" s="28"/>
-      <c r="AD79" s="28"/>
-      <c r="AE79" s="28"/>
-      <c r="AF79" s="28"/>
-      <c r="AG79" s="28"/>
-      <c r="AH79" s="28"/>
-      <c r="AI79" s="28"/>
-      <c r="AJ79" s="28"/>
-      <c r="AK79" s="28"/>
-      <c r="AL79" s="28"/>
-      <c r="AM79" s="28"/>
-      <c r="AN79" s="31"/>
-      <c r="AO79" s="31"/>
-      <c r="AP79" s="31"/>
-      <c r="AQ79" s="31"/>
-      <c r="AR79" s="31"/>
-      <c r="AS79" s="31"/>
-      <c r="AT79" s="31"/>
-      <c r="AU79" s="31"/>
-      <c r="AV79" s="31"/>
-      <c r="AW79" s="31"/>
-      <c r="AX79" s="31"/>
-      <c r="AY79" s="31"/>
-      <c r="AZ79" s="31"/>
-      <c r="BA79" s="31"/>
-      <c r="BB79" s="31"/>
-      <c r="BC79" s="31"/>
-      <c r="BD79" s="31"/>
-      <c r="BE79" s="31"/>
-      <c r="BF79" s="31"/>
-      <c r="BG79" s="31"/>
-      <c r="BH79" s="31"/>
-      <c r="BI79" s="31"/>
-      <c r="BJ79" s="28"/>
-      <c r="BK79" s="28"/>
-      <c r="BL79" s="28"/>
-      <c r="BM79" s="28"/>
-      <c r="BN79" s="28"/>
-      <c r="BO79" s="28"/>
-      <c r="BP79" s="28"/>
-      <c r="BQ79" s="28"/>
-      <c r="BR79" s="28"/>
-      <c r="BS79" s="28"/>
-      <c r="BT79" s="28"/>
-      <c r="BU79" s="28"/>
-      <c r="BV79" s="28"/>
-      <c r="BW79" s="28"/>
-      <c r="BX79" s="28"/>
-      <c r="BY79" s="28"/>
-      <c r="BZ79" s="28"/>
-      <c r="CA79" s="28"/>
-      <c r="CB79" s="28"/>
-      <c r="CC79" s="28"/>
-      <c r="CD79" s="28"/>
-      <c r="CE79" s="28"/>
-      <c r="CF79" s="28"/>
-      <c r="CG79" s="28"/>
-      <c r="CH79" s="28"/>
-      <c r="CI79" s="28"/>
-      <c r="CJ79" s="28"/>
-      <c r="CK79" s="28"/>
-      <c r="CL79" s="28"/>
-      <c r="CM79" s="28"/>
-      <c r="CN79" s="28"/>
-      <c r="CO79" s="28"/>
-      <c r="CP79" s="28"/>
-      <c r="CQ79" s="28"/>
-      <c r="CR79" s="28"/>
-      <c r="CS79" s="28"/>
-      <c r="CT79" s="29"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="21"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="14"/>
+      <c r="J79" s="14"/>
+      <c r="K79" s="14"/>
+      <c r="L79" s="14"/>
+      <c r="M79" s="14"/>
+      <c r="N79" s="14"/>
+      <c r="O79" s="14"/>
+      <c r="P79" s="14"/>
+      <c r="Q79" s="14"/>
+      <c r="R79" s="14"/>
+      <c r="S79" s="14"/>
+      <c r="T79" s="14"/>
+      <c r="U79" s="14"/>
+      <c r="V79" s="14"/>
+      <c r="W79" s="14"/>
+      <c r="X79" s="14"/>
+      <c r="Y79" s="14"/>
+      <c r="Z79" s="14"/>
+      <c r="AA79" s="14"/>
+      <c r="AB79" s="14"/>
+      <c r="AC79" s="14"/>
+      <c r="AD79" s="14"/>
+      <c r="AE79" s="14"/>
+      <c r="AF79" s="14"/>
+      <c r="AG79" s="14"/>
+      <c r="AH79" s="14"/>
+      <c r="AI79" s="14"/>
+      <c r="AJ79" s="14"/>
+      <c r="AK79" s="14"/>
+      <c r="AL79" s="14"/>
+      <c r="AM79" s="14"/>
+      <c r="AN79" s="21"/>
+      <c r="AO79" s="21"/>
+      <c r="AP79" s="21"/>
+      <c r="AQ79" s="21"/>
+      <c r="AR79" s="21"/>
+      <c r="AS79" s="21"/>
+      <c r="AT79" s="21"/>
+      <c r="AU79" s="21"/>
+      <c r="AV79" s="21"/>
+      <c r="AW79" s="21"/>
+      <c r="AX79" s="21"/>
+      <c r="AY79" s="21"/>
+      <c r="AZ79" s="21"/>
+      <c r="BA79" s="21"/>
+      <c r="BB79" s="21"/>
+      <c r="BC79" s="21"/>
+      <c r="BD79" s="21"/>
+      <c r="BE79" s="21"/>
+      <c r="BF79" s="21"/>
+      <c r="BG79" s="21"/>
+      <c r="BH79" s="21"/>
+      <c r="BI79" s="21"/>
+      <c r="BJ79" s="14"/>
+      <c r="BK79" s="14"/>
+      <c r="BL79" s="14"/>
+      <c r="BM79" s="14"/>
+      <c r="BN79" s="14"/>
+      <c r="BO79" s="14"/>
+      <c r="BP79" s="14"/>
+      <c r="BQ79" s="14"/>
+      <c r="BR79" s="14"/>
+      <c r="BS79" s="14"/>
+      <c r="BT79" s="14"/>
+      <c r="BU79" s="14"/>
+      <c r="BV79" s="14"/>
+      <c r="BW79" s="14"/>
+      <c r="BX79" s="14"/>
+      <c r="BY79" s="14"/>
+      <c r="BZ79" s="14"/>
+      <c r="CA79" s="14"/>
+      <c r="CB79" s="14"/>
+      <c r="CC79" s="14"/>
+      <c r="CD79" s="14"/>
+      <c r="CE79" s="14"/>
+      <c r="CF79" s="14"/>
+      <c r="CG79" s="14"/>
+      <c r="CH79" s="14"/>
+      <c r="CI79" s="14"/>
+      <c r="CJ79" s="14"/>
+      <c r="CK79" s="14"/>
+      <c r="CL79" s="14"/>
+      <c r="CM79" s="14"/>
+      <c r="CN79" s="14"/>
+      <c r="CO79" s="14"/>
+      <c r="CP79" s="14"/>
+      <c r="CQ79" s="14"/>
+      <c r="CR79" s="14"/>
+      <c r="CS79" s="14"/>
+      <c r="CT79" s="15"/>
     </row>
     <row r="80" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9911,42 +9911,30 @@
     <row r="85" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="BZ79:CT79"/>
-    <mergeCell ref="C78:F78"/>
-    <mergeCell ref="G78:X78"/>
-    <mergeCell ref="Y78:AM78"/>
-    <mergeCell ref="AN78:BI78"/>
-    <mergeCell ref="BJ78:BY78"/>
-    <mergeCell ref="BZ78:CT78"/>
-    <mergeCell ref="C79:F79"/>
-    <mergeCell ref="G79:X79"/>
-    <mergeCell ref="Y79:AM79"/>
-    <mergeCell ref="AN79:BI79"/>
-    <mergeCell ref="BJ79:BY79"/>
-    <mergeCell ref="BZ77:CT77"/>
-    <mergeCell ref="C76:F76"/>
-    <mergeCell ref="G76:X76"/>
-    <mergeCell ref="Y76:AM76"/>
-    <mergeCell ref="AN76:BI76"/>
-    <mergeCell ref="BJ76:BY76"/>
-    <mergeCell ref="BZ76:CT76"/>
-    <mergeCell ref="C77:F77"/>
-    <mergeCell ref="G77:X77"/>
-    <mergeCell ref="Y77:AM77"/>
-    <mergeCell ref="AN77:BI77"/>
-    <mergeCell ref="BJ77:BY77"/>
-    <mergeCell ref="BZ75:CT75"/>
-    <mergeCell ref="C74:F74"/>
-    <mergeCell ref="G74:X74"/>
-    <mergeCell ref="Y74:AM74"/>
-    <mergeCell ref="AN74:BI74"/>
-    <mergeCell ref="BJ74:BY74"/>
-    <mergeCell ref="BZ74:CT74"/>
-    <mergeCell ref="C75:F75"/>
-    <mergeCell ref="G75:X75"/>
-    <mergeCell ref="Y75:AM75"/>
-    <mergeCell ref="AN75:BI75"/>
-    <mergeCell ref="BJ75:BY75"/>
+    <mergeCell ref="BZ71:CT71"/>
+    <mergeCell ref="C71:F71"/>
+    <mergeCell ref="G71:X71"/>
+    <mergeCell ref="Y71:AM71"/>
+    <mergeCell ref="AN71:BI71"/>
+    <mergeCell ref="BJ71:BY71"/>
+    <mergeCell ref="BZ69:CT69"/>
+    <mergeCell ref="A1:F3"/>
+    <mergeCell ref="A4:F6"/>
+    <mergeCell ref="G1:AD3"/>
+    <mergeCell ref="G4:AD6"/>
+    <mergeCell ref="BZ68:CT68"/>
+    <mergeCell ref="BJ68:BY68"/>
+    <mergeCell ref="AN68:BI68"/>
+    <mergeCell ref="Y68:AM68"/>
+    <mergeCell ref="G68:X68"/>
+    <mergeCell ref="C68:F68"/>
+    <mergeCell ref="Y70:AM70"/>
+    <mergeCell ref="AN70:BI70"/>
+    <mergeCell ref="BJ70:BY70"/>
+    <mergeCell ref="C69:F69"/>
+    <mergeCell ref="G69:X69"/>
+    <mergeCell ref="Y69:AM69"/>
+    <mergeCell ref="AN69:BI69"/>
     <mergeCell ref="BZ70:CT70"/>
     <mergeCell ref="BJ69:BY69"/>
     <mergeCell ref="BZ73:CT73"/>
@@ -9963,30 +9951,42 @@
     <mergeCell ref="BJ73:BY73"/>
     <mergeCell ref="C70:F70"/>
     <mergeCell ref="G70:X70"/>
-    <mergeCell ref="Y70:AM70"/>
-    <mergeCell ref="AN70:BI70"/>
-    <mergeCell ref="BJ70:BY70"/>
-    <mergeCell ref="C69:F69"/>
-    <mergeCell ref="G69:X69"/>
-    <mergeCell ref="Y69:AM69"/>
-    <mergeCell ref="AN69:BI69"/>
-    <mergeCell ref="BZ69:CT69"/>
-    <mergeCell ref="A1:F3"/>
-    <mergeCell ref="A4:F6"/>
-    <mergeCell ref="G1:AD3"/>
-    <mergeCell ref="G4:AD6"/>
-    <mergeCell ref="BZ68:CT68"/>
-    <mergeCell ref="BJ68:BY68"/>
-    <mergeCell ref="AN68:BI68"/>
-    <mergeCell ref="Y68:AM68"/>
-    <mergeCell ref="G68:X68"/>
-    <mergeCell ref="C68:F68"/>
-    <mergeCell ref="BZ71:CT71"/>
-    <mergeCell ref="C71:F71"/>
-    <mergeCell ref="G71:X71"/>
-    <mergeCell ref="Y71:AM71"/>
-    <mergeCell ref="AN71:BI71"/>
-    <mergeCell ref="BJ71:BY71"/>
+    <mergeCell ref="BZ75:CT75"/>
+    <mergeCell ref="C74:F74"/>
+    <mergeCell ref="G74:X74"/>
+    <mergeCell ref="Y74:AM74"/>
+    <mergeCell ref="AN74:BI74"/>
+    <mergeCell ref="BJ74:BY74"/>
+    <mergeCell ref="BZ74:CT74"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="G75:X75"/>
+    <mergeCell ref="Y75:AM75"/>
+    <mergeCell ref="AN75:BI75"/>
+    <mergeCell ref="BJ75:BY75"/>
+    <mergeCell ref="BZ77:CT77"/>
+    <mergeCell ref="C76:F76"/>
+    <mergeCell ref="G76:X76"/>
+    <mergeCell ref="Y76:AM76"/>
+    <mergeCell ref="AN76:BI76"/>
+    <mergeCell ref="BJ76:BY76"/>
+    <mergeCell ref="BZ76:CT76"/>
+    <mergeCell ref="C77:F77"/>
+    <mergeCell ref="G77:X77"/>
+    <mergeCell ref="Y77:AM77"/>
+    <mergeCell ref="AN77:BI77"/>
+    <mergeCell ref="BJ77:BY77"/>
+    <mergeCell ref="BZ79:CT79"/>
+    <mergeCell ref="C78:F78"/>
+    <mergeCell ref="G78:X78"/>
+    <mergeCell ref="Y78:AM78"/>
+    <mergeCell ref="AN78:BI78"/>
+    <mergeCell ref="BJ78:BY78"/>
+    <mergeCell ref="BZ78:CT78"/>
+    <mergeCell ref="C79:F79"/>
+    <mergeCell ref="G79:X79"/>
+    <mergeCell ref="Y79:AM79"/>
+    <mergeCell ref="AN79:BI79"/>
+    <mergeCell ref="BJ79:BY79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
REMOVE hard coded value.
</commit_message>
<xml_diff>
--- a/Documents/ScreenLayouts/Dashboard-Customer.xlsx
+++ b/Documents/ScreenLayouts/Dashboard-Customer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev/booking/Documents/ScreenLayouts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev-int/Documents/ScreenLayouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8FDC28-2978-1744-9D64-7FEB516D959E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F37CC74-2A21-9F41-97C7-40B2AA24EB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{90052BEC-FEBB-F247-ACB1-709744DE85BE}"/>
   </bookViews>
@@ -481,10 +481,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -493,29 +493,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -536,6 +515,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1103,10 +1103,10 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="19" name="Group 18">
+        <xdr:cNvPr id="7" name="Group 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D341672-93E2-4F43-8CAE-DF1C1179CA94}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F394905-536E-CA46-95DA-B9898F838359}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1116,16 +1116,16 @@
         <a:xfrm>
           <a:off x="838200" y="2273300"/>
           <a:ext cx="6946900" cy="1549400"/>
-          <a:chOff x="838200" y="2273300"/>
-          <a:chExt cx="6946900" cy="1549400"/>
+          <a:chOff x="9080500" y="546100"/>
+          <a:chExt cx="6908800" cy="1527054"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="7" name="Group 6">
+          <xdr:cNvPr id="8" name="Group 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F394905-536E-CA46-95DA-B9898F838359}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AE84D52-0C91-284A-B8AB-FBFEC999541F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1133,18 +1133,566 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="838200" y="2273300"/>
-            <a:ext cx="6946900" cy="1549400"/>
+            <a:off x="9080500" y="546100"/>
+            <a:ext cx="6908800" cy="1527054"/>
+            <a:chOff x="3898900" y="406400"/>
+            <a:chExt cx="6908800" cy="1527054"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="Rounded Rectangle 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6BC8E69-B1FC-CD48-B4C4-5958BFE8BEE4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3898900" y="406400"/>
+              <a:ext cx="6908800" cy="1527054"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst>
+                <a:gd name="adj" fmla="val 4235"/>
+              </a:avLst>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1600" b="1"/>
+                <a:t>Transport</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="TextBox 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62F46121-7338-9C4D-87B6-CC70D59B8D89}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8330165" y="727112"/>
+              <a:ext cx="2171700" cy="271086"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Vehicle Type: </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="1"/>
+                <a:t>Tampo</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="12" name="Rounded Rectangle 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42029719-CC9D-5A42-AB4C-DB129211DA58}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4394200" y="1628425"/>
+              <a:ext cx="1549400" cy="254000"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent6">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent6"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent6"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+                <a:t>5 Pepole sent request</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="13" name="TextBox 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F376FFBB-C23A-EC4B-8540-63AFE20CD45C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8305800" y="562066"/>
+              <a:ext cx="2451100" cy="264560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>Date:</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>2021-8-1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+                <a:t> 12:00 ~  2021-8-2 15:00</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14" name="TextBox 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF28F4E3-5B1A-7543-878C-8E726A8F8BAA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4127500" y="1312191"/>
+              <a:ext cx="1447800" cy="271086"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>From: </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>Narhe</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+                <a:t> Pune </a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="15" name="TextBox 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D96A4D1-5A94-6042-ABA2-090F36DF4256}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6921500" y="1291434"/>
+              <a:ext cx="3276600" cy="271086"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1400" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Destination: </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>Chandan nagar</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+                <a:t> Pune </a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="16" name="Rounded Rectangle 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75B3FA17-9202-3D45-85C6-9CFD2C589564}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6323276" y="1628425"/>
+              <a:ext cx="1422400" cy="266700"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent6">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent6"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent6"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+                <a:t>Find Service provider</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="35" name="Rounded Rectangle 34">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71E45CD0-EF64-D34A-B09F-BCD466313D25}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9645708" y="1633050"/>
+              <a:ext cx="1068100" cy="212008"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent6">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent6"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent6"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+                <a:t>Delete Post</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="TextBox 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{989706D7-2972-1F48-9E56-27A24912583D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9309006" y="855627"/>
+            <a:ext cx="3175000" cy="508353"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>House stuff shifting..................</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1100"/>
+              <a:t>................</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="37" name="Group 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E9F3824-8CEA-6B41-B7E6-68F5F55E9BCC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="825500" y="3848100"/>
+          <a:ext cx="6959600" cy="1612900"/>
+          <a:chOff x="825500" y="3848100"/>
+          <a:chExt cx="6959600" cy="1612900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="22" name="Group 21">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{124D3953-D963-E245-A4AE-0280AEA0AEA9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="825500" y="3848100"/>
+            <a:ext cx="6959600" cy="1612900"/>
             <a:chOff x="9080500" y="546100"/>
             <a:chExt cx="6908800" cy="1527054"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:grpSp>
           <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="8" name="Group 7">
+            <xdr:cNvPr id="23" name="Group 22">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AE84D52-0C91-284A-B8AB-FBFEC999541F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DC5F632-8F46-FE4C-B2DB-3D6385B38BA2}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1160,10 +1708,10 @@
           </xdr:grpSpPr>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
-              <xdr:cNvPr id="10" name="Rounded Rectangle 9">
+              <xdr:cNvPr id="25" name="Rounded Rectangle 24">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6BC8E69-B1FC-CD48-B4C4-5958BFE8BEE4}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8609092-EBDA-384C-8B94-DD1C63AD9E51}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1210,10 +1758,10 @@
           </xdr:sp>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
-              <xdr:cNvPr id="11" name="TextBox 10">
+              <xdr:cNvPr id="26" name="TextBox 25">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62F46121-7338-9C4D-87B6-CC70D59B8D89}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42DEC0F0-1283-E641-838F-3AE0DF737868}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1266,10 +1814,10 @@
           </xdr:sp>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
-              <xdr:cNvPr id="12" name="Rounded Rectangle 11">
+              <xdr:cNvPr id="27" name="Rounded Rectangle 26">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42029719-CC9D-5A42-AB4C-DB129211DA58}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70A3C786-73ED-4040-BCF2-1611B5493632}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1315,10 +1863,10 @@
           </xdr:sp>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
-              <xdr:cNvPr id="13" name="TextBox 12">
+              <xdr:cNvPr id="28" name="TextBox 27">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F376FFBB-C23A-EC4B-8540-63AFE20CD45C}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{898EF0F1-34A0-1142-B25F-CF9E08F7ABF9}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1376,10 +1924,10 @@
           </xdr:sp>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
-              <xdr:cNvPr id="14" name="TextBox 13">
+              <xdr:cNvPr id="29" name="TextBox 28">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF28F4E3-5B1A-7543-878C-8E726A8F8BAA}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{281FE097-7220-AF4E-A902-979F41B2DB6B}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1437,10 +1985,10 @@
           </xdr:sp>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
-              <xdr:cNvPr id="15" name="TextBox 14">
+              <xdr:cNvPr id="30" name="TextBox 29">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D96A4D1-5A94-6042-ABA2-090F36DF4256}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFBA7980-FF5D-0E4A-BB3F-E15F942DB593}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1498,10 +2046,10 @@
           </xdr:sp>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
-              <xdr:cNvPr id="16" name="Rounded Rectangle 15">
+              <xdr:cNvPr id="31" name="Rounded Rectangle 30">
                 <a:extLst>
                   <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75B3FA17-9202-3D45-85C6-9CFD2C589564}"/>
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72ACD219-0E1F-B34F-8C27-B7393DF2EE03}"/>
                   </a:ext>
                 </a:extLst>
               </xdr:cNvPr>
@@ -1509,7 +2057,7 @@
             </xdr:nvSpPr>
             <xdr:spPr>
               <a:xfrm>
-                <a:off x="6323276" y="1628425"/>
+                <a:off x="6083300" y="1628425"/>
                 <a:ext cx="1422400" cy="266700"/>
               </a:xfrm>
               <a:prstGeom prst="roundRect">
@@ -1545,65 +2093,13 @@
               </a:p>
             </xdr:txBody>
           </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="35" name="Rounded Rectangle 34">
-                <a:extLst>
-                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71E45CD0-EF64-D34A-B09F-BCD466313D25}"/>
-                  </a:ext>
-                </a:extLst>
-              </xdr:cNvPr>
-              <xdr:cNvSpPr/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="9645708" y="1633050"/>
-                <a:ext cx="1068100" cy="212008"/>
-              </a:xfrm>
-              <a:prstGeom prst="roundRect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="2">
-                <a:schemeClr val="accent6">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:lnRef>
-              <a:fillRef idx="1">
-                <a:schemeClr val="accent6"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent6"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="ctr"/>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-                  <a:t>Delete Post</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB" sz="1100"/>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
         </xdr:grpSp>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="9" name="TextBox 8">
+            <xdr:cNvPr id="24" name="TextBox 23">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{989706D7-2972-1F48-9E56-27A24912583D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DADC75B-96AF-3348-BF09-88D702255AF2}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1655,10 +2151,10 @@
       </xdr:grpSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="38" name="Rounded Rectangle 37">
+          <xdr:cNvPr id="36" name="Rounded Rectangle 35">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A26D927E-A158-FB42-990A-B9A5BA08E79B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1A52EE4-4030-8348-9948-0D2A06610E58}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1666,14 +2162,14 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="5549900" y="3492500"/>
-            <a:ext cx="1016000" cy="254000"/>
+            <a:off x="6616700" y="5181600"/>
+            <a:ext cx="1073990" cy="215110"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
             <a:avLst/>
           </a:prstGeom>
           <a:solidFill>
-            <a:schemeClr val="accent4"/>
+            <a:schemeClr val="accent2"/>
           </a:solidFill>
         </xdr:spPr>
         <xdr:style>
@@ -1693,661 +2189,13 @@
           </a:fontRef>
         </xdr:style>
         <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr algn="l"/>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1100"/>
-              <a:t>Update</a:t>
-            </a:r>
+            <a:pPr algn="ctr"/>
             <a:r>
               <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-              <a:t> Post</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="32" name="Group 31">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56CB1962-38B4-0C4A-9262-4393BF55A308}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="825500" y="3848100"/>
-          <a:ext cx="6959600" cy="1612900"/>
-          <a:chOff x="825500" y="3848100"/>
-          <a:chExt cx="6959600" cy="1612900"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="37" name="Group 36">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E9F3824-8CEA-6B41-B7E6-68F5F55E9BCC}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="825500" y="3848100"/>
-            <a:ext cx="6959600" cy="1612900"/>
-            <a:chOff x="825500" y="3848100"/>
-            <a:chExt cx="6959600" cy="1612900"/>
-          </a:xfrm>
-        </xdr:grpSpPr>
-        <xdr:grpSp>
-          <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="22" name="Group 21">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{124D3953-D963-E245-A4AE-0280AEA0AEA9}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGrpSpPr/>
-          </xdr:nvGrpSpPr>
-          <xdr:grpSpPr>
-            <a:xfrm>
-              <a:off x="825500" y="3848100"/>
-              <a:ext cx="6959600" cy="1612900"/>
-              <a:chOff x="9080500" y="546100"/>
-              <a:chExt cx="6908800" cy="1527054"/>
-            </a:xfrm>
-          </xdr:grpSpPr>
-          <xdr:grpSp>
-            <xdr:nvGrpSpPr>
-              <xdr:cNvPr id="23" name="Group 22">
-                <a:extLst>
-                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DC5F632-8F46-FE4C-B2DB-3D6385B38BA2}"/>
-                  </a:ext>
-                </a:extLst>
-              </xdr:cNvPr>
-              <xdr:cNvGrpSpPr/>
-            </xdr:nvGrpSpPr>
-            <xdr:grpSpPr>
-              <a:xfrm>
-                <a:off x="9080500" y="546100"/>
-                <a:ext cx="6908800" cy="1527054"/>
-                <a:chOff x="3898900" y="406400"/>
-                <a:chExt cx="6908800" cy="1527054"/>
-              </a:xfrm>
-            </xdr:grpSpPr>
-            <xdr:sp macro="" textlink="">
-              <xdr:nvSpPr>
-                <xdr:cNvPr id="25" name="Rounded Rectangle 24">
-                  <a:extLst>
-                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8609092-EBDA-384C-8B94-DD1C63AD9E51}"/>
-                    </a:ext>
-                  </a:extLst>
-                </xdr:cNvPr>
-                <xdr:cNvSpPr/>
-              </xdr:nvSpPr>
-              <xdr:spPr>
-                <a:xfrm>
-                  <a:off x="3898900" y="406400"/>
-                  <a:ext cx="6908800" cy="1527054"/>
-                </a:xfrm>
-                <a:prstGeom prst="roundRect">
-                  <a:avLst>
-                    <a:gd name="adj" fmla="val 4235"/>
-                  </a:avLst>
-                </a:prstGeom>
-              </xdr:spPr>
-              <xdr:style>
-                <a:lnRef idx="2">
-                  <a:schemeClr val="accent1">
-                    <a:shade val="50000"/>
-                  </a:schemeClr>
-                </a:lnRef>
-                <a:fillRef idx="1">
-                  <a:schemeClr val="accent1"/>
-                </a:fillRef>
-                <a:effectRef idx="0">
-                  <a:schemeClr val="accent1"/>
-                </a:effectRef>
-                <a:fontRef idx="minor">
-                  <a:schemeClr val="lt1"/>
-                </a:fontRef>
-              </xdr:style>
-              <xdr:txBody>
-                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr algn="l"/>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1600" b="1"/>
-                    <a:t>Transport</a:t>
-                  </a:r>
-                </a:p>
-              </xdr:txBody>
-            </xdr:sp>
-            <xdr:sp macro="" textlink="">
-              <xdr:nvSpPr>
-                <xdr:cNvPr id="26" name="TextBox 25">
-                  <a:extLst>
-                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42DEC0F0-1283-E641-838F-3AE0DF737868}"/>
-                    </a:ext>
-                  </a:extLst>
-                </xdr:cNvPr>
-                <xdr:cNvSpPr txBox="1"/>
-              </xdr:nvSpPr>
-              <xdr:spPr>
-                <a:xfrm>
-                  <a:off x="8330165" y="727112"/>
-                  <a:ext cx="2171700" cy="271086"/>
-                </a:xfrm>
-                <a:prstGeom prst="rect">
-                  <a:avLst/>
-                </a:prstGeom>
-                <a:noFill/>
-              </xdr:spPr>
-              <xdr:style>
-                <a:lnRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:lnRef>
-                <a:fillRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:fillRef>
-                <a:effectRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:effectRef>
-                <a:fontRef idx="minor">
-                  <a:schemeClr val="tx1"/>
-                </a:fontRef>
-              </xdr:style>
-              <xdr:txBody>
-                <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1400" b="1">
-                      <a:solidFill>
-                        <a:schemeClr val="bg1"/>
-                      </a:solidFill>
-                    </a:rPr>
-                    <a:t>Vehicle Type: </a:t>
-                  </a:r>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1100" b="1"/>
-                    <a:t>Tampo</a:t>
-                  </a:r>
-                </a:p>
-              </xdr:txBody>
-            </xdr:sp>
-            <xdr:sp macro="" textlink="">
-              <xdr:nvSpPr>
-                <xdr:cNvPr id="27" name="Rounded Rectangle 26">
-                  <a:extLst>
-                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70A3C786-73ED-4040-BCF2-1611B5493632}"/>
-                    </a:ext>
-                  </a:extLst>
-                </xdr:cNvPr>
-                <xdr:cNvSpPr/>
-              </xdr:nvSpPr>
-              <xdr:spPr>
-                <a:xfrm>
-                  <a:off x="4394200" y="1628425"/>
-                  <a:ext cx="1549400" cy="254000"/>
-                </a:xfrm>
-                <a:prstGeom prst="roundRect">
-                  <a:avLst/>
-                </a:prstGeom>
-              </xdr:spPr>
-              <xdr:style>
-                <a:lnRef idx="2">
-                  <a:schemeClr val="accent6">
-                    <a:shade val="50000"/>
-                  </a:schemeClr>
-                </a:lnRef>
-                <a:fillRef idx="1">
-                  <a:schemeClr val="accent6"/>
-                </a:fillRef>
-                <a:effectRef idx="0">
-                  <a:schemeClr val="accent6"/>
-                </a:effectRef>
-                <a:fontRef idx="minor">
-                  <a:schemeClr val="lt1"/>
-                </a:fontRef>
-              </xdr:style>
-              <xdr:txBody>
-                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr algn="l"/>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-                    <a:t>5 Pepole sent request</a:t>
-                  </a:r>
-                  <a:endParaRPr lang="en-GB" sz="1100"/>
-                </a:p>
-              </xdr:txBody>
-            </xdr:sp>
-            <xdr:sp macro="" textlink="">
-              <xdr:nvSpPr>
-                <xdr:cNvPr id="28" name="TextBox 27">
-                  <a:extLst>
-                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{898EF0F1-34A0-1142-B25F-CF9E08F7ABF9}"/>
-                    </a:ext>
-                  </a:extLst>
-                </xdr:cNvPr>
-                <xdr:cNvSpPr txBox="1"/>
-              </xdr:nvSpPr>
-              <xdr:spPr>
-                <a:xfrm>
-                  <a:off x="8305800" y="562066"/>
-                  <a:ext cx="2451100" cy="264560"/>
-                </a:xfrm>
-                <a:prstGeom prst="rect">
-                  <a:avLst/>
-                </a:prstGeom>
-                <a:noFill/>
-              </xdr:spPr>
-              <xdr:style>
-                <a:lnRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:lnRef>
-                <a:fillRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:fillRef>
-                <a:effectRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:effectRef>
-                <a:fontRef idx="minor">
-                  <a:schemeClr val="tx1"/>
-                </a:fontRef>
-              </xdr:style>
-              <xdr:txBody>
-                <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1100"/>
-                    <a:t>Date:</a:t>
-                  </a:r>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-                    <a:t> </a:t>
-                  </a:r>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1100"/>
-                    <a:t>2021-8-1</a:t>
-                  </a:r>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-                    <a:t> 12:00 ~  2021-8-2 15:00</a:t>
-                  </a:r>
-                  <a:endParaRPr lang="en-GB" sz="1100"/>
-                </a:p>
-              </xdr:txBody>
-            </xdr:sp>
-            <xdr:sp macro="" textlink="">
-              <xdr:nvSpPr>
-                <xdr:cNvPr id="29" name="TextBox 28">
-                  <a:extLst>
-                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{281FE097-7220-AF4E-A902-979F41B2DB6B}"/>
-                    </a:ext>
-                  </a:extLst>
-                </xdr:cNvPr>
-                <xdr:cNvSpPr txBox="1"/>
-              </xdr:nvSpPr>
-              <xdr:spPr>
-                <a:xfrm>
-                  <a:off x="4127500" y="1312191"/>
-                  <a:ext cx="1447800" cy="271086"/>
-                </a:xfrm>
-                <a:prstGeom prst="rect">
-                  <a:avLst/>
-                </a:prstGeom>
-                <a:noFill/>
-              </xdr:spPr>
-              <xdr:style>
-                <a:lnRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:lnRef>
-                <a:fillRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:fillRef>
-                <a:effectRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:effectRef>
-                <a:fontRef idx="minor">
-                  <a:schemeClr val="tx1"/>
-                </a:fontRef>
-              </xdr:style>
-              <xdr:txBody>
-                <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1400" b="1">
-                      <a:solidFill>
-                        <a:schemeClr val="bg1"/>
-                      </a:solidFill>
-                    </a:rPr>
-                    <a:t>From: </a:t>
-                  </a:r>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1100"/>
-                    <a:t>Narhe</a:t>
-                  </a:r>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-                    <a:t> Pune </a:t>
-                  </a:r>
-                  <a:endParaRPr lang="en-GB" sz="1100"/>
-                </a:p>
-              </xdr:txBody>
-            </xdr:sp>
-            <xdr:sp macro="" textlink="">
-              <xdr:nvSpPr>
-                <xdr:cNvPr id="30" name="TextBox 29">
-                  <a:extLst>
-                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFBA7980-FF5D-0E4A-BB3F-E15F942DB593}"/>
-                    </a:ext>
-                  </a:extLst>
-                </xdr:cNvPr>
-                <xdr:cNvSpPr txBox="1"/>
-              </xdr:nvSpPr>
-              <xdr:spPr>
-                <a:xfrm>
-                  <a:off x="6921500" y="1291434"/>
-                  <a:ext cx="3276600" cy="271086"/>
-                </a:xfrm>
-                <a:prstGeom prst="rect">
-                  <a:avLst/>
-                </a:prstGeom>
-                <a:noFill/>
-              </xdr:spPr>
-              <xdr:style>
-                <a:lnRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:lnRef>
-                <a:fillRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:fillRef>
-                <a:effectRef idx="0">
-                  <a:scrgbClr r="0" g="0" b="0"/>
-                </a:effectRef>
-                <a:fontRef idx="minor">
-                  <a:schemeClr val="tx1"/>
-                </a:fontRef>
-              </xdr:style>
-              <xdr:txBody>
-                <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1400" b="1">
-                      <a:solidFill>
-                        <a:schemeClr val="bg1"/>
-                      </a:solidFill>
-                    </a:rPr>
-                    <a:t>Destination: </a:t>
-                  </a:r>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1100"/>
-                    <a:t>Chandan nagar</a:t>
-                  </a:r>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-                    <a:t> Pune </a:t>
-                  </a:r>
-                  <a:endParaRPr lang="en-GB" sz="1100"/>
-                </a:p>
-              </xdr:txBody>
-            </xdr:sp>
-            <xdr:sp macro="" textlink="">
-              <xdr:nvSpPr>
-                <xdr:cNvPr id="31" name="Rounded Rectangle 30">
-                  <a:extLst>
-                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72ACD219-0E1F-B34F-8C27-B7393DF2EE03}"/>
-                    </a:ext>
-                  </a:extLst>
-                </xdr:cNvPr>
-                <xdr:cNvSpPr/>
-              </xdr:nvSpPr>
-              <xdr:spPr>
-                <a:xfrm>
-                  <a:off x="6083300" y="1628425"/>
-                  <a:ext cx="1422400" cy="266700"/>
-                </a:xfrm>
-                <a:prstGeom prst="roundRect">
-                  <a:avLst/>
-                </a:prstGeom>
-              </xdr:spPr>
-              <xdr:style>
-                <a:lnRef idx="2">
-                  <a:schemeClr val="accent6">
-                    <a:shade val="50000"/>
-                  </a:schemeClr>
-                </a:lnRef>
-                <a:fillRef idx="1">
-                  <a:schemeClr val="accent6"/>
-                </a:fillRef>
-                <a:effectRef idx="0">
-                  <a:schemeClr val="accent6"/>
-                </a:effectRef>
-                <a:fontRef idx="minor">
-                  <a:schemeClr val="lt1"/>
-                </a:fontRef>
-              </xdr:style>
-              <xdr:txBody>
-                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr algn="l"/>
-                  <a:r>
-                    <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-                    <a:t>Find Service provider</a:t>
-                  </a:r>
-                  <a:endParaRPr lang="en-GB" sz="1100"/>
-                </a:p>
-              </xdr:txBody>
-            </xdr:sp>
-          </xdr:grpSp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="24" name="TextBox 23">
-                <a:extLst>
-                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DADC75B-96AF-3348-BF09-88D702255AF2}"/>
-                  </a:ext>
-                </a:extLst>
-              </xdr:cNvPr>
-              <xdr:cNvSpPr txBox="1"/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="9309006" y="855627"/>
-                <a:ext cx="3175000" cy="508353"/>
-              </a:xfrm>
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="0">
-                <a:scrgbClr r="0" g="0" b="0"/>
-              </a:lnRef>
-              <a:fillRef idx="0">
-                <a:scrgbClr r="0" g="0" b="0"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:scrgbClr r="0" g="0" b="0"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="tx1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-                <a:noAutofit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1100"/>
-                  <a:t>House stuff shifting..................</a:t>
-                </a:r>
-              </a:p>
-              <a:p>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1100"/>
-                  <a:t>................</a:t>
-                </a:r>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-        </xdr:grpSp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="36" name="Rounded Rectangle 35">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1A52EE4-4030-8348-9948-0D2A06610E58}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6616700" y="5181600"/>
-              <a:ext cx="1073990" cy="215110"/>
-            </a:xfrm>
-            <a:prstGeom prst="roundRect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent6">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent6"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent6"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr"/>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-                <a:t>Delete Post</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-GB" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="39" name="Rounded Rectangle 38">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40E47B09-A755-FD42-B9B8-C4C0A261D367}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5511800" y="5143500"/>
-            <a:ext cx="1016000" cy="254000"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent4"/>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent6">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1100"/>
-              <a:t>Update</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-              <a:t> Post</a:t>
+              <a:t>Delete Post</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB" sz="1100"/>
           </a:p>
@@ -2658,7 +2506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43867302-6022-BC45-9802-796B2A9AA285}">
   <dimension ref="A1:DD85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
       <selection activeCell="BJ73" sqref="BJ73:BY73"/>
     </sheetView>
   </sheetViews>
@@ -2668,204 +2516,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="21"/>
     </row>
     <row r="2" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="28"/>
-      <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="28"/>
-      <c r="Z2" s="28"/>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="28"/>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="28"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="21"/>
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="21"/>
     </row>
     <row r="3" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="28"/>
-      <c r="Y3" s="28"/>
-      <c r="Z3" s="28"/>
-      <c r="AA3" s="28"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="28"/>
-      <c r="AD3" s="28"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="21"/>
+      <c r="AD3" s="21"/>
     </row>
     <row r="4" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="29" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
-      <c r="W4" s="29"/>
-      <c r="X4" s="29"/>
-      <c r="Y4" s="29"/>
-      <c r="Z4" s="29"/>
-      <c r="AA4" s="29"/>
-      <c r="AB4" s="29"/>
-      <c r="AC4" s="29"/>
-      <c r="AD4" s="29"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
     </row>
     <row r="5" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="29"/>
-      <c r="Z5" s="29"/>
-      <c r="AA5" s="29"/>
-      <c r="AB5" s="29"/>
-      <c r="AC5" s="29"/>
-      <c r="AD5" s="29"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="22"/>
+      <c r="Y5" s="22"/>
+      <c r="Z5" s="22"/>
+      <c r="AA5" s="22"/>
+      <c r="AB5" s="22"/>
+      <c r="AC5" s="22"/>
+      <c r="AD5" s="22"/>
     </row>
     <row r="6" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="29"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="29"/>
-      <c r="Z6" s="29"/>
-      <c r="AA6" s="29"/>
-      <c r="AB6" s="29"/>
-      <c r="AC6" s="29"/>
-      <c r="AD6" s="29"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="22"/>
     </row>
     <row r="9" spans="1:108" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:108" ht="8" customHeight="1" x14ac:dyDescent="0.2">
@@ -8638,222 +8486,222 @@
       <c r="CT67" s="11"/>
     </row>
     <row r="68" spans="3:98" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C68" s="32" t="s">
+      <c r="C68" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D68" s="30"/>
-      <c r="E68" s="30"/>
-      <c r="F68" s="30"/>
-      <c r="G68" s="30" t="s">
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H68" s="30"/>
-      <c r="I68" s="30"/>
-      <c r="J68" s="30"/>
-      <c r="K68" s="30"/>
-      <c r="L68" s="30"/>
-      <c r="M68" s="30"/>
-      <c r="N68" s="30"/>
-      <c r="O68" s="30"/>
-      <c r="P68" s="30"/>
-      <c r="Q68" s="30"/>
-      <c r="R68" s="30"/>
-      <c r="S68" s="30"/>
-      <c r="T68" s="30"/>
-      <c r="U68" s="30"/>
-      <c r="V68" s="30"/>
-      <c r="W68" s="30"/>
-      <c r="X68" s="30"/>
-      <c r="Y68" s="30" t="s">
+      <c r="H68" s="23"/>
+      <c r="I68" s="23"/>
+      <c r="J68" s="23"/>
+      <c r="K68" s="23"/>
+      <c r="L68" s="23"/>
+      <c r="M68" s="23"/>
+      <c r="N68" s="23"/>
+      <c r="O68" s="23"/>
+      <c r="P68" s="23"/>
+      <c r="Q68" s="23"/>
+      <c r="R68" s="23"/>
+      <c r="S68" s="23"/>
+      <c r="T68" s="23"/>
+      <c r="U68" s="23"/>
+      <c r="V68" s="23"/>
+      <c r="W68" s="23"/>
+      <c r="X68" s="23"/>
+      <c r="Y68" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="Z68" s="30"/>
-      <c r="AA68" s="30"/>
-      <c r="AB68" s="30"/>
-      <c r="AC68" s="30"/>
-      <c r="AD68" s="30"/>
-      <c r="AE68" s="30"/>
-      <c r="AF68" s="30"/>
-      <c r="AG68" s="30"/>
-      <c r="AH68" s="30"/>
-      <c r="AI68" s="30"/>
-      <c r="AJ68" s="30"/>
-      <c r="AK68" s="30"/>
-      <c r="AL68" s="30"/>
-      <c r="AM68" s="30"/>
-      <c r="AN68" s="30" t="s">
+      <c r="Z68" s="23"/>
+      <c r="AA68" s="23"/>
+      <c r="AB68" s="23"/>
+      <c r="AC68" s="23"/>
+      <c r="AD68" s="23"/>
+      <c r="AE68" s="23"/>
+      <c r="AF68" s="23"/>
+      <c r="AG68" s="23"/>
+      <c r="AH68" s="23"/>
+      <c r="AI68" s="23"/>
+      <c r="AJ68" s="23"/>
+      <c r="AK68" s="23"/>
+      <c r="AL68" s="23"/>
+      <c r="AM68" s="23"/>
+      <c r="AN68" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="AO68" s="30"/>
-      <c r="AP68" s="30"/>
-      <c r="AQ68" s="30"/>
-      <c r="AR68" s="30"/>
-      <c r="AS68" s="30"/>
-      <c r="AT68" s="30"/>
-      <c r="AU68" s="30"/>
-      <c r="AV68" s="30"/>
-      <c r="AW68" s="30"/>
-      <c r="AX68" s="30"/>
-      <c r="AY68" s="30"/>
-      <c r="AZ68" s="30"/>
-      <c r="BA68" s="30"/>
-      <c r="BB68" s="30"/>
-      <c r="BC68" s="30"/>
-      <c r="BD68" s="30"/>
-      <c r="BE68" s="30"/>
-      <c r="BF68" s="30"/>
-      <c r="BG68" s="30"/>
-      <c r="BH68" s="30"/>
-      <c r="BI68" s="30"/>
-      <c r="BJ68" s="30" t="s">
+      <c r="AO68" s="23"/>
+      <c r="AP68" s="23"/>
+      <c r="AQ68" s="23"/>
+      <c r="AR68" s="23"/>
+      <c r="AS68" s="23"/>
+      <c r="AT68" s="23"/>
+      <c r="AU68" s="23"/>
+      <c r="AV68" s="23"/>
+      <c r="AW68" s="23"/>
+      <c r="AX68" s="23"/>
+      <c r="AY68" s="23"/>
+      <c r="AZ68" s="23"/>
+      <c r="BA68" s="23"/>
+      <c r="BB68" s="23"/>
+      <c r="BC68" s="23"/>
+      <c r="BD68" s="23"/>
+      <c r="BE68" s="23"/>
+      <c r="BF68" s="23"/>
+      <c r="BG68" s="23"/>
+      <c r="BH68" s="23"/>
+      <c r="BI68" s="23"/>
+      <c r="BJ68" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="BK68" s="30"/>
-      <c r="BL68" s="30"/>
-      <c r="BM68" s="30"/>
-      <c r="BN68" s="30"/>
-      <c r="BO68" s="30"/>
-      <c r="BP68" s="30"/>
-      <c r="BQ68" s="30"/>
-      <c r="BR68" s="30"/>
-      <c r="BS68" s="30"/>
-      <c r="BT68" s="30"/>
-      <c r="BU68" s="30"/>
-      <c r="BV68" s="30"/>
-      <c r="BW68" s="30"/>
-      <c r="BX68" s="30"/>
-      <c r="BY68" s="30"/>
-      <c r="BZ68" s="30" t="s">
+      <c r="BK68" s="23"/>
+      <c r="BL68" s="23"/>
+      <c r="BM68" s="23"/>
+      <c r="BN68" s="23"/>
+      <c r="BO68" s="23"/>
+      <c r="BP68" s="23"/>
+      <c r="BQ68" s="23"/>
+      <c r="BR68" s="23"/>
+      <c r="BS68" s="23"/>
+      <c r="BT68" s="23"/>
+      <c r="BU68" s="23"/>
+      <c r="BV68" s="23"/>
+      <c r="BW68" s="23"/>
+      <c r="BX68" s="23"/>
+      <c r="BY68" s="23"/>
+      <c r="BZ68" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="CA68" s="30"/>
-      <c r="CB68" s="30"/>
-      <c r="CC68" s="30"/>
-      <c r="CD68" s="30"/>
-      <c r="CE68" s="30"/>
-      <c r="CF68" s="30"/>
-      <c r="CG68" s="30"/>
-      <c r="CH68" s="30"/>
-      <c r="CI68" s="30"/>
-      <c r="CJ68" s="30"/>
-      <c r="CK68" s="30"/>
-      <c r="CL68" s="30"/>
-      <c r="CM68" s="30"/>
-      <c r="CN68" s="30"/>
-      <c r="CO68" s="30"/>
-      <c r="CP68" s="30"/>
-      <c r="CQ68" s="30"/>
-      <c r="CR68" s="30"/>
-      <c r="CS68" s="30"/>
-      <c r="CT68" s="31"/>
+      <c r="CA68" s="23"/>
+      <c r="CB68" s="23"/>
+      <c r="CC68" s="23"/>
+      <c r="CD68" s="23"/>
+      <c r="CE68" s="23"/>
+      <c r="CF68" s="23"/>
+      <c r="CG68" s="23"/>
+      <c r="CH68" s="23"/>
+      <c r="CI68" s="23"/>
+      <c r="CJ68" s="23"/>
+      <c r="CK68" s="23"/>
+      <c r="CL68" s="23"/>
+      <c r="CM68" s="23"/>
+      <c r="CN68" s="23"/>
+      <c r="CO68" s="23"/>
+      <c r="CP68" s="23"/>
+      <c r="CQ68" s="23"/>
+      <c r="CR68" s="23"/>
+      <c r="CS68" s="23"/>
+      <c r="CT68" s="24"/>
     </row>
     <row r="69" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C69" s="24">
+      <c r="C69" s="26">
         <v>1</v>
       </c>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="23" t="s">
+      <c r="D69" s="27"/>
+      <c r="E69" s="27"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H69" s="23"/>
-      <c r="I69" s="23"/>
-      <c r="J69" s="23"/>
-      <c r="K69" s="23"/>
-      <c r="L69" s="23"/>
-      <c r="M69" s="23"/>
-      <c r="N69" s="23"/>
-      <c r="O69" s="23"/>
-      <c r="P69" s="23"/>
-      <c r="Q69" s="23"/>
-      <c r="R69" s="23"/>
-      <c r="S69" s="23"/>
-      <c r="T69" s="23"/>
-      <c r="U69" s="23"/>
-      <c r="V69" s="23"/>
-      <c r="W69" s="23"/>
-      <c r="X69" s="23"/>
-      <c r="Y69" s="23" t="s">
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
+      <c r="J69" s="18"/>
+      <c r="K69" s="18"/>
+      <c r="L69" s="18"/>
+      <c r="M69" s="18"/>
+      <c r="N69" s="18"/>
+      <c r="O69" s="18"/>
+      <c r="P69" s="18"/>
+      <c r="Q69" s="18"/>
+      <c r="R69" s="18"/>
+      <c r="S69" s="18"/>
+      <c r="T69" s="18"/>
+      <c r="U69" s="18"/>
+      <c r="V69" s="18"/>
+      <c r="W69" s="18"/>
+      <c r="X69" s="18"/>
+      <c r="Y69" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="Z69" s="23"/>
-      <c r="AA69" s="23"/>
-      <c r="AB69" s="23"/>
-      <c r="AC69" s="23"/>
-      <c r="AD69" s="23"/>
-      <c r="AE69" s="23"/>
-      <c r="AF69" s="23"/>
-      <c r="AG69" s="23"/>
-      <c r="AH69" s="23"/>
-      <c r="AI69" s="23"/>
-      <c r="AJ69" s="23"/>
-      <c r="AK69" s="23"/>
-      <c r="AL69" s="23"/>
-      <c r="AM69" s="23"/>
-      <c r="AN69" s="25" t="s">
+      <c r="Z69" s="18"/>
+      <c r="AA69" s="18"/>
+      <c r="AB69" s="18"/>
+      <c r="AC69" s="18"/>
+      <c r="AD69" s="18"/>
+      <c r="AE69" s="18"/>
+      <c r="AF69" s="18"/>
+      <c r="AG69" s="18"/>
+      <c r="AH69" s="18"/>
+      <c r="AI69" s="18"/>
+      <c r="AJ69" s="18"/>
+      <c r="AK69" s="18"/>
+      <c r="AL69" s="18"/>
+      <c r="AM69" s="18"/>
+      <c r="AN69" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="AO69" s="25"/>
-      <c r="AP69" s="25"/>
-      <c r="AQ69" s="25"/>
-      <c r="AR69" s="25"/>
-      <c r="AS69" s="25"/>
-      <c r="AT69" s="25"/>
-      <c r="AU69" s="25"/>
-      <c r="AV69" s="25"/>
-      <c r="AW69" s="25"/>
-      <c r="AX69" s="25"/>
-      <c r="AY69" s="25"/>
-      <c r="AZ69" s="25"/>
-      <c r="BA69" s="25"/>
-      <c r="BB69" s="25"/>
-      <c r="BC69" s="25"/>
-      <c r="BD69" s="25"/>
-      <c r="BE69" s="25"/>
-      <c r="BF69" s="25"/>
-      <c r="BG69" s="25"/>
-      <c r="BH69" s="25"/>
-      <c r="BI69" s="25"/>
-      <c r="BJ69" s="23" t="s">
+      <c r="AO69" s="27"/>
+      <c r="AP69" s="27"/>
+      <c r="AQ69" s="27"/>
+      <c r="AR69" s="27"/>
+      <c r="AS69" s="27"/>
+      <c r="AT69" s="27"/>
+      <c r="AU69" s="27"/>
+      <c r="AV69" s="27"/>
+      <c r="AW69" s="27"/>
+      <c r="AX69" s="27"/>
+      <c r="AY69" s="27"/>
+      <c r="AZ69" s="27"/>
+      <c r="BA69" s="27"/>
+      <c r="BB69" s="27"/>
+      <c r="BC69" s="27"/>
+      <c r="BD69" s="27"/>
+      <c r="BE69" s="27"/>
+      <c r="BF69" s="27"/>
+      <c r="BG69" s="27"/>
+      <c r="BH69" s="27"/>
+      <c r="BI69" s="27"/>
+      <c r="BJ69" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="BK69" s="23"/>
-      <c r="BL69" s="23"/>
-      <c r="BM69" s="23"/>
-      <c r="BN69" s="23"/>
-      <c r="BO69" s="23"/>
-      <c r="BP69" s="23"/>
-      <c r="BQ69" s="23"/>
-      <c r="BR69" s="23"/>
-      <c r="BS69" s="23"/>
-      <c r="BT69" s="23"/>
-      <c r="BU69" s="23"/>
-      <c r="BV69" s="23"/>
-      <c r="BW69" s="23"/>
-      <c r="BX69" s="23"/>
-      <c r="BY69" s="23"/>
-      <c r="BZ69" s="23"/>
-      <c r="CA69" s="23"/>
-      <c r="CB69" s="23"/>
-      <c r="CC69" s="23"/>
-      <c r="CD69" s="23"/>
-      <c r="CE69" s="23"/>
-      <c r="CF69" s="23"/>
-      <c r="CG69" s="23"/>
-      <c r="CH69" s="23"/>
-      <c r="CI69" s="23"/>
-      <c r="CJ69" s="23"/>
-      <c r="CK69" s="23"/>
-      <c r="CL69" s="23"/>
-      <c r="CM69" s="23"/>
-      <c r="CN69" s="23"/>
-      <c r="CO69" s="23"/>
-      <c r="CP69" s="23"/>
-      <c r="CQ69" s="23"/>
-      <c r="CR69" s="23"/>
-      <c r="CS69" s="23"/>
-      <c r="CT69" s="26"/>
+      <c r="BK69" s="18"/>
+      <c r="BL69" s="18"/>
+      <c r="BM69" s="18"/>
+      <c r="BN69" s="18"/>
+      <c r="BO69" s="18"/>
+      <c r="BP69" s="18"/>
+      <c r="BQ69" s="18"/>
+      <c r="BR69" s="18"/>
+      <c r="BS69" s="18"/>
+      <c r="BT69" s="18"/>
+      <c r="BU69" s="18"/>
+      <c r="BV69" s="18"/>
+      <c r="BW69" s="18"/>
+      <c r="BX69" s="18"/>
+      <c r="BY69" s="18"/>
+      <c r="BZ69" s="18"/>
+      <c r="CA69" s="18"/>
+      <c r="CB69" s="18"/>
+      <c r="CC69" s="18"/>
+      <c r="CD69" s="18"/>
+      <c r="CE69" s="18"/>
+      <c r="CF69" s="18"/>
+      <c r="CG69" s="18"/>
+      <c r="CH69" s="18"/>
+      <c r="CI69" s="18"/>
+      <c r="CJ69" s="18"/>
+      <c r="CK69" s="18"/>
+      <c r="CL69" s="18"/>
+      <c r="CM69" s="18"/>
+      <c r="CN69" s="18"/>
+      <c r="CO69" s="18"/>
+      <c r="CP69" s="18"/>
+      <c r="CQ69" s="18"/>
+      <c r="CR69" s="18"/>
+      <c r="CS69" s="18"/>
+      <c r="CT69" s="19"/>
     </row>
     <row r="70" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C70" s="16">
@@ -8862,43 +8710,43 @@
       <c r="D70" s="17"/>
       <c r="E70" s="17"/>
       <c r="F70" s="17"/>
-      <c r="G70" s="22" t="s">
+      <c r="G70" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H70" s="18"/>
-      <c r="I70" s="18"/>
-      <c r="J70" s="18"/>
-      <c r="K70" s="18"/>
-      <c r="L70" s="18"/>
-      <c r="M70" s="18"/>
-      <c r="N70" s="18"/>
-      <c r="O70" s="18"/>
-      <c r="P70" s="18"/>
-      <c r="Q70" s="18"/>
-      <c r="R70" s="18"/>
-      <c r="S70" s="18"/>
-      <c r="T70" s="18"/>
-      <c r="U70" s="18"/>
-      <c r="V70" s="18"/>
-      <c r="W70" s="18"/>
-      <c r="X70" s="18"/>
-      <c r="Y70" s="18" t="s">
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="14"/>
+      <c r="K70" s="14"/>
+      <c r="L70" s="14"/>
+      <c r="M70" s="14"/>
+      <c r="N70" s="14"/>
+      <c r="O70" s="14"/>
+      <c r="P70" s="14"/>
+      <c r="Q70" s="14"/>
+      <c r="R70" s="14"/>
+      <c r="S70" s="14"/>
+      <c r="T70" s="14"/>
+      <c r="U70" s="14"/>
+      <c r="V70" s="14"/>
+      <c r="W70" s="14"/>
+      <c r="X70" s="14"/>
+      <c r="Y70" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="Z70" s="18"/>
-      <c r="AA70" s="18"/>
-      <c r="AB70" s="18"/>
-      <c r="AC70" s="18"/>
-      <c r="AD70" s="18"/>
-      <c r="AE70" s="18"/>
-      <c r="AF70" s="18"/>
-      <c r="AG70" s="18"/>
-      <c r="AH70" s="18"/>
-      <c r="AI70" s="18"/>
-      <c r="AJ70" s="18"/>
-      <c r="AK70" s="18"/>
-      <c r="AL70" s="18"/>
-      <c r="AM70" s="18"/>
+      <c r="Z70" s="14"/>
+      <c r="AA70" s="14"/>
+      <c r="AB70" s="14"/>
+      <c r="AC70" s="14"/>
+      <c r="AD70" s="14"/>
+      <c r="AE70" s="14"/>
+      <c r="AF70" s="14"/>
+      <c r="AG70" s="14"/>
+      <c r="AH70" s="14"/>
+      <c r="AI70" s="14"/>
+      <c r="AJ70" s="14"/>
+      <c r="AK70" s="14"/>
+      <c r="AL70" s="14"/>
+      <c r="AM70" s="14"/>
       <c r="AN70" s="17" t="s">
         <v>16</v>
       </c>
@@ -8923,45 +8771,45 @@
       <c r="BG70" s="17"/>
       <c r="BH70" s="17"/>
       <c r="BI70" s="17"/>
-      <c r="BJ70" s="18" t="s">
+      <c r="BJ70" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="BK70" s="18"/>
-      <c r="BL70" s="18"/>
-      <c r="BM70" s="18"/>
-      <c r="BN70" s="18"/>
-      <c r="BO70" s="18"/>
-      <c r="BP70" s="18"/>
-      <c r="BQ70" s="18"/>
-      <c r="BR70" s="18"/>
-      <c r="BS70" s="18"/>
-      <c r="BT70" s="18"/>
-      <c r="BU70" s="18"/>
-      <c r="BV70" s="18"/>
-      <c r="BW70" s="18"/>
-      <c r="BX70" s="18"/>
-      <c r="BY70" s="18"/>
-      <c r="BZ70" s="18"/>
-      <c r="CA70" s="18"/>
-      <c r="CB70" s="18"/>
-      <c r="CC70" s="18"/>
-      <c r="CD70" s="18"/>
-      <c r="CE70" s="18"/>
-      <c r="CF70" s="18"/>
-      <c r="CG70" s="18"/>
-      <c r="CH70" s="18"/>
-      <c r="CI70" s="18"/>
-      <c r="CJ70" s="18"/>
-      <c r="CK70" s="18"/>
-      <c r="CL70" s="18"/>
-      <c r="CM70" s="18"/>
-      <c r="CN70" s="18"/>
-      <c r="CO70" s="18"/>
-      <c r="CP70" s="18"/>
-      <c r="CQ70" s="18"/>
-      <c r="CR70" s="18"/>
-      <c r="CS70" s="18"/>
-      <c r="CT70" s="19"/>
+      <c r="BK70" s="14"/>
+      <c r="BL70" s="14"/>
+      <c r="BM70" s="14"/>
+      <c r="BN70" s="14"/>
+      <c r="BO70" s="14"/>
+      <c r="BP70" s="14"/>
+      <c r="BQ70" s="14"/>
+      <c r="BR70" s="14"/>
+      <c r="BS70" s="14"/>
+      <c r="BT70" s="14"/>
+      <c r="BU70" s="14"/>
+      <c r="BV70" s="14"/>
+      <c r="BW70" s="14"/>
+      <c r="BX70" s="14"/>
+      <c r="BY70" s="14"/>
+      <c r="BZ70" s="14"/>
+      <c r="CA70" s="14"/>
+      <c r="CB70" s="14"/>
+      <c r="CC70" s="14"/>
+      <c r="CD70" s="14"/>
+      <c r="CE70" s="14"/>
+      <c r="CF70" s="14"/>
+      <c r="CG70" s="14"/>
+      <c r="CH70" s="14"/>
+      <c r="CI70" s="14"/>
+      <c r="CJ70" s="14"/>
+      <c r="CK70" s="14"/>
+      <c r="CL70" s="14"/>
+      <c r="CM70" s="14"/>
+      <c r="CN70" s="14"/>
+      <c r="CO70" s="14"/>
+      <c r="CP70" s="14"/>
+      <c r="CQ70" s="14"/>
+      <c r="CR70" s="14"/>
+      <c r="CS70" s="14"/>
+      <c r="CT70" s="15"/>
     </row>
     <row r="71" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C71" s="16">
@@ -8970,43 +8818,43 @@
       <c r="D71" s="17"/>
       <c r="E71" s="17"/>
       <c r="F71" s="17"/>
-      <c r="G71" s="18" t="s">
+      <c r="G71" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H71" s="18"/>
-      <c r="I71" s="18"/>
-      <c r="J71" s="18"/>
-      <c r="K71" s="18"/>
-      <c r="L71" s="18"/>
-      <c r="M71" s="18"/>
-      <c r="N71" s="18"/>
-      <c r="O71" s="18"/>
-      <c r="P71" s="18"/>
-      <c r="Q71" s="18"/>
-      <c r="R71" s="18"/>
-      <c r="S71" s="18"/>
-      <c r="T71" s="18"/>
-      <c r="U71" s="18"/>
-      <c r="V71" s="18"/>
-      <c r="W71" s="18"/>
-      <c r="X71" s="18"/>
-      <c r="Y71" s="18" t="s">
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
+      <c r="K71" s="14"/>
+      <c r="L71" s="14"/>
+      <c r="M71" s="14"/>
+      <c r="N71" s="14"/>
+      <c r="O71" s="14"/>
+      <c r="P71" s="14"/>
+      <c r="Q71" s="14"/>
+      <c r="R71" s="14"/>
+      <c r="S71" s="14"/>
+      <c r="T71" s="14"/>
+      <c r="U71" s="14"/>
+      <c r="V71" s="14"/>
+      <c r="W71" s="14"/>
+      <c r="X71" s="14"/>
+      <c r="Y71" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="Z71" s="18"/>
-      <c r="AA71" s="18"/>
-      <c r="AB71" s="18"/>
-      <c r="AC71" s="18"/>
-      <c r="AD71" s="18"/>
-      <c r="AE71" s="18"/>
-      <c r="AF71" s="18"/>
-      <c r="AG71" s="18"/>
-      <c r="AH71" s="18"/>
-      <c r="AI71" s="18"/>
-      <c r="AJ71" s="18"/>
-      <c r="AK71" s="18"/>
-      <c r="AL71" s="18"/>
-      <c r="AM71" s="18"/>
+      <c r="Z71" s="14"/>
+      <c r="AA71" s="14"/>
+      <c r="AB71" s="14"/>
+      <c r="AC71" s="14"/>
+      <c r="AD71" s="14"/>
+      <c r="AE71" s="14"/>
+      <c r="AF71" s="14"/>
+      <c r="AG71" s="14"/>
+      <c r="AH71" s="14"/>
+      <c r="AI71" s="14"/>
+      <c r="AJ71" s="14"/>
+      <c r="AK71" s="14"/>
+      <c r="AL71" s="14"/>
+      <c r="AM71" s="14"/>
       <c r="AN71" s="17" t="s">
         <v>16</v>
       </c>
@@ -9031,45 +8879,45 @@
       <c r="BG71" s="17"/>
       <c r="BH71" s="17"/>
       <c r="BI71" s="17"/>
-      <c r="BJ71" s="18" t="s">
+      <c r="BJ71" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="BK71" s="18"/>
-      <c r="BL71" s="18"/>
-      <c r="BM71" s="18"/>
-      <c r="BN71" s="18"/>
-      <c r="BO71" s="18"/>
-      <c r="BP71" s="18"/>
-      <c r="BQ71" s="18"/>
-      <c r="BR71" s="18"/>
-      <c r="BS71" s="18"/>
-      <c r="BT71" s="18"/>
-      <c r="BU71" s="18"/>
-      <c r="BV71" s="18"/>
-      <c r="BW71" s="18"/>
-      <c r="BX71" s="18"/>
-      <c r="BY71" s="18"/>
-      <c r="BZ71" s="18"/>
-      <c r="CA71" s="18"/>
-      <c r="CB71" s="18"/>
-      <c r="CC71" s="18"/>
-      <c r="CD71" s="18"/>
-      <c r="CE71" s="18"/>
-      <c r="CF71" s="18"/>
-      <c r="CG71" s="18"/>
-      <c r="CH71" s="18"/>
-      <c r="CI71" s="18"/>
-      <c r="CJ71" s="18"/>
-      <c r="CK71" s="18"/>
-      <c r="CL71" s="18"/>
-      <c r="CM71" s="18"/>
-      <c r="CN71" s="18"/>
-      <c r="CO71" s="18"/>
-      <c r="CP71" s="18"/>
-      <c r="CQ71" s="18"/>
-      <c r="CR71" s="18"/>
-      <c r="CS71" s="18"/>
-      <c r="CT71" s="19"/>
+      <c r="BK71" s="14"/>
+      <c r="BL71" s="14"/>
+      <c r="BM71" s="14"/>
+      <c r="BN71" s="14"/>
+      <c r="BO71" s="14"/>
+      <c r="BP71" s="14"/>
+      <c r="BQ71" s="14"/>
+      <c r="BR71" s="14"/>
+      <c r="BS71" s="14"/>
+      <c r="BT71" s="14"/>
+      <c r="BU71" s="14"/>
+      <c r="BV71" s="14"/>
+      <c r="BW71" s="14"/>
+      <c r="BX71" s="14"/>
+      <c r="BY71" s="14"/>
+      <c r="BZ71" s="14"/>
+      <c r="CA71" s="14"/>
+      <c r="CB71" s="14"/>
+      <c r="CC71" s="14"/>
+      <c r="CD71" s="14"/>
+      <c r="CE71" s="14"/>
+      <c r="CF71" s="14"/>
+      <c r="CG71" s="14"/>
+      <c r="CH71" s="14"/>
+      <c r="CI71" s="14"/>
+      <c r="CJ71" s="14"/>
+      <c r="CK71" s="14"/>
+      <c r="CL71" s="14"/>
+      <c r="CM71" s="14"/>
+      <c r="CN71" s="14"/>
+      <c r="CO71" s="14"/>
+      <c r="CP71" s="14"/>
+      <c r="CQ71" s="14"/>
+      <c r="CR71" s="14"/>
+      <c r="CS71" s="14"/>
+      <c r="CT71" s="15"/>
     </row>
     <row r="72" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C72" s="16">
@@ -9078,43 +8926,43 @@
       <c r="D72" s="17"/>
       <c r="E72" s="17"/>
       <c r="F72" s="17"/>
-      <c r="G72" s="18" t="s">
+      <c r="G72" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H72" s="18"/>
-      <c r="I72" s="18"/>
-      <c r="J72" s="18"/>
-      <c r="K72" s="18"/>
-      <c r="L72" s="18"/>
-      <c r="M72" s="18"/>
-      <c r="N72" s="18"/>
-      <c r="O72" s="18"/>
-      <c r="P72" s="18"/>
-      <c r="Q72" s="18"/>
-      <c r="R72" s="18"/>
-      <c r="S72" s="18"/>
-      <c r="T72" s="18"/>
-      <c r="U72" s="18"/>
-      <c r="V72" s="18"/>
-      <c r="W72" s="18"/>
-      <c r="X72" s="18"/>
-      <c r="Y72" s="18" t="s">
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+      <c r="K72" s="14"/>
+      <c r="L72" s="14"/>
+      <c r="M72" s="14"/>
+      <c r="N72" s="14"/>
+      <c r="O72" s="14"/>
+      <c r="P72" s="14"/>
+      <c r="Q72" s="14"/>
+      <c r="R72" s="14"/>
+      <c r="S72" s="14"/>
+      <c r="T72" s="14"/>
+      <c r="U72" s="14"/>
+      <c r="V72" s="14"/>
+      <c r="W72" s="14"/>
+      <c r="X72" s="14"/>
+      <c r="Y72" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="Z72" s="18"/>
-      <c r="AA72" s="18"/>
-      <c r="AB72" s="18"/>
-      <c r="AC72" s="18"/>
-      <c r="AD72" s="18"/>
-      <c r="AE72" s="18"/>
-      <c r="AF72" s="18"/>
-      <c r="AG72" s="18"/>
-      <c r="AH72" s="18"/>
-      <c r="AI72" s="18"/>
-      <c r="AJ72" s="18"/>
-      <c r="AK72" s="18"/>
-      <c r="AL72" s="18"/>
-      <c r="AM72" s="18"/>
+      <c r="Z72" s="14"/>
+      <c r="AA72" s="14"/>
+      <c r="AB72" s="14"/>
+      <c r="AC72" s="14"/>
+      <c r="AD72" s="14"/>
+      <c r="AE72" s="14"/>
+      <c r="AF72" s="14"/>
+      <c r="AG72" s="14"/>
+      <c r="AH72" s="14"/>
+      <c r="AI72" s="14"/>
+      <c r="AJ72" s="14"/>
+      <c r="AK72" s="14"/>
+      <c r="AL72" s="14"/>
+      <c r="AM72" s="14"/>
       <c r="AN72" s="17" t="s">
         <v>19</v>
       </c>
@@ -9139,45 +8987,45 @@
       <c r="BG72" s="17"/>
       <c r="BH72" s="17"/>
       <c r="BI72" s="17"/>
-      <c r="BJ72" s="18" t="s">
+      <c r="BJ72" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="BK72" s="18"/>
-      <c r="BL72" s="18"/>
-      <c r="BM72" s="18"/>
-      <c r="BN72" s="18"/>
-      <c r="BO72" s="18"/>
-      <c r="BP72" s="18"/>
-      <c r="BQ72" s="18"/>
-      <c r="BR72" s="18"/>
-      <c r="BS72" s="18"/>
-      <c r="BT72" s="18"/>
-      <c r="BU72" s="18"/>
-      <c r="BV72" s="18"/>
-      <c r="BW72" s="18"/>
-      <c r="BX72" s="18"/>
-      <c r="BY72" s="18"/>
-      <c r="BZ72" s="18"/>
-      <c r="CA72" s="18"/>
-      <c r="CB72" s="18"/>
-      <c r="CC72" s="18"/>
-      <c r="CD72" s="18"/>
-      <c r="CE72" s="18"/>
-      <c r="CF72" s="18"/>
-      <c r="CG72" s="18"/>
-      <c r="CH72" s="18"/>
-      <c r="CI72" s="18"/>
-      <c r="CJ72" s="18"/>
-      <c r="CK72" s="18"/>
-      <c r="CL72" s="18"/>
-      <c r="CM72" s="18"/>
-      <c r="CN72" s="18"/>
-      <c r="CO72" s="18"/>
-      <c r="CP72" s="18"/>
-      <c r="CQ72" s="18"/>
-      <c r="CR72" s="18"/>
-      <c r="CS72" s="18"/>
-      <c r="CT72" s="19"/>
+      <c r="BK72" s="14"/>
+      <c r="BL72" s="14"/>
+      <c r="BM72" s="14"/>
+      <c r="BN72" s="14"/>
+      <c r="BO72" s="14"/>
+      <c r="BP72" s="14"/>
+      <c r="BQ72" s="14"/>
+      <c r="BR72" s="14"/>
+      <c r="BS72" s="14"/>
+      <c r="BT72" s="14"/>
+      <c r="BU72" s="14"/>
+      <c r="BV72" s="14"/>
+      <c r="BW72" s="14"/>
+      <c r="BX72" s="14"/>
+      <c r="BY72" s="14"/>
+      <c r="BZ72" s="14"/>
+      <c r="CA72" s="14"/>
+      <c r="CB72" s="14"/>
+      <c r="CC72" s="14"/>
+      <c r="CD72" s="14"/>
+      <c r="CE72" s="14"/>
+      <c r="CF72" s="14"/>
+      <c r="CG72" s="14"/>
+      <c r="CH72" s="14"/>
+      <c r="CI72" s="14"/>
+      <c r="CJ72" s="14"/>
+      <c r="CK72" s="14"/>
+      <c r="CL72" s="14"/>
+      <c r="CM72" s="14"/>
+      <c r="CN72" s="14"/>
+      <c r="CO72" s="14"/>
+      <c r="CP72" s="14"/>
+      <c r="CQ72" s="14"/>
+      <c r="CR72" s="14"/>
+      <c r="CS72" s="14"/>
+      <c r="CT72" s="15"/>
     </row>
     <row r="73" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C73" s="16">
@@ -9186,43 +9034,43 @@
       <c r="D73" s="17"/>
       <c r="E73" s="17"/>
       <c r="F73" s="17"/>
-      <c r="G73" s="18" t="s">
+      <c r="G73" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H73" s="18"/>
-      <c r="I73" s="18"/>
-      <c r="J73" s="18"/>
-      <c r="K73" s="18"/>
-      <c r="L73" s="18"/>
-      <c r="M73" s="18"/>
-      <c r="N73" s="18"/>
-      <c r="O73" s="18"/>
-      <c r="P73" s="18"/>
-      <c r="Q73" s="18"/>
-      <c r="R73" s="18"/>
-      <c r="S73" s="18"/>
-      <c r="T73" s="18"/>
-      <c r="U73" s="18"/>
-      <c r="V73" s="18"/>
-      <c r="W73" s="18"/>
-      <c r="X73" s="18"/>
-      <c r="Y73" s="18" t="s">
+      <c r="H73" s="14"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="14"/>
+      <c r="L73" s="14"/>
+      <c r="M73" s="14"/>
+      <c r="N73" s="14"/>
+      <c r="O73" s="14"/>
+      <c r="P73" s="14"/>
+      <c r="Q73" s="14"/>
+      <c r="R73" s="14"/>
+      <c r="S73" s="14"/>
+      <c r="T73" s="14"/>
+      <c r="U73" s="14"/>
+      <c r="V73" s="14"/>
+      <c r="W73" s="14"/>
+      <c r="X73" s="14"/>
+      <c r="Y73" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="Z73" s="18"/>
-      <c r="AA73" s="18"/>
-      <c r="AB73" s="18"/>
-      <c r="AC73" s="18"/>
-      <c r="AD73" s="18"/>
-      <c r="AE73" s="18"/>
-      <c r="AF73" s="18"/>
-      <c r="AG73" s="18"/>
-      <c r="AH73" s="18"/>
-      <c r="AI73" s="18"/>
-      <c r="AJ73" s="18"/>
-      <c r="AK73" s="18"/>
-      <c r="AL73" s="18"/>
-      <c r="AM73" s="18"/>
+      <c r="Z73" s="14"/>
+      <c r="AA73" s="14"/>
+      <c r="AB73" s="14"/>
+      <c r="AC73" s="14"/>
+      <c r="AD73" s="14"/>
+      <c r="AE73" s="14"/>
+      <c r="AF73" s="14"/>
+      <c r="AG73" s="14"/>
+      <c r="AH73" s="14"/>
+      <c r="AI73" s="14"/>
+      <c r="AJ73" s="14"/>
+      <c r="AK73" s="14"/>
+      <c r="AL73" s="14"/>
+      <c r="AM73" s="14"/>
       <c r="AN73" s="17" t="s">
         <v>21</v>
       </c>
@@ -9247,45 +9095,45 @@
       <c r="BG73" s="17"/>
       <c r="BH73" s="17"/>
       <c r="BI73" s="17"/>
-      <c r="BJ73" s="18" t="s">
+      <c r="BJ73" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="BK73" s="18"/>
-      <c r="BL73" s="18"/>
-      <c r="BM73" s="18"/>
-      <c r="BN73" s="18"/>
-      <c r="BO73" s="18"/>
-      <c r="BP73" s="18"/>
-      <c r="BQ73" s="18"/>
-      <c r="BR73" s="18"/>
-      <c r="BS73" s="18"/>
-      <c r="BT73" s="18"/>
-      <c r="BU73" s="18"/>
-      <c r="BV73" s="18"/>
-      <c r="BW73" s="18"/>
-      <c r="BX73" s="18"/>
-      <c r="BY73" s="18"/>
-      <c r="BZ73" s="18"/>
-      <c r="CA73" s="18"/>
-      <c r="CB73" s="18"/>
-      <c r="CC73" s="18"/>
-      <c r="CD73" s="18"/>
-      <c r="CE73" s="18"/>
-      <c r="CF73" s="18"/>
-      <c r="CG73" s="18"/>
-      <c r="CH73" s="18"/>
-      <c r="CI73" s="18"/>
-      <c r="CJ73" s="18"/>
-      <c r="CK73" s="18"/>
-      <c r="CL73" s="18"/>
-      <c r="CM73" s="18"/>
-      <c r="CN73" s="18"/>
-      <c r="CO73" s="18"/>
-      <c r="CP73" s="18"/>
-      <c r="CQ73" s="18"/>
-      <c r="CR73" s="18"/>
-      <c r="CS73" s="18"/>
-      <c r="CT73" s="19"/>
+      <c r="BK73" s="14"/>
+      <c r="BL73" s="14"/>
+      <c r="BM73" s="14"/>
+      <c r="BN73" s="14"/>
+      <c r="BO73" s="14"/>
+      <c r="BP73" s="14"/>
+      <c r="BQ73" s="14"/>
+      <c r="BR73" s="14"/>
+      <c r="BS73" s="14"/>
+      <c r="BT73" s="14"/>
+      <c r="BU73" s="14"/>
+      <c r="BV73" s="14"/>
+      <c r="BW73" s="14"/>
+      <c r="BX73" s="14"/>
+      <c r="BY73" s="14"/>
+      <c r="BZ73" s="14"/>
+      <c r="CA73" s="14"/>
+      <c r="CB73" s="14"/>
+      <c r="CC73" s="14"/>
+      <c r="CD73" s="14"/>
+      <c r="CE73" s="14"/>
+      <c r="CF73" s="14"/>
+      <c r="CG73" s="14"/>
+      <c r="CH73" s="14"/>
+      <c r="CI73" s="14"/>
+      <c r="CJ73" s="14"/>
+      <c r="CK73" s="14"/>
+      <c r="CL73" s="14"/>
+      <c r="CM73" s="14"/>
+      <c r="CN73" s="14"/>
+      <c r="CO73" s="14"/>
+      <c r="CP73" s="14"/>
+      <c r="CQ73" s="14"/>
+      <c r="CR73" s="14"/>
+      <c r="CS73" s="14"/>
+      <c r="CT73" s="15"/>
     </row>
     <row r="74" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C74" s="16">
@@ -9294,43 +9142,43 @@
       <c r="D74" s="17"/>
       <c r="E74" s="17"/>
       <c r="F74" s="17"/>
-      <c r="G74" s="18" t="s">
+      <c r="G74" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
-      <c r="J74" s="18"/>
-      <c r="K74" s="18"/>
-      <c r="L74" s="18"/>
-      <c r="M74" s="18"/>
-      <c r="N74" s="18"/>
-      <c r="O74" s="18"/>
-      <c r="P74" s="18"/>
-      <c r="Q74" s="18"/>
-      <c r="R74" s="18"/>
-      <c r="S74" s="18"/>
-      <c r="T74" s="18"/>
-      <c r="U74" s="18"/>
-      <c r="V74" s="18"/>
-      <c r="W74" s="18"/>
-      <c r="X74" s="18"/>
-      <c r="Y74" s="18" t="s">
+      <c r="H74" s="14"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="14"/>
+      <c r="K74" s="14"/>
+      <c r="L74" s="14"/>
+      <c r="M74" s="14"/>
+      <c r="N74" s="14"/>
+      <c r="O74" s="14"/>
+      <c r="P74" s="14"/>
+      <c r="Q74" s="14"/>
+      <c r="R74" s="14"/>
+      <c r="S74" s="14"/>
+      <c r="T74" s="14"/>
+      <c r="U74" s="14"/>
+      <c r="V74" s="14"/>
+      <c r="W74" s="14"/>
+      <c r="X74" s="14"/>
+      <c r="Y74" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="Z74" s="18"/>
-      <c r="AA74" s="18"/>
-      <c r="AB74" s="18"/>
-      <c r="AC74" s="18"/>
-      <c r="AD74" s="18"/>
-      <c r="AE74" s="18"/>
-      <c r="AF74" s="18"/>
-      <c r="AG74" s="18"/>
-      <c r="AH74" s="18"/>
-      <c r="AI74" s="18"/>
-      <c r="AJ74" s="18"/>
-      <c r="AK74" s="18"/>
-      <c r="AL74" s="18"/>
-      <c r="AM74" s="18"/>
+      <c r="Z74" s="14"/>
+      <c r="AA74" s="14"/>
+      <c r="AB74" s="14"/>
+      <c r="AC74" s="14"/>
+      <c r="AD74" s="14"/>
+      <c r="AE74" s="14"/>
+      <c r="AF74" s="14"/>
+      <c r="AG74" s="14"/>
+      <c r="AH74" s="14"/>
+      <c r="AI74" s="14"/>
+      <c r="AJ74" s="14"/>
+      <c r="AK74" s="14"/>
+      <c r="AL74" s="14"/>
+      <c r="AM74" s="14"/>
       <c r="AN74" s="17" t="s">
         <v>23</v>
       </c>
@@ -9355,45 +9203,45 @@
       <c r="BG74" s="17"/>
       <c r="BH74" s="17"/>
       <c r="BI74" s="17"/>
-      <c r="BJ74" s="18" t="s">
+      <c r="BJ74" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="BK74" s="18"/>
-      <c r="BL74" s="18"/>
-      <c r="BM74" s="18"/>
-      <c r="BN74" s="18"/>
-      <c r="BO74" s="18"/>
-      <c r="BP74" s="18"/>
-      <c r="BQ74" s="18"/>
-      <c r="BR74" s="18"/>
-      <c r="BS74" s="18"/>
-      <c r="BT74" s="18"/>
-      <c r="BU74" s="18"/>
-      <c r="BV74" s="18"/>
-      <c r="BW74" s="18"/>
-      <c r="BX74" s="18"/>
-      <c r="BY74" s="18"/>
-      <c r="BZ74" s="18"/>
-      <c r="CA74" s="18"/>
-      <c r="CB74" s="18"/>
-      <c r="CC74" s="18"/>
-      <c r="CD74" s="18"/>
-      <c r="CE74" s="18"/>
-      <c r="CF74" s="18"/>
-      <c r="CG74" s="18"/>
-      <c r="CH74" s="18"/>
-      <c r="CI74" s="18"/>
-      <c r="CJ74" s="18"/>
-      <c r="CK74" s="18"/>
-      <c r="CL74" s="18"/>
-      <c r="CM74" s="18"/>
-      <c r="CN74" s="18"/>
-      <c r="CO74" s="18"/>
-      <c r="CP74" s="18"/>
-      <c r="CQ74" s="18"/>
-      <c r="CR74" s="18"/>
-      <c r="CS74" s="18"/>
-      <c r="CT74" s="19"/>
+      <c r="BK74" s="14"/>
+      <c r="BL74" s="14"/>
+      <c r="BM74" s="14"/>
+      <c r="BN74" s="14"/>
+      <c r="BO74" s="14"/>
+      <c r="BP74" s="14"/>
+      <c r="BQ74" s="14"/>
+      <c r="BR74" s="14"/>
+      <c r="BS74" s="14"/>
+      <c r="BT74" s="14"/>
+      <c r="BU74" s="14"/>
+      <c r="BV74" s="14"/>
+      <c r="BW74" s="14"/>
+      <c r="BX74" s="14"/>
+      <c r="BY74" s="14"/>
+      <c r="BZ74" s="14"/>
+      <c r="CA74" s="14"/>
+      <c r="CB74" s="14"/>
+      <c r="CC74" s="14"/>
+      <c r="CD74" s="14"/>
+      <c r="CE74" s="14"/>
+      <c r="CF74" s="14"/>
+      <c r="CG74" s="14"/>
+      <c r="CH74" s="14"/>
+      <c r="CI74" s="14"/>
+      <c r="CJ74" s="14"/>
+      <c r="CK74" s="14"/>
+      <c r="CL74" s="14"/>
+      <c r="CM74" s="14"/>
+      <c r="CN74" s="14"/>
+      <c r="CO74" s="14"/>
+      <c r="CP74" s="14"/>
+      <c r="CQ74" s="14"/>
+      <c r="CR74" s="14"/>
+      <c r="CS74" s="14"/>
+      <c r="CT74" s="15"/>
     </row>
     <row r="75" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C75" s="16">
@@ -9402,43 +9250,43 @@
       <c r="D75" s="17"/>
       <c r="E75" s="17"/>
       <c r="F75" s="17"/>
-      <c r="G75" s="18" t="s">
+      <c r="G75" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="H75" s="18"/>
-      <c r="I75" s="18"/>
-      <c r="J75" s="18"/>
-      <c r="K75" s="18"/>
-      <c r="L75" s="18"/>
-      <c r="M75" s="18"/>
-      <c r="N75" s="18"/>
-      <c r="O75" s="18"/>
-      <c r="P75" s="18"/>
-      <c r="Q75" s="18"/>
-      <c r="R75" s="18"/>
-      <c r="S75" s="18"/>
-      <c r="T75" s="18"/>
-      <c r="U75" s="18"/>
-      <c r="V75" s="18"/>
-      <c r="W75" s="18"/>
-      <c r="X75" s="18"/>
-      <c r="Y75" s="18" t="s">
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="14"/>
+      <c r="K75" s="14"/>
+      <c r="L75" s="14"/>
+      <c r="M75" s="14"/>
+      <c r="N75" s="14"/>
+      <c r="O75" s="14"/>
+      <c r="P75" s="14"/>
+      <c r="Q75" s="14"/>
+      <c r="R75" s="14"/>
+      <c r="S75" s="14"/>
+      <c r="T75" s="14"/>
+      <c r="U75" s="14"/>
+      <c r="V75" s="14"/>
+      <c r="W75" s="14"/>
+      <c r="X75" s="14"/>
+      <c r="Y75" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="Z75" s="18"/>
-      <c r="AA75" s="18"/>
-      <c r="AB75" s="18"/>
-      <c r="AC75" s="18"/>
-      <c r="AD75" s="18"/>
-      <c r="AE75" s="18"/>
-      <c r="AF75" s="18"/>
-      <c r="AG75" s="18"/>
-      <c r="AH75" s="18"/>
-      <c r="AI75" s="18"/>
-      <c r="AJ75" s="18"/>
-      <c r="AK75" s="18"/>
-      <c r="AL75" s="18"/>
-      <c r="AM75" s="18"/>
+      <c r="Z75" s="14"/>
+      <c r="AA75" s="14"/>
+      <c r="AB75" s="14"/>
+      <c r="AC75" s="14"/>
+      <c r="AD75" s="14"/>
+      <c r="AE75" s="14"/>
+      <c r="AF75" s="14"/>
+      <c r="AG75" s="14"/>
+      <c r="AH75" s="14"/>
+      <c r="AI75" s="14"/>
+      <c r="AJ75" s="14"/>
+      <c r="AK75" s="14"/>
+      <c r="AL75" s="14"/>
+      <c r="AM75" s="14"/>
       <c r="AN75" s="17" t="s">
         <v>13</v>
       </c>
@@ -9463,43 +9311,43 @@
       <c r="BG75" s="17"/>
       <c r="BH75" s="17"/>
       <c r="BI75" s="17"/>
-      <c r="BJ75" s="18"/>
-      <c r="BK75" s="18"/>
-      <c r="BL75" s="18"/>
-      <c r="BM75" s="18"/>
-      <c r="BN75" s="18"/>
-      <c r="BO75" s="18"/>
-      <c r="BP75" s="18"/>
-      <c r="BQ75" s="18"/>
-      <c r="BR75" s="18"/>
-      <c r="BS75" s="18"/>
-      <c r="BT75" s="18"/>
-      <c r="BU75" s="18"/>
-      <c r="BV75" s="18"/>
-      <c r="BW75" s="18"/>
-      <c r="BX75" s="18"/>
-      <c r="BY75" s="18"/>
-      <c r="BZ75" s="18"/>
-      <c r="CA75" s="18"/>
-      <c r="CB75" s="18"/>
-      <c r="CC75" s="18"/>
-      <c r="CD75" s="18"/>
-      <c r="CE75" s="18"/>
-      <c r="CF75" s="18"/>
-      <c r="CG75" s="18"/>
-      <c r="CH75" s="18"/>
-      <c r="CI75" s="18"/>
-      <c r="CJ75" s="18"/>
-      <c r="CK75" s="18"/>
-      <c r="CL75" s="18"/>
-      <c r="CM75" s="18"/>
-      <c r="CN75" s="18"/>
-      <c r="CO75" s="18"/>
-      <c r="CP75" s="18"/>
-      <c r="CQ75" s="18"/>
-      <c r="CR75" s="18"/>
-      <c r="CS75" s="18"/>
-      <c r="CT75" s="19"/>
+      <c r="BJ75" s="14"/>
+      <c r="BK75" s="14"/>
+      <c r="BL75" s="14"/>
+      <c r="BM75" s="14"/>
+      <c r="BN75" s="14"/>
+      <c r="BO75" s="14"/>
+      <c r="BP75" s="14"/>
+      <c r="BQ75" s="14"/>
+      <c r="BR75" s="14"/>
+      <c r="BS75" s="14"/>
+      <c r="BT75" s="14"/>
+      <c r="BU75" s="14"/>
+      <c r="BV75" s="14"/>
+      <c r="BW75" s="14"/>
+      <c r="BX75" s="14"/>
+      <c r="BY75" s="14"/>
+      <c r="BZ75" s="14"/>
+      <c r="CA75" s="14"/>
+      <c r="CB75" s="14"/>
+      <c r="CC75" s="14"/>
+      <c r="CD75" s="14"/>
+      <c r="CE75" s="14"/>
+      <c r="CF75" s="14"/>
+      <c r="CG75" s="14"/>
+      <c r="CH75" s="14"/>
+      <c r="CI75" s="14"/>
+      <c r="CJ75" s="14"/>
+      <c r="CK75" s="14"/>
+      <c r="CL75" s="14"/>
+      <c r="CM75" s="14"/>
+      <c r="CN75" s="14"/>
+      <c r="CO75" s="14"/>
+      <c r="CP75" s="14"/>
+      <c r="CQ75" s="14"/>
+      <c r="CR75" s="14"/>
+      <c r="CS75" s="14"/>
+      <c r="CT75" s="15"/>
     </row>
     <row r="76" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C76" s="16">
@@ -9508,43 +9356,43 @@
       <c r="D76" s="17"/>
       <c r="E76" s="17"/>
       <c r="F76" s="17"/>
-      <c r="G76" s="18" t="s">
+      <c r="G76" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H76" s="18"/>
-      <c r="I76" s="18"/>
-      <c r="J76" s="18"/>
-      <c r="K76" s="18"/>
-      <c r="L76" s="18"/>
-      <c r="M76" s="18"/>
-      <c r="N76" s="18"/>
-      <c r="O76" s="18"/>
-      <c r="P76" s="18"/>
-      <c r="Q76" s="18"/>
-      <c r="R76" s="18"/>
-      <c r="S76" s="18"/>
-      <c r="T76" s="18"/>
-      <c r="U76" s="18"/>
-      <c r="V76" s="18"/>
-      <c r="W76" s="18"/>
-      <c r="X76" s="18"/>
-      <c r="Y76" s="18" t="s">
+      <c r="H76" s="14"/>
+      <c r="I76" s="14"/>
+      <c r="J76" s="14"/>
+      <c r="K76" s="14"/>
+      <c r="L76" s="14"/>
+      <c r="M76" s="14"/>
+      <c r="N76" s="14"/>
+      <c r="O76" s="14"/>
+      <c r="P76" s="14"/>
+      <c r="Q76" s="14"/>
+      <c r="R76" s="14"/>
+      <c r="S76" s="14"/>
+      <c r="T76" s="14"/>
+      <c r="U76" s="14"/>
+      <c r="V76" s="14"/>
+      <c r="W76" s="14"/>
+      <c r="X76" s="14"/>
+      <c r="Y76" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="Z76" s="18"/>
-      <c r="AA76" s="18"/>
-      <c r="AB76" s="18"/>
-      <c r="AC76" s="18"/>
-      <c r="AD76" s="18"/>
-      <c r="AE76" s="18"/>
-      <c r="AF76" s="18"/>
-      <c r="AG76" s="18"/>
-      <c r="AH76" s="18"/>
-      <c r="AI76" s="18"/>
-      <c r="AJ76" s="18"/>
-      <c r="AK76" s="18"/>
-      <c r="AL76" s="18"/>
-      <c r="AM76" s="18"/>
+      <c r="Z76" s="14"/>
+      <c r="AA76" s="14"/>
+      <c r="AB76" s="14"/>
+      <c r="AC76" s="14"/>
+      <c r="AD76" s="14"/>
+      <c r="AE76" s="14"/>
+      <c r="AF76" s="14"/>
+      <c r="AG76" s="14"/>
+      <c r="AH76" s="14"/>
+      <c r="AI76" s="14"/>
+      <c r="AJ76" s="14"/>
+      <c r="AK76" s="14"/>
+      <c r="AL76" s="14"/>
+      <c r="AM76" s="14"/>
       <c r="AN76" s="17" t="s">
         <v>13</v>
       </c>
@@ -9569,43 +9417,43 @@
       <c r="BG76" s="17"/>
       <c r="BH76" s="17"/>
       <c r="BI76" s="17"/>
-      <c r="BJ76" s="18"/>
-      <c r="BK76" s="18"/>
-      <c r="BL76" s="18"/>
-      <c r="BM76" s="18"/>
-      <c r="BN76" s="18"/>
-      <c r="BO76" s="18"/>
-      <c r="BP76" s="18"/>
-      <c r="BQ76" s="18"/>
-      <c r="BR76" s="18"/>
-      <c r="BS76" s="18"/>
-      <c r="BT76" s="18"/>
-      <c r="BU76" s="18"/>
-      <c r="BV76" s="18"/>
-      <c r="BW76" s="18"/>
-      <c r="BX76" s="18"/>
-      <c r="BY76" s="18"/>
-      <c r="BZ76" s="18"/>
-      <c r="CA76" s="18"/>
-      <c r="CB76" s="18"/>
-      <c r="CC76" s="18"/>
-      <c r="CD76" s="18"/>
-      <c r="CE76" s="18"/>
-      <c r="CF76" s="18"/>
-      <c r="CG76" s="18"/>
-      <c r="CH76" s="18"/>
-      <c r="CI76" s="18"/>
-      <c r="CJ76" s="18"/>
-      <c r="CK76" s="18"/>
-      <c r="CL76" s="18"/>
-      <c r="CM76" s="18"/>
-      <c r="CN76" s="18"/>
-      <c r="CO76" s="18"/>
-      <c r="CP76" s="18"/>
-      <c r="CQ76" s="18"/>
-      <c r="CR76" s="18"/>
-      <c r="CS76" s="18"/>
-      <c r="CT76" s="19"/>
+      <c r="BJ76" s="14"/>
+      <c r="BK76" s="14"/>
+      <c r="BL76" s="14"/>
+      <c r="BM76" s="14"/>
+      <c r="BN76" s="14"/>
+      <c r="BO76" s="14"/>
+      <c r="BP76" s="14"/>
+      <c r="BQ76" s="14"/>
+      <c r="BR76" s="14"/>
+      <c r="BS76" s="14"/>
+      <c r="BT76" s="14"/>
+      <c r="BU76" s="14"/>
+      <c r="BV76" s="14"/>
+      <c r="BW76" s="14"/>
+      <c r="BX76" s="14"/>
+      <c r="BY76" s="14"/>
+      <c r="BZ76" s="14"/>
+      <c r="CA76" s="14"/>
+      <c r="CB76" s="14"/>
+      <c r="CC76" s="14"/>
+      <c r="CD76" s="14"/>
+      <c r="CE76" s="14"/>
+      <c r="CF76" s="14"/>
+      <c r="CG76" s="14"/>
+      <c r="CH76" s="14"/>
+      <c r="CI76" s="14"/>
+      <c r="CJ76" s="14"/>
+      <c r="CK76" s="14"/>
+      <c r="CL76" s="14"/>
+      <c r="CM76" s="14"/>
+      <c r="CN76" s="14"/>
+      <c r="CO76" s="14"/>
+      <c r="CP76" s="14"/>
+      <c r="CQ76" s="14"/>
+      <c r="CR76" s="14"/>
+      <c r="CS76" s="14"/>
+      <c r="CT76" s="15"/>
     </row>
     <row r="77" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C77" s="16">
@@ -9614,39 +9462,39 @@
       <c r="D77" s="17"/>
       <c r="E77" s="17"/>
       <c r="F77" s="17"/>
-      <c r="G77" s="22"/>
-      <c r="H77" s="18"/>
-      <c r="I77" s="18"/>
-      <c r="J77" s="18"/>
-      <c r="K77" s="18"/>
-      <c r="L77" s="18"/>
-      <c r="M77" s="18"/>
-      <c r="N77" s="18"/>
-      <c r="O77" s="18"/>
-      <c r="P77" s="18"/>
-      <c r="Q77" s="18"/>
-      <c r="R77" s="18"/>
-      <c r="S77" s="18"/>
-      <c r="T77" s="18"/>
-      <c r="U77" s="18"/>
-      <c r="V77" s="18"/>
-      <c r="W77" s="18"/>
-      <c r="X77" s="18"/>
-      <c r="Y77" s="18"/>
-      <c r="Z77" s="18"/>
-      <c r="AA77" s="18"/>
-      <c r="AB77" s="18"/>
-      <c r="AC77" s="18"/>
-      <c r="AD77" s="18"/>
-      <c r="AE77" s="18"/>
-      <c r="AF77" s="18"/>
-      <c r="AG77" s="18"/>
-      <c r="AH77" s="18"/>
-      <c r="AI77" s="18"/>
-      <c r="AJ77" s="18"/>
-      <c r="AK77" s="18"/>
-      <c r="AL77" s="18"/>
-      <c r="AM77" s="18"/>
+      <c r="G77" s="28"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="14"/>
+      <c r="K77" s="14"/>
+      <c r="L77" s="14"/>
+      <c r="M77" s="14"/>
+      <c r="N77" s="14"/>
+      <c r="O77" s="14"/>
+      <c r="P77" s="14"/>
+      <c r="Q77" s="14"/>
+      <c r="R77" s="14"/>
+      <c r="S77" s="14"/>
+      <c r="T77" s="14"/>
+      <c r="U77" s="14"/>
+      <c r="V77" s="14"/>
+      <c r="W77" s="14"/>
+      <c r="X77" s="14"/>
+      <c r="Y77" s="14"/>
+      <c r="Z77" s="14"/>
+      <c r="AA77" s="14"/>
+      <c r="AB77" s="14"/>
+      <c r="AC77" s="14"/>
+      <c r="AD77" s="14"/>
+      <c r="AE77" s="14"/>
+      <c r="AF77" s="14"/>
+      <c r="AG77" s="14"/>
+      <c r="AH77" s="14"/>
+      <c r="AI77" s="14"/>
+      <c r="AJ77" s="14"/>
+      <c r="AK77" s="14"/>
+      <c r="AL77" s="14"/>
+      <c r="AM77" s="14"/>
       <c r="AN77" s="17"/>
       <c r="AO77" s="17"/>
       <c r="AP77" s="17"/>
@@ -9669,82 +9517,82 @@
       <c r="BG77" s="17"/>
       <c r="BH77" s="17"/>
       <c r="BI77" s="17"/>
-      <c r="BJ77" s="18"/>
-      <c r="BK77" s="18"/>
-      <c r="BL77" s="18"/>
-      <c r="BM77" s="18"/>
-      <c r="BN77" s="18"/>
-      <c r="BO77" s="18"/>
-      <c r="BP77" s="18"/>
-      <c r="BQ77" s="18"/>
-      <c r="BR77" s="18"/>
-      <c r="BS77" s="18"/>
-      <c r="BT77" s="18"/>
-      <c r="BU77" s="18"/>
-      <c r="BV77" s="18"/>
-      <c r="BW77" s="18"/>
-      <c r="BX77" s="18"/>
-      <c r="BY77" s="18"/>
-      <c r="BZ77" s="18"/>
-      <c r="CA77" s="18"/>
-      <c r="CB77" s="18"/>
-      <c r="CC77" s="18"/>
-      <c r="CD77" s="18"/>
-      <c r="CE77" s="18"/>
-      <c r="CF77" s="18"/>
-      <c r="CG77" s="18"/>
-      <c r="CH77" s="18"/>
-      <c r="CI77" s="18"/>
-      <c r="CJ77" s="18"/>
-      <c r="CK77" s="18"/>
-      <c r="CL77" s="18"/>
-      <c r="CM77" s="18"/>
-      <c r="CN77" s="18"/>
-      <c r="CO77" s="18"/>
-      <c r="CP77" s="18"/>
-      <c r="CQ77" s="18"/>
-      <c r="CR77" s="18"/>
-      <c r="CS77" s="18"/>
-      <c r="CT77" s="19"/>
+      <c r="BJ77" s="14"/>
+      <c r="BK77" s="14"/>
+      <c r="BL77" s="14"/>
+      <c r="BM77" s="14"/>
+      <c r="BN77" s="14"/>
+      <c r="BO77" s="14"/>
+      <c r="BP77" s="14"/>
+      <c r="BQ77" s="14"/>
+      <c r="BR77" s="14"/>
+      <c r="BS77" s="14"/>
+      <c r="BT77" s="14"/>
+      <c r="BU77" s="14"/>
+      <c r="BV77" s="14"/>
+      <c r="BW77" s="14"/>
+      <c r="BX77" s="14"/>
+      <c r="BY77" s="14"/>
+      <c r="BZ77" s="14"/>
+      <c r="CA77" s="14"/>
+      <c r="CB77" s="14"/>
+      <c r="CC77" s="14"/>
+      <c r="CD77" s="14"/>
+      <c r="CE77" s="14"/>
+      <c r="CF77" s="14"/>
+      <c r="CG77" s="14"/>
+      <c r="CH77" s="14"/>
+      <c r="CI77" s="14"/>
+      <c r="CJ77" s="14"/>
+      <c r="CK77" s="14"/>
+      <c r="CL77" s="14"/>
+      <c r="CM77" s="14"/>
+      <c r="CN77" s="14"/>
+      <c r="CO77" s="14"/>
+      <c r="CP77" s="14"/>
+      <c r="CQ77" s="14"/>
+      <c r="CR77" s="14"/>
+      <c r="CS77" s="14"/>
+      <c r="CT77" s="15"/>
     </row>
     <row r="78" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C78" s="16"/>
       <c r="D78" s="17"/>
       <c r="E78" s="17"/>
       <c r="F78" s="17"/>
-      <c r="G78" s="18"/>
-      <c r="H78" s="18"/>
-      <c r="I78" s="18"/>
-      <c r="J78" s="18"/>
-      <c r="K78" s="18"/>
-      <c r="L78" s="18"/>
-      <c r="M78" s="18"/>
-      <c r="N78" s="18"/>
-      <c r="O78" s="18"/>
-      <c r="P78" s="18"/>
-      <c r="Q78" s="18"/>
-      <c r="R78" s="18"/>
-      <c r="S78" s="18"/>
-      <c r="T78" s="18"/>
-      <c r="U78" s="18"/>
-      <c r="V78" s="18"/>
-      <c r="W78" s="18"/>
-      <c r="X78" s="18"/>
-      <c r="Y78" s="18"/>
-      <c r="Z78" s="18"/>
-      <c r="AA78" s="18"/>
-      <c r="AB78" s="18"/>
-      <c r="AC78" s="18"/>
-      <c r="AD78" s="18"/>
-      <c r="AE78" s="18"/>
-      <c r="AF78" s="18"/>
-      <c r="AG78" s="18"/>
-      <c r="AH78" s="18"/>
-      <c r="AI78" s="18"/>
-      <c r="AJ78" s="18"/>
-      <c r="AK78" s="18"/>
-      <c r="AL78" s="18"/>
-      <c r="AM78" s="18"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
+      <c r="I78" s="14"/>
+      <c r="J78" s="14"/>
+      <c r="K78" s="14"/>
+      <c r="L78" s="14"/>
+      <c r="M78" s="14"/>
+      <c r="N78" s="14"/>
+      <c r="O78" s="14"/>
+      <c r="P78" s="14"/>
+      <c r="Q78" s="14"/>
+      <c r="R78" s="14"/>
+      <c r="S78" s="14"/>
+      <c r="T78" s="14"/>
+      <c r="U78" s="14"/>
+      <c r="V78" s="14"/>
+      <c r="W78" s="14"/>
+      <c r="X78" s="14"/>
+      <c r="Y78" s="14"/>
+      <c r="Z78" s="14"/>
+      <c r="AA78" s="14"/>
+      <c r="AB78" s="14"/>
+      <c r="AC78" s="14"/>
+      <c r="AD78" s="14"/>
+      <c r="AE78" s="14"/>
+      <c r="AF78" s="14"/>
+      <c r="AG78" s="14"/>
+      <c r="AH78" s="14"/>
+      <c r="AI78" s="14"/>
+      <c r="AJ78" s="14"/>
+      <c r="AK78" s="14"/>
+      <c r="AL78" s="14"/>
+      <c r="AM78" s="14"/>
       <c r="AN78" s="17"/>
       <c r="AO78" s="17"/>
       <c r="AP78" s="17"/>
@@ -9767,141 +9615,141 @@
       <c r="BG78" s="17"/>
       <c r="BH78" s="17"/>
       <c r="BI78" s="17"/>
-      <c r="BJ78" s="18"/>
-      <c r="BK78" s="18"/>
-      <c r="BL78" s="18"/>
-      <c r="BM78" s="18"/>
-      <c r="BN78" s="18"/>
-      <c r="BO78" s="18"/>
-      <c r="BP78" s="18"/>
-      <c r="BQ78" s="18"/>
-      <c r="BR78" s="18"/>
-      <c r="BS78" s="18"/>
-      <c r="BT78" s="18"/>
-      <c r="BU78" s="18"/>
-      <c r="BV78" s="18"/>
-      <c r="BW78" s="18"/>
-      <c r="BX78" s="18"/>
-      <c r="BY78" s="18"/>
-      <c r="BZ78" s="18"/>
-      <c r="CA78" s="18"/>
-      <c r="CB78" s="18"/>
-      <c r="CC78" s="18"/>
-      <c r="CD78" s="18"/>
-      <c r="CE78" s="18"/>
-      <c r="CF78" s="18"/>
-      <c r="CG78" s="18"/>
-      <c r="CH78" s="18"/>
-      <c r="CI78" s="18"/>
-      <c r="CJ78" s="18"/>
-      <c r="CK78" s="18"/>
-      <c r="CL78" s="18"/>
-      <c r="CM78" s="18"/>
-      <c r="CN78" s="18"/>
-      <c r="CO78" s="18"/>
-      <c r="CP78" s="18"/>
-      <c r="CQ78" s="18"/>
-      <c r="CR78" s="18"/>
-      <c r="CS78" s="18"/>
-      <c r="CT78" s="19"/>
+      <c r="BJ78" s="14"/>
+      <c r="BK78" s="14"/>
+      <c r="BL78" s="14"/>
+      <c r="BM78" s="14"/>
+      <c r="BN78" s="14"/>
+      <c r="BO78" s="14"/>
+      <c r="BP78" s="14"/>
+      <c r="BQ78" s="14"/>
+      <c r="BR78" s="14"/>
+      <c r="BS78" s="14"/>
+      <c r="BT78" s="14"/>
+      <c r="BU78" s="14"/>
+      <c r="BV78" s="14"/>
+      <c r="BW78" s="14"/>
+      <c r="BX78" s="14"/>
+      <c r="BY78" s="14"/>
+      <c r="BZ78" s="14"/>
+      <c r="CA78" s="14"/>
+      <c r="CB78" s="14"/>
+      <c r="CC78" s="14"/>
+      <c r="CD78" s="14"/>
+      <c r="CE78" s="14"/>
+      <c r="CF78" s="14"/>
+      <c r="CG78" s="14"/>
+      <c r="CH78" s="14"/>
+      <c r="CI78" s="14"/>
+      <c r="CJ78" s="14"/>
+      <c r="CK78" s="14"/>
+      <c r="CL78" s="14"/>
+      <c r="CM78" s="14"/>
+      <c r="CN78" s="14"/>
+      <c r="CO78" s="14"/>
+      <c r="CP78" s="14"/>
+      <c r="CQ78" s="14"/>
+      <c r="CR78" s="14"/>
+      <c r="CS78" s="14"/>
+      <c r="CT78" s="15"/>
     </row>
     <row r="79" spans="3:98" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C79" s="20"/>
-      <c r="D79" s="21"/>
-      <c r="E79" s="21"/>
-      <c r="F79" s="21"/>
-      <c r="G79" s="14"/>
-      <c r="H79" s="14"/>
-      <c r="I79" s="14"/>
-      <c r="J79" s="14"/>
-      <c r="K79" s="14"/>
-      <c r="L79" s="14"/>
-      <c r="M79" s="14"/>
-      <c r="N79" s="14"/>
-      <c r="O79" s="14"/>
-      <c r="P79" s="14"/>
-      <c r="Q79" s="14"/>
-      <c r="R79" s="14"/>
-      <c r="S79" s="14"/>
-      <c r="T79" s="14"/>
-      <c r="U79" s="14"/>
-      <c r="V79" s="14"/>
-      <c r="W79" s="14"/>
-      <c r="X79" s="14"/>
-      <c r="Y79" s="14"/>
-      <c r="Z79" s="14"/>
-      <c r="AA79" s="14"/>
-      <c r="AB79" s="14"/>
-      <c r="AC79" s="14"/>
-      <c r="AD79" s="14"/>
-      <c r="AE79" s="14"/>
-      <c r="AF79" s="14"/>
-      <c r="AG79" s="14"/>
-      <c r="AH79" s="14"/>
-      <c r="AI79" s="14"/>
-      <c r="AJ79" s="14"/>
-      <c r="AK79" s="14"/>
-      <c r="AL79" s="14"/>
-      <c r="AM79" s="14"/>
-      <c r="AN79" s="21"/>
-      <c r="AO79" s="21"/>
-      <c r="AP79" s="21"/>
-      <c r="AQ79" s="21"/>
-      <c r="AR79" s="21"/>
-      <c r="AS79" s="21"/>
-      <c r="AT79" s="21"/>
-      <c r="AU79" s="21"/>
-      <c r="AV79" s="21"/>
-      <c r="AW79" s="21"/>
-      <c r="AX79" s="21"/>
-      <c r="AY79" s="21"/>
-      <c r="AZ79" s="21"/>
-      <c r="BA79" s="21"/>
-      <c r="BB79" s="21"/>
-      <c r="BC79" s="21"/>
-      <c r="BD79" s="21"/>
-      <c r="BE79" s="21"/>
-      <c r="BF79" s="21"/>
-      <c r="BG79" s="21"/>
-      <c r="BH79" s="21"/>
-      <c r="BI79" s="21"/>
-      <c r="BJ79" s="14"/>
-      <c r="BK79" s="14"/>
-      <c r="BL79" s="14"/>
-      <c r="BM79" s="14"/>
-      <c r="BN79" s="14"/>
-      <c r="BO79" s="14"/>
-      <c r="BP79" s="14"/>
-      <c r="BQ79" s="14"/>
-      <c r="BR79" s="14"/>
-      <c r="BS79" s="14"/>
-      <c r="BT79" s="14"/>
-      <c r="BU79" s="14"/>
-      <c r="BV79" s="14"/>
-      <c r="BW79" s="14"/>
-      <c r="BX79" s="14"/>
-      <c r="BY79" s="14"/>
-      <c r="BZ79" s="14"/>
-      <c r="CA79" s="14"/>
-      <c r="CB79" s="14"/>
-      <c r="CC79" s="14"/>
-      <c r="CD79" s="14"/>
-      <c r="CE79" s="14"/>
-      <c r="CF79" s="14"/>
-      <c r="CG79" s="14"/>
-      <c r="CH79" s="14"/>
-      <c r="CI79" s="14"/>
-      <c r="CJ79" s="14"/>
-      <c r="CK79" s="14"/>
-      <c r="CL79" s="14"/>
-      <c r="CM79" s="14"/>
-      <c r="CN79" s="14"/>
-      <c r="CO79" s="14"/>
-      <c r="CP79" s="14"/>
-      <c r="CQ79" s="14"/>
-      <c r="CR79" s="14"/>
-      <c r="CS79" s="14"/>
-      <c r="CT79" s="15"/>
+      <c r="C79" s="31"/>
+      <c r="D79" s="32"/>
+      <c r="E79" s="32"/>
+      <c r="F79" s="32"/>
+      <c r="G79" s="29"/>
+      <c r="H79" s="29"/>
+      <c r="I79" s="29"/>
+      <c r="J79" s="29"/>
+      <c r="K79" s="29"/>
+      <c r="L79" s="29"/>
+      <c r="M79" s="29"/>
+      <c r="N79" s="29"/>
+      <c r="O79" s="29"/>
+      <c r="P79" s="29"/>
+      <c r="Q79" s="29"/>
+      <c r="R79" s="29"/>
+      <c r="S79" s="29"/>
+      <c r="T79" s="29"/>
+      <c r="U79" s="29"/>
+      <c r="V79" s="29"/>
+      <c r="W79" s="29"/>
+      <c r="X79" s="29"/>
+      <c r="Y79" s="29"/>
+      <c r="Z79" s="29"/>
+      <c r="AA79" s="29"/>
+      <c r="AB79" s="29"/>
+      <c r="AC79" s="29"/>
+      <c r="AD79" s="29"/>
+      <c r="AE79" s="29"/>
+      <c r="AF79" s="29"/>
+      <c r="AG79" s="29"/>
+      <c r="AH79" s="29"/>
+      <c r="AI79" s="29"/>
+      <c r="AJ79" s="29"/>
+      <c r="AK79" s="29"/>
+      <c r="AL79" s="29"/>
+      <c r="AM79" s="29"/>
+      <c r="AN79" s="32"/>
+      <c r="AO79" s="32"/>
+      <c r="AP79" s="32"/>
+      <c r="AQ79" s="32"/>
+      <c r="AR79" s="32"/>
+      <c r="AS79" s="32"/>
+      <c r="AT79" s="32"/>
+      <c r="AU79" s="32"/>
+      <c r="AV79" s="32"/>
+      <c r="AW79" s="32"/>
+      <c r="AX79" s="32"/>
+      <c r="AY79" s="32"/>
+      <c r="AZ79" s="32"/>
+      <c r="BA79" s="32"/>
+      <c r="BB79" s="32"/>
+      <c r="BC79" s="32"/>
+      <c r="BD79" s="32"/>
+      <c r="BE79" s="32"/>
+      <c r="BF79" s="32"/>
+      <c r="BG79" s="32"/>
+      <c r="BH79" s="32"/>
+      <c r="BI79" s="32"/>
+      <c r="BJ79" s="29"/>
+      <c r="BK79" s="29"/>
+      <c r="BL79" s="29"/>
+      <c r="BM79" s="29"/>
+      <c r="BN79" s="29"/>
+      <c r="BO79" s="29"/>
+      <c r="BP79" s="29"/>
+      <c r="BQ79" s="29"/>
+      <c r="BR79" s="29"/>
+      <c r="BS79" s="29"/>
+      <c r="BT79" s="29"/>
+      <c r="BU79" s="29"/>
+      <c r="BV79" s="29"/>
+      <c r="BW79" s="29"/>
+      <c r="BX79" s="29"/>
+      <c r="BY79" s="29"/>
+      <c r="BZ79" s="29"/>
+      <c r="CA79" s="29"/>
+      <c r="CB79" s="29"/>
+      <c r="CC79" s="29"/>
+      <c r="CD79" s="29"/>
+      <c r="CE79" s="29"/>
+      <c r="CF79" s="29"/>
+      <c r="CG79" s="29"/>
+      <c r="CH79" s="29"/>
+      <c r="CI79" s="29"/>
+      <c r="CJ79" s="29"/>
+      <c r="CK79" s="29"/>
+      <c r="CL79" s="29"/>
+      <c r="CM79" s="29"/>
+      <c r="CN79" s="29"/>
+      <c r="CO79" s="29"/>
+      <c r="CP79" s="29"/>
+      <c r="CQ79" s="29"/>
+      <c r="CR79" s="29"/>
+      <c r="CS79" s="29"/>
+      <c r="CT79" s="30"/>
     </row>
     <row r="80" spans="3:98" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9911,30 +9759,42 @@
     <row r="85" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="BZ71:CT71"/>
-    <mergeCell ref="C71:F71"/>
-    <mergeCell ref="G71:X71"/>
-    <mergeCell ref="Y71:AM71"/>
-    <mergeCell ref="AN71:BI71"/>
-    <mergeCell ref="BJ71:BY71"/>
-    <mergeCell ref="BZ69:CT69"/>
-    <mergeCell ref="A1:F3"/>
-    <mergeCell ref="A4:F6"/>
-    <mergeCell ref="G1:AD3"/>
-    <mergeCell ref="G4:AD6"/>
-    <mergeCell ref="BZ68:CT68"/>
-    <mergeCell ref="BJ68:BY68"/>
-    <mergeCell ref="AN68:BI68"/>
-    <mergeCell ref="Y68:AM68"/>
-    <mergeCell ref="G68:X68"/>
-    <mergeCell ref="C68:F68"/>
-    <mergeCell ref="Y70:AM70"/>
-    <mergeCell ref="AN70:BI70"/>
-    <mergeCell ref="BJ70:BY70"/>
-    <mergeCell ref="C69:F69"/>
-    <mergeCell ref="G69:X69"/>
-    <mergeCell ref="Y69:AM69"/>
-    <mergeCell ref="AN69:BI69"/>
+    <mergeCell ref="BZ79:CT79"/>
+    <mergeCell ref="C78:F78"/>
+    <mergeCell ref="G78:X78"/>
+    <mergeCell ref="Y78:AM78"/>
+    <mergeCell ref="AN78:BI78"/>
+    <mergeCell ref="BJ78:BY78"/>
+    <mergeCell ref="BZ78:CT78"/>
+    <mergeCell ref="C79:F79"/>
+    <mergeCell ref="G79:X79"/>
+    <mergeCell ref="Y79:AM79"/>
+    <mergeCell ref="AN79:BI79"/>
+    <mergeCell ref="BJ79:BY79"/>
+    <mergeCell ref="BZ77:CT77"/>
+    <mergeCell ref="C76:F76"/>
+    <mergeCell ref="G76:X76"/>
+    <mergeCell ref="Y76:AM76"/>
+    <mergeCell ref="AN76:BI76"/>
+    <mergeCell ref="BJ76:BY76"/>
+    <mergeCell ref="BZ76:CT76"/>
+    <mergeCell ref="C77:F77"/>
+    <mergeCell ref="G77:X77"/>
+    <mergeCell ref="Y77:AM77"/>
+    <mergeCell ref="AN77:BI77"/>
+    <mergeCell ref="BJ77:BY77"/>
+    <mergeCell ref="BZ75:CT75"/>
+    <mergeCell ref="C74:F74"/>
+    <mergeCell ref="G74:X74"/>
+    <mergeCell ref="Y74:AM74"/>
+    <mergeCell ref="AN74:BI74"/>
+    <mergeCell ref="BJ74:BY74"/>
+    <mergeCell ref="BZ74:CT74"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="G75:X75"/>
+    <mergeCell ref="Y75:AM75"/>
+    <mergeCell ref="AN75:BI75"/>
+    <mergeCell ref="BJ75:BY75"/>
     <mergeCell ref="BZ70:CT70"/>
     <mergeCell ref="BJ69:BY69"/>
     <mergeCell ref="BZ73:CT73"/>
@@ -9951,42 +9811,30 @@
     <mergeCell ref="BJ73:BY73"/>
     <mergeCell ref="C70:F70"/>
     <mergeCell ref="G70:X70"/>
-    <mergeCell ref="BZ75:CT75"/>
-    <mergeCell ref="C74:F74"/>
-    <mergeCell ref="G74:X74"/>
-    <mergeCell ref="Y74:AM74"/>
-    <mergeCell ref="AN74:BI74"/>
-    <mergeCell ref="BJ74:BY74"/>
-    <mergeCell ref="BZ74:CT74"/>
-    <mergeCell ref="C75:F75"/>
-    <mergeCell ref="G75:X75"/>
-    <mergeCell ref="Y75:AM75"/>
-    <mergeCell ref="AN75:BI75"/>
-    <mergeCell ref="BJ75:BY75"/>
-    <mergeCell ref="BZ77:CT77"/>
-    <mergeCell ref="C76:F76"/>
-    <mergeCell ref="G76:X76"/>
-    <mergeCell ref="Y76:AM76"/>
-    <mergeCell ref="AN76:BI76"/>
-    <mergeCell ref="BJ76:BY76"/>
-    <mergeCell ref="BZ76:CT76"/>
-    <mergeCell ref="C77:F77"/>
-    <mergeCell ref="G77:X77"/>
-    <mergeCell ref="Y77:AM77"/>
-    <mergeCell ref="AN77:BI77"/>
-    <mergeCell ref="BJ77:BY77"/>
-    <mergeCell ref="BZ79:CT79"/>
-    <mergeCell ref="C78:F78"/>
-    <mergeCell ref="G78:X78"/>
-    <mergeCell ref="Y78:AM78"/>
-    <mergeCell ref="AN78:BI78"/>
-    <mergeCell ref="BJ78:BY78"/>
-    <mergeCell ref="BZ78:CT78"/>
-    <mergeCell ref="C79:F79"/>
-    <mergeCell ref="G79:X79"/>
-    <mergeCell ref="Y79:AM79"/>
-    <mergeCell ref="AN79:BI79"/>
-    <mergeCell ref="BJ79:BY79"/>
+    <mergeCell ref="Y70:AM70"/>
+    <mergeCell ref="AN70:BI70"/>
+    <mergeCell ref="BJ70:BY70"/>
+    <mergeCell ref="C69:F69"/>
+    <mergeCell ref="G69:X69"/>
+    <mergeCell ref="Y69:AM69"/>
+    <mergeCell ref="AN69:BI69"/>
+    <mergeCell ref="BZ69:CT69"/>
+    <mergeCell ref="A1:F3"/>
+    <mergeCell ref="A4:F6"/>
+    <mergeCell ref="G1:AD3"/>
+    <mergeCell ref="G4:AD6"/>
+    <mergeCell ref="BZ68:CT68"/>
+    <mergeCell ref="BJ68:BY68"/>
+    <mergeCell ref="AN68:BI68"/>
+    <mergeCell ref="Y68:AM68"/>
+    <mergeCell ref="G68:X68"/>
+    <mergeCell ref="C68:F68"/>
+    <mergeCell ref="BZ71:CT71"/>
+    <mergeCell ref="C71:F71"/>
+    <mergeCell ref="G71:X71"/>
+    <mergeCell ref="Y71:AM71"/>
+    <mergeCell ref="AN71:BI71"/>
+    <mergeCell ref="BJ71:BY71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>